<commit_message>
Actualizando estado de recursos
</commit_message>
<xml_diff>
--- a/fuentes/contenidos/grado08/guion08/ESCALETA_MA_08_08_CO.xlsx
+++ b/fuentes/contenidos/grado08/guion08/ESCALETA_MA_08_08_CO.xlsx
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="673" uniqueCount="263">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="675" uniqueCount="263">
   <si>
     <t>Asignatura</t>
   </si>
@@ -1341,7 +1341,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="229">
+  <cellXfs count="231">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
@@ -1842,81 +1842,6 @@
     <xf numFmtId="0" fontId="0" fillId="18" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="12" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="10" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="9" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="11" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="12" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="19" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="17" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -1953,6 +1878,85 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="17" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="17" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="12" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="12" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="10" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="11" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="18" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="19" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2259,9 +2263,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Y287"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="K1" zoomScale="70" zoomScaleNormal="70" zoomScalePageLayoutView="91" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="J1" zoomScale="70" zoomScaleNormal="70" zoomScalePageLayoutView="91" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="Y29" sqref="Y29"/>
+      <selection pane="bottomLeft" activeCell="W39" sqref="W39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2293,68 +2297,68 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:24" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="202" t="s">
+      <c r="A1" s="210" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="200" t="s">
+      <c r="B1" s="208" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="213" t="s">
+      <c r="C1" s="221" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="202" t="s">
+      <c r="D1" s="210" t="s">
         <v>110</v>
       </c>
-      <c r="E1" s="200" t="s">
+      <c r="E1" s="208" t="s">
         <v>111</v>
       </c>
-      <c r="F1" s="198" t="s">
+      <c r="F1" s="204" t="s">
         <v>112</v>
       </c>
-      <c r="G1" s="211" t="s">
+      <c r="G1" s="219" t="s">
         <v>3</v>
       </c>
-      <c r="H1" s="198" t="s">
+      <c r="H1" s="204" t="s">
         <v>113</v>
       </c>
-      <c r="I1" s="198" t="s">
+      <c r="I1" s="204" t="s">
         <v>107</v>
       </c>
-      <c r="J1" s="208" t="s">
+      <c r="J1" s="216" t="s">
         <v>4</v>
       </c>
-      <c r="K1" s="206" t="s">
+      <c r="K1" s="214" t="s">
         <v>108</v>
       </c>
-      <c r="L1" s="204" t="s">
+      <c r="L1" s="212" t="s">
         <v>14</v>
       </c>
-      <c r="M1" s="210" t="s">
+      <c r="M1" s="218" t="s">
         <v>21</v>
       </c>
-      <c r="N1" s="210"/>
-      <c r="O1" s="190" t="s">
+      <c r="N1" s="218"/>
+      <c r="O1" s="206" t="s">
         <v>109</v>
       </c>
-      <c r="P1" s="190" t="s">
+      <c r="P1" s="206" t="s">
         <v>114</v>
       </c>
-      <c r="Q1" s="192" t="s">
+      <c r="Q1" s="223" t="s">
         <v>85</v>
       </c>
-      <c r="R1" s="196" t="s">
+      <c r="R1" s="227" t="s">
         <v>86</v>
       </c>
-      <c r="S1" s="192" t="s">
+      <c r="S1" s="223" t="s">
         <v>87</v>
       </c>
-      <c r="T1" s="194" t="s">
+      <c r="T1" s="225" t="s">
         <v>88</v>
       </c>
-      <c r="U1" s="192" t="s">
+      <c r="U1" s="223" t="s">
         <v>89</v>
       </c>
-      <c r="V1" s="227" t="s">
+      <c r="V1" s="202" t="s">
         <v>251</v>
       </c>
       <c r="W1" s="173" t="s">
@@ -2365,31 +2369,31 @@
       </c>
     </row>
     <row r="2" spans="1:24" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="203"/>
-      <c r="B2" s="201"/>
-      <c r="C2" s="214"/>
-      <c r="D2" s="203"/>
-      <c r="E2" s="201"/>
-      <c r="F2" s="199"/>
-      <c r="G2" s="212"/>
-      <c r="H2" s="199"/>
-      <c r="I2" s="199"/>
-      <c r="J2" s="209"/>
-      <c r="K2" s="207"/>
-      <c r="L2" s="205"/>
+      <c r="A2" s="211"/>
+      <c r="B2" s="209"/>
+      <c r="C2" s="222"/>
+      <c r="D2" s="211"/>
+      <c r="E2" s="209"/>
+      <c r="F2" s="205"/>
+      <c r="G2" s="220"/>
+      <c r="H2" s="205"/>
+      <c r="I2" s="205"/>
+      <c r="J2" s="217"/>
+      <c r="K2" s="215"/>
+      <c r="L2" s="213"/>
       <c r="M2" s="5" t="s">
         <v>90</v>
       </c>
       <c r="N2" s="5" t="s">
         <v>91</v>
       </c>
-      <c r="O2" s="191"/>
-      <c r="P2" s="191"/>
-      <c r="Q2" s="193"/>
-      <c r="R2" s="197"/>
-      <c r="S2" s="193"/>
-      <c r="T2" s="195"/>
-      <c r="U2" s="193"/>
+      <c r="O2" s="207"/>
+      <c r="P2" s="207"/>
+      <c r="Q2" s="224"/>
+      <c r="R2" s="228"/>
+      <c r="S2" s="224"/>
+      <c r="T2" s="226"/>
+      <c r="U2" s="224"/>
       <c r="V2" s="167"/>
       <c r="W2" s="3"/>
       <c r="X2" s="3"/>
@@ -2793,54 +2797,58 @@
       </c>
       <c r="E9" s="25"/>
       <c r="F9" s="25"/>
-      <c r="G9" s="30" t="s">
+      <c r="G9" s="185" t="s">
         <v>223</v>
       </c>
-      <c r="H9" s="122">
+      <c r="H9" s="187">
         <v>7</v>
       </c>
-      <c r="I9" s="122" t="s">
+      <c r="I9" s="187" t="s">
         <v>20</v>
       </c>
-      <c r="J9" s="25" t="s">
+      <c r="J9" s="173" t="s">
         <v>227</v>
       </c>
-      <c r="K9" s="122" t="s">
+      <c r="K9" s="187" t="s">
         <v>20</v>
       </c>
-      <c r="L9" s="122" t="s">
+      <c r="L9" s="187" t="s">
         <v>8</v>
       </c>
-      <c r="M9" s="122"/>
-      <c r="N9" s="122" t="s">
+      <c r="M9" s="187"/>
+      <c r="N9" s="187" t="s">
         <v>32</v>
       </c>
-      <c r="O9" s="25" t="s">
+      <c r="O9" s="173" t="s">
         <v>136</v>
       </c>
-      <c r="P9" s="123" t="s">
+      <c r="P9" s="186" t="s">
         <v>20</v>
       </c>
-      <c r="Q9" s="124">
+      <c r="Q9" s="188">
         <v>6</v>
       </c>
-      <c r="R9" s="124" t="s">
+      <c r="R9" s="188" t="s">
         <v>192</v>
       </c>
-      <c r="S9" s="124" t="s">
+      <c r="S9" s="188" t="s">
         <v>193</v>
       </c>
-      <c r="T9" s="163" t="s">
+      <c r="T9" s="229" t="s">
         <v>200</v>
       </c>
-      <c r="U9" s="164" t="s">
+      <c r="U9" s="189" t="s">
         <v>195</v>
       </c>
-      <c r="V9" s="168" t="s">
+      <c r="V9" s="190" t="s">
         <v>250</v>
       </c>
-      <c r="W9" s="3"/>
-      <c r="X9" s="3"/>
+      <c r="W9" s="178">
+        <v>42408</v>
+      </c>
+      <c r="X9" s="3" t="s">
+        <v>257</v>
+      </c>
     </row>
     <row r="10" spans="1:24" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="161" t="s">
@@ -2921,54 +2929,58 @@
       </c>
       <c r="E11" s="26"/>
       <c r="F11" s="26"/>
-      <c r="G11" s="61" t="s">
+      <c r="G11" s="185" t="s">
         <v>138</v>
       </c>
-      <c r="H11" s="63">
+      <c r="H11" s="187">
         <v>9</v>
       </c>
-      <c r="I11" s="63" t="s">
+      <c r="I11" s="187" t="s">
         <v>20</v>
       </c>
-      <c r="J11" s="26" t="s">
+      <c r="J11" s="173" t="s">
         <v>139</v>
       </c>
-      <c r="K11" s="63" t="s">
+      <c r="K11" s="187" t="s">
         <v>20</v>
       </c>
-      <c r="L11" s="63" t="s">
+      <c r="L11" s="187" t="s">
         <v>8</v>
       </c>
-      <c r="M11" s="63"/>
-      <c r="N11" s="63" t="s">
+      <c r="M11" s="187"/>
+      <c r="N11" s="187" t="s">
         <v>24</v>
       </c>
-      <c r="O11" s="26" t="s">
+      <c r="O11" s="173" t="s">
         <v>140</v>
       </c>
-      <c r="P11" s="62" t="s">
+      <c r="P11" s="186" t="s">
         <v>19</v>
       </c>
-      <c r="Q11" s="64">
+      <c r="Q11" s="188">
         <v>6</v>
       </c>
-      <c r="R11" s="64" t="s">
+      <c r="R11" s="188" t="s">
         <v>192</v>
       </c>
-      <c r="S11" s="64" t="s">
+      <c r="S11" s="188" t="s">
         <v>193</v>
       </c>
-      <c r="T11" s="65" t="s">
+      <c r="T11" s="229" t="s">
         <v>202</v>
       </c>
-      <c r="U11" s="66" t="s">
+      <c r="U11" s="189" t="s">
         <v>195</v>
       </c>
-      <c r="V11" s="168" t="s">
+      <c r="V11" s="190" t="s">
         <v>250</v>
       </c>
-      <c r="W11" s="3"/>
-      <c r="X11" s="3"/>
+      <c r="W11" s="178">
+        <v>42408</v>
+      </c>
+      <c r="X11" s="3" t="s">
+        <v>257</v>
+      </c>
     </row>
     <row r="12" spans="1:24" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="67" t="s">
@@ -3410,10 +3422,10 @@
       <c r="U18" s="184" t="s">
         <v>219</v>
       </c>
-      <c r="V18" s="215" t="s">
+      <c r="V18" s="190" t="s">
         <v>246</v>
       </c>
-      <c r="W18" s="178">
+      <c r="W18" s="230">
         <v>42403</v>
       </c>
       <c r="X18" s="177" t="s">
@@ -3474,10 +3486,10 @@
       <c r="U19" s="189" t="s">
         <v>219</v>
       </c>
-      <c r="V19" s="215" t="s">
+      <c r="V19" s="190" t="s">
         <v>246</v>
       </c>
-      <c r="W19" s="178">
+      <c r="W19" s="230">
         <v>42403</v>
       </c>
       <c r="X19" s="25" t="s">
@@ -3691,53 +3703,55 @@
       </c>
       <c r="E23" s="19"/>
       <c r="F23" s="19"/>
-      <c r="G23" s="102" t="s">
+      <c r="G23" s="185" t="s">
         <v>159</v>
       </c>
-      <c r="H23" s="104">
+      <c r="H23" s="186">
         <v>21</v>
       </c>
-      <c r="I23" s="103" t="s">
+      <c r="I23" s="187" t="s">
         <v>20</v>
       </c>
-      <c r="J23" s="19" t="s">
+      <c r="J23" s="173" t="s">
         <v>160</v>
       </c>
-      <c r="K23" s="103" t="s">
+      <c r="K23" s="187" t="s">
         <v>20</v>
       </c>
-      <c r="L23" s="103" t="s">
+      <c r="L23" s="187" t="s">
         <v>8</v>
       </c>
-      <c r="M23" s="103"/>
-      <c r="N23" s="103" t="s">
+      <c r="M23" s="187"/>
+      <c r="N23" s="187" t="s">
         <v>24</v>
       </c>
-      <c r="O23" s="19" t="s">
+      <c r="O23" s="173" t="s">
         <v>161</v>
       </c>
-      <c r="P23" s="104" t="s">
+      <c r="P23" s="186" t="s">
         <v>19</v>
       </c>
-      <c r="Q23" s="105">
+      <c r="Q23" s="188">
         <v>6</v>
       </c>
-      <c r="R23" s="105" t="s">
+      <c r="R23" s="188" t="s">
         <v>192</v>
       </c>
-      <c r="S23" s="105" t="s">
+      <c r="S23" s="188" t="s">
         <v>193</v>
       </c>
-      <c r="T23" s="106" t="s">
+      <c r="T23" s="229" t="s">
         <v>212</v>
       </c>
-      <c r="U23" s="107" t="s">
+      <c r="U23" s="189" t="s">
         <v>195</v>
       </c>
-      <c r="V23" s="168" t="s">
+      <c r="V23" s="190" t="s">
         <v>250</v>
       </c>
-      <c r="W23" s="3"/>
+      <c r="W23" s="178">
+        <v>42408</v>
+      </c>
       <c r="X23" s="3"/>
     </row>
     <row r="24" spans="1:25" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
@@ -3858,10 +3872,10 @@
       <c r="U25" s="184" t="s">
         <v>219</v>
       </c>
-      <c r="V25" s="215" t="s">
+      <c r="V25" s="190" t="s">
         <v>246</v>
       </c>
-      <c r="W25" s="178">
+      <c r="W25" s="230">
         <v>42404</v>
       </c>
       <c r="X25" s="25" t="s">
@@ -3922,10 +3936,10 @@
       <c r="U26" s="189" t="s">
         <v>219</v>
       </c>
-      <c r="V26" s="215" t="s">
+      <c r="V26" s="190" t="s">
         <v>246</v>
       </c>
-      <c r="W26" s="178">
+      <c r="W26" s="230">
         <v>42404</v>
       </c>
       <c r="X26" s="25" t="s">
@@ -3947,46 +3961,46 @@
       </c>
       <c r="E27" s="22"/>
       <c r="F27" s="22"/>
-      <c r="G27" s="221" t="s">
+      <c r="G27" s="196" t="s">
         <v>167</v>
       </c>
-      <c r="H27" s="222">
+      <c r="H27" s="197">
         <v>25</v>
       </c>
-      <c r="I27" s="223" t="s">
+      <c r="I27" s="198" t="s">
         <v>20</v>
       </c>
       <c r="J27" s="176" t="s">
         <v>259</v>
       </c>
-      <c r="K27" s="223" t="s">
+      <c r="K27" s="198" t="s">
         <v>19</v>
       </c>
-      <c r="L27" s="223" t="s">
+      <c r="L27" s="198" t="s">
         <v>8</v>
       </c>
-      <c r="M27" s="223"/>
-      <c r="N27" s="223"/>
+      <c r="M27" s="198"/>
+      <c r="N27" s="198"/>
       <c r="O27" s="176"/>
-      <c r="P27" s="222" t="s">
+      <c r="P27" s="197" t="s">
         <v>19</v>
       </c>
-      <c r="Q27" s="224">
+      <c r="Q27" s="199">
         <v>8</v>
       </c>
-      <c r="R27" s="224" t="s">
+      <c r="R27" s="199" t="s">
         <v>217</v>
       </c>
-      <c r="S27" s="224" t="s">
+      <c r="S27" s="199" t="s">
         <v>218</v>
       </c>
-      <c r="T27" s="224" t="s">
+      <c r="T27" s="199" t="s">
         <v>220</v>
       </c>
-      <c r="U27" s="225" t="s">
+      <c r="U27" s="200" t="s">
         <v>219</v>
       </c>
-      <c r="V27" s="215" t="s">
+      <c r="V27" s="190" t="s">
         <v>246</v>
       </c>
       <c r="W27" s="25" t="s">
@@ -4050,10 +4064,10 @@
       <c r="U28" s="189" t="s">
         <v>219</v>
       </c>
-      <c r="V28" s="215" t="s">
+      <c r="V28" s="190" t="s">
         <v>246</v>
       </c>
-      <c r="W28" s="177">
+      <c r="W28" s="230">
         <v>42404</v>
       </c>
       <c r="X28" s="25" t="s">
@@ -4075,46 +4089,46 @@
       </c>
       <c r="E29" s="25"/>
       <c r="F29" s="25"/>
-      <c r="G29" s="216" t="s">
+      <c r="G29" s="191" t="s">
         <v>169</v>
       </c>
-      <c r="H29" s="217">
+      <c r="H29" s="192">
         <v>27</v>
       </c>
-      <c r="I29" s="218" t="s">
+      <c r="I29" s="193" t="s">
         <v>19</v>
       </c>
       <c r="J29" s="172" t="s">
         <v>170</v>
       </c>
-      <c r="K29" s="218" t="s">
+      <c r="K29" s="193" t="s">
         <v>19</v>
       </c>
-      <c r="L29" s="218" t="s">
+      <c r="L29" s="193" t="s">
         <v>5</v>
       </c>
-      <c r="M29" s="218"/>
-      <c r="N29" s="218"/>
+      <c r="M29" s="193"/>
+      <c r="N29" s="193"/>
       <c r="O29" s="172"/>
-      <c r="P29" s="217" t="s">
+      <c r="P29" s="192" t="s">
         <v>20</v>
       </c>
-      <c r="Q29" s="219">
+      <c r="Q29" s="194">
         <v>8</v>
       </c>
-      <c r="R29" s="219" t="s">
+      <c r="R29" s="194" t="s">
         <v>217</v>
       </c>
-      <c r="S29" s="219" t="s">
+      <c r="S29" s="194" t="s">
         <v>218</v>
       </c>
-      <c r="T29" s="219" t="s">
+      <c r="T29" s="194" t="s">
         <v>169</v>
       </c>
-      <c r="U29" s="220" t="s">
+      <c r="U29" s="195" t="s">
         <v>219</v>
       </c>
-      <c r="V29" s="228" t="s">
+      <c r="V29" s="203" t="s">
         <v>246</v>
       </c>
       <c r="W29" s="25"/>
@@ -4330,39 +4344,39 @@
       </c>
       <c r="E33" s="76"/>
       <c r="F33" s="76"/>
-      <c r="G33" s="221" t="s">
+      <c r="G33" s="196" t="s">
         <v>10</v>
       </c>
-      <c r="H33" s="222">
+      <c r="H33" s="197">
         <v>31</v>
       </c>
-      <c r="I33" s="223" t="s">
+      <c r="I33" s="198" t="s">
         <v>20</v>
       </c>
       <c r="J33" s="176" t="s">
         <v>179</v>
       </c>
-      <c r="K33" s="223" t="s">
+      <c r="K33" s="198" t="s">
         <v>20</v>
       </c>
-      <c r="L33" s="223" t="s">
+      <c r="L33" s="198" t="s">
         <v>10</v>
       </c>
-      <c r="M33" s="223"/>
-      <c r="N33" s="223"/>
+      <c r="M33" s="198"/>
+      <c r="N33" s="198"/>
       <c r="O33" s="176"/>
-      <c r="P33" s="222" t="s">
+      <c r="P33" s="197" t="s">
         <v>19</v>
       </c>
-      <c r="Q33" s="224"/>
-      <c r="R33" s="224"/>
-      <c r="S33" s="224"/>
-      <c r="T33" s="224"/>
-      <c r="U33" s="224"/>
-      <c r="V33" s="226" t="s">
+      <c r="Q33" s="199"/>
+      <c r="R33" s="199"/>
+      <c r="S33" s="199"/>
+      <c r="T33" s="199"/>
+      <c r="U33" s="199"/>
+      <c r="V33" s="201" t="s">
         <v>246</v>
       </c>
-      <c r="W33" s="222"/>
+      <c r="W33" s="197"/>
       <c r="X33" s="175"/>
     </row>
     <row r="34" spans="1:24" ht="15.75" x14ac:dyDescent="0.25">
@@ -5772,6 +5786,12 @@
     <row r="287" hidden="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="20">
+    <mergeCell ref="P1:P2"/>
+    <mergeCell ref="U1:U2"/>
+    <mergeCell ref="T1:T2"/>
+    <mergeCell ref="S1:S2"/>
+    <mergeCell ref="R1:R2"/>
+    <mergeCell ref="Q1:Q2"/>
     <mergeCell ref="I1:I2"/>
     <mergeCell ref="H1:H2"/>
     <mergeCell ref="O1:O2"/>
@@ -5786,12 +5806,6 @@
     <mergeCell ref="D1:D2"/>
     <mergeCell ref="C1:C2"/>
     <mergeCell ref="F1:F2"/>
-    <mergeCell ref="P1:P2"/>
-    <mergeCell ref="U1:U2"/>
-    <mergeCell ref="T1:T2"/>
-    <mergeCell ref="S1:S2"/>
-    <mergeCell ref="R1:R2"/>
-    <mergeCell ref="Q1:Q2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Actualizando estado recursos MA_08_09_CO
</commit_message>
<xml_diff>
--- a/fuentes/contenidos/grado08/guion08/ESCALETA_MA_08_08_CO.xlsx
+++ b/fuentes/contenidos/grado08/guion08/ESCALETA_MA_08_08_CO.xlsx
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="686" uniqueCount="273">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="688" uniqueCount="271">
   <si>
     <t>Asignatura</t>
   </si>
@@ -949,9 +949,6 @@
     <t>Actividad para deducir el valor de ángulos en polígonos y circunferencias</t>
   </si>
   <si>
-    <t>Se deben arreglar las fichas de docente y estudiante</t>
-  </si>
-  <si>
     <t>Corrección de estilo y edición con imágenes, esta en carpeta</t>
   </si>
   <si>
@@ -964,22 +961,19 @@
     <t>Listos 8</t>
   </si>
   <si>
-    <t>Faltan 20</t>
-  </si>
-  <si>
-    <t>En proceso 1</t>
-  </si>
-  <si>
     <t>En proceso 7</t>
   </si>
   <si>
     <t>Faltan 17</t>
   </si>
   <si>
-    <t>Listos 18</t>
-  </si>
-  <si>
-    <t>Faltan 14</t>
+    <t>Listos 19</t>
+  </si>
+  <si>
+    <t>Faltan 13</t>
+  </si>
+  <si>
+    <t>Faltan 15</t>
   </si>
 </sst>
 </file>
@@ -1371,7 +1365,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="225">
+  <cellXfs count="218">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
@@ -1760,7 +1754,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="17" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="18" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="16" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1801,21 +1794,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="19" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="17" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="17" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="17" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="17" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="17" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="19" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -1835,7 +1813,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="17" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="17" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="18" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1890,18 +1867,36 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="16" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="12" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="10" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="11" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="12" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="12" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1945,24 +1940,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="10" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="9" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="11" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -2271,9 +2248,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Y287"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="Q1" zoomScale="70" zoomScaleNormal="70" zoomScalePageLayoutView="91" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="I1" zoomScale="70" zoomScaleNormal="70" zoomScalePageLayoutView="91" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A6" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G32" sqref="G32"/>
+      <selection pane="bottomLeft" activeCell="Y23" sqref="Y23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2305,103 +2282,103 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:25" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="206" t="s">
+      <c r="A1" s="205" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="204" t="s">
+      <c r="B1" s="203" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="217" t="s">
+      <c r="C1" s="216" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="206" t="s">
+      <c r="D1" s="205" t="s">
         <v>110</v>
       </c>
-      <c r="E1" s="204" t="s">
+      <c r="E1" s="203" t="s">
         <v>111</v>
       </c>
-      <c r="F1" s="200" t="s">
+      <c r="F1" s="201" t="s">
         <v>112</v>
       </c>
-      <c r="G1" s="215" t="s">
+      <c r="G1" s="214" t="s">
         <v>3</v>
       </c>
-      <c r="H1" s="200" t="s">
+      <c r="H1" s="201" t="s">
         <v>113</v>
       </c>
-      <c r="I1" s="200" t="s">
+      <c r="I1" s="201" t="s">
         <v>107</v>
       </c>
-      <c r="J1" s="212" t="s">
+      <c r="J1" s="211" t="s">
         <v>4</v>
       </c>
-      <c r="K1" s="210" t="s">
+      <c r="K1" s="209" t="s">
         <v>108</v>
       </c>
-      <c r="L1" s="208" t="s">
+      <c r="L1" s="207" t="s">
         <v>14</v>
       </c>
-      <c r="M1" s="214" t="s">
+      <c r="M1" s="213" t="s">
         <v>21</v>
       </c>
-      <c r="N1" s="214"/>
-      <c r="O1" s="202" t="s">
+      <c r="N1" s="213"/>
+      <c r="O1" s="193" t="s">
         <v>109</v>
       </c>
-      <c r="P1" s="202" t="s">
+      <c r="P1" s="193" t="s">
         <v>114</v>
       </c>
-      <c r="Q1" s="219" t="s">
+      <c r="Q1" s="195" t="s">
         <v>85</v>
       </c>
-      <c r="R1" s="223" t="s">
+      <c r="R1" s="199" t="s">
         <v>86</v>
       </c>
-      <c r="S1" s="219" t="s">
+      <c r="S1" s="195" t="s">
         <v>87</v>
       </c>
-      <c r="T1" s="221" t="s">
+      <c r="T1" s="197" t="s">
         <v>88</v>
       </c>
-      <c r="U1" s="219" t="s">
+      <c r="U1" s="195" t="s">
         <v>89</v>
       </c>
-      <c r="V1" s="178" t="s">
+      <c r="V1" s="172" t="s">
         <v>251</v>
       </c>
-      <c r="W1" s="149" t="s">
+      <c r="W1" s="148" t="s">
         <v>255</v>
       </c>
-      <c r="X1" s="150" t="s">
+      <c r="X1" s="149" t="s">
         <v>256</v>
       </c>
     </row>
     <row r="2" spans="1:25" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="207"/>
-      <c r="B2" s="205"/>
-      <c r="C2" s="218"/>
-      <c r="D2" s="207"/>
-      <c r="E2" s="205"/>
-      <c r="F2" s="201"/>
-      <c r="G2" s="216"/>
-      <c r="H2" s="201"/>
-      <c r="I2" s="201"/>
-      <c r="J2" s="213"/>
-      <c r="K2" s="211"/>
-      <c r="L2" s="209"/>
+      <c r="A2" s="206"/>
+      <c r="B2" s="204"/>
+      <c r="C2" s="217"/>
+      <c r="D2" s="206"/>
+      <c r="E2" s="204"/>
+      <c r="F2" s="202"/>
+      <c r="G2" s="215"/>
+      <c r="H2" s="202"/>
+      <c r="I2" s="202"/>
+      <c r="J2" s="212"/>
+      <c r="K2" s="210"/>
+      <c r="L2" s="208"/>
       <c r="M2" s="5" t="s">
         <v>90</v>
       </c>
       <c r="N2" s="5" t="s">
         <v>91</v>
       </c>
-      <c r="O2" s="203"/>
-      <c r="P2" s="203"/>
-      <c r="Q2" s="220"/>
-      <c r="R2" s="224"/>
-      <c r="S2" s="220"/>
-      <c r="T2" s="222"/>
-      <c r="U2" s="220"/>
+      <c r="O2" s="194"/>
+      <c r="P2" s="194"/>
+      <c r="Q2" s="196"/>
+      <c r="R2" s="200"/>
+      <c r="S2" s="196"/>
+      <c r="T2" s="198"/>
+      <c r="U2" s="196"/>
       <c r="V2" s="143"/>
       <c r="W2" s="3"/>
       <c r="X2" s="3"/>
@@ -2421,54 +2398,54 @@
       </c>
       <c r="E3" s="119"/>
       <c r="F3" s="119"/>
-      <c r="G3" s="189" t="s">
+      <c r="G3" s="182" t="s">
         <v>125</v>
       </c>
-      <c r="H3" s="190">
+      <c r="H3" s="183">
         <v>1</v>
       </c>
-      <c r="I3" s="190" t="s">
+      <c r="I3" s="183" t="s">
         <v>19</v>
       </c>
-      <c r="J3" s="191" t="s">
+      <c r="J3" s="184" t="s">
         <v>225</v>
       </c>
-      <c r="K3" s="190" t="s">
+      <c r="K3" s="183" t="s">
         <v>20</v>
       </c>
-      <c r="L3" s="190" t="s">
+      <c r="L3" s="183" t="s">
         <v>5</v>
       </c>
-      <c r="M3" s="190" t="s">
+      <c r="M3" s="183" t="s">
         <v>60</v>
       </c>
-      <c r="N3" s="190"/>
-      <c r="O3" s="191" t="s">
+      <c r="N3" s="183"/>
+      <c r="O3" s="184" t="s">
         <v>234</v>
       </c>
-      <c r="P3" s="192" t="s">
+      <c r="P3" s="185" t="s">
         <v>19</v>
       </c>
-      <c r="Q3" s="193">
+      <c r="Q3" s="186">
         <v>6</v>
       </c>
-      <c r="R3" s="193" t="s">
+      <c r="R3" s="186" t="s">
         <v>188</v>
       </c>
-      <c r="S3" s="193" t="s">
+      <c r="S3" s="186" t="s">
         <v>189</v>
       </c>
-      <c r="T3" s="194" t="s">
+      <c r="T3" s="187" t="s">
         <v>190</v>
       </c>
-      <c r="U3" s="195" t="s">
+      <c r="U3" s="188" t="s">
         <v>191</v>
       </c>
-      <c r="V3" s="166" t="s">
+      <c r="V3" s="165" t="s">
         <v>250</v>
       </c>
       <c r="W3" s="3"/>
-      <c r="X3" s="182">
+      <c r="X3" s="175">
         <v>42411</v>
       </c>
     </row>
@@ -2551,58 +2528,58 @@
       </c>
       <c r="E5" s="20"/>
       <c r="F5" s="20"/>
-      <c r="G5" s="183" t="s">
+      <c r="G5" s="176" t="s">
         <v>128</v>
       </c>
-      <c r="H5" s="184">
+      <c r="H5" s="177">
         <v>3</v>
       </c>
-      <c r="I5" s="184" t="s">
+      <c r="I5" s="177" t="s">
         <v>19</v>
       </c>
-      <c r="J5" s="150" t="s">
+      <c r="J5" s="149" t="s">
         <v>226</v>
       </c>
-      <c r="K5" s="184" t="s">
+      <c r="K5" s="177" t="s">
         <v>20</v>
       </c>
-      <c r="L5" s="184" t="s">
+      <c r="L5" s="177" t="s">
         <v>5</v>
       </c>
-      <c r="M5" s="184" t="s">
+      <c r="M5" s="177" t="s">
         <v>53</v>
       </c>
-      <c r="N5" s="184"/>
-      <c r="O5" s="196" t="s">
+      <c r="N5" s="177"/>
+      <c r="O5" s="189" t="s">
         <v>129</v>
       </c>
-      <c r="P5" s="185" t="s">
+      <c r="P5" s="178" t="s">
         <v>20</v>
       </c>
-      <c r="Q5" s="186">
+      <c r="Q5" s="179">
         <v>6</v>
       </c>
-      <c r="R5" s="186" t="s">
+      <c r="R5" s="179" t="s">
         <v>188</v>
       </c>
-      <c r="S5" s="186" t="s">
+      <c r="S5" s="179" t="s">
         <v>189</v>
       </c>
-      <c r="T5" s="187" t="s">
+      <c r="T5" s="180" t="s">
         <v>196</v>
       </c>
-      <c r="U5" s="188" t="s">
+      <c r="U5" s="181" t="s">
         <v>191</v>
       </c>
-      <c r="V5" s="166" t="s">
+      <c r="V5" s="165" t="s">
         <v>253</v>
       </c>
       <c r="W5" s="3"/>
-      <c r="X5" s="182">
+      <c r="X5" s="175">
         <v>42412</v>
       </c>
       <c r="Y5" s="114" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
     </row>
     <row r="6" spans="1:25" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
@@ -2684,56 +2661,56 @@
       </c>
       <c r="E7" s="40"/>
       <c r="F7" s="40"/>
-      <c r="G7" s="197" t="s">
+      <c r="G7" s="190" t="s">
         <v>132</v>
       </c>
-      <c r="H7" s="190">
+      <c r="H7" s="183">
         <v>5</v>
       </c>
-      <c r="I7" s="190" t="s">
+      <c r="I7" s="183" t="s">
         <v>19</v>
       </c>
-      <c r="J7" s="198" t="s">
+      <c r="J7" s="191" t="s">
         <v>237</v>
       </c>
-      <c r="K7" s="190" t="s">
+      <c r="K7" s="183" t="s">
         <v>20</v>
       </c>
-      <c r="L7" s="190" t="s">
+      <c r="L7" s="183" t="s">
         <v>5</v>
       </c>
-      <c r="M7" s="190" t="s">
+      <c r="M7" s="183" t="s">
         <v>57</v>
       </c>
-      <c r="N7" s="190"/>
-      <c r="O7" s="191" t="s">
+      <c r="N7" s="183"/>
+      <c r="O7" s="184" t="s">
         <v>235</v>
       </c>
-      <c r="P7" s="192" t="s">
+      <c r="P7" s="185" t="s">
         <v>19</v>
       </c>
-      <c r="Q7" s="193">
+      <c r="Q7" s="186">
         <v>6</v>
       </c>
-      <c r="R7" s="193" t="s">
+      <c r="R7" s="186" t="s">
         <v>188</v>
       </c>
-      <c r="S7" s="193" t="s">
+      <c r="S7" s="186" t="s">
         <v>189</v>
       </c>
-      <c r="T7" s="194" t="s">
+      <c r="T7" s="187" t="s">
         <v>198</v>
       </c>
-      <c r="U7" s="195" t="s">
+      <c r="U7" s="188" t="s">
         <v>191</v>
       </c>
-      <c r="V7" s="166" t="s">
+      <c r="V7" s="165" t="s">
         <v>252</v>
       </c>
-      <c r="W7" s="181">
+      <c r="W7" s="174">
         <v>42412</v>
       </c>
-      <c r="X7" s="182">
+      <c r="X7" s="175">
         <v>42047</v>
       </c>
     </row>
@@ -2816,53 +2793,53 @@
       </c>
       <c r="E9" s="20"/>
       <c r="F9" s="20"/>
-      <c r="G9" s="161" t="s">
+      <c r="G9" s="160" t="s">
         <v>223</v>
       </c>
-      <c r="H9" s="163">
+      <c r="H9" s="162">
         <v>7</v>
       </c>
-      <c r="I9" s="163" t="s">
+      <c r="I9" s="162" t="s">
         <v>20</v>
       </c>
-      <c r="J9" s="149" t="s">
+      <c r="J9" s="148" t="s">
         <v>227</v>
       </c>
-      <c r="K9" s="163" t="s">
+      <c r="K9" s="162" t="s">
         <v>20</v>
       </c>
-      <c r="L9" s="163" t="s">
+      <c r="L9" s="162" t="s">
         <v>8</v>
       </c>
-      <c r="M9" s="163"/>
-      <c r="N9" s="163" t="s">
+      <c r="M9" s="162"/>
+      <c r="N9" s="162" t="s">
         <v>32</v>
       </c>
-      <c r="O9" s="149" t="s">
+      <c r="O9" s="148" t="s">
         <v>136</v>
       </c>
-      <c r="P9" s="162" t="s">
+      <c r="P9" s="161" t="s">
         <v>20</v>
       </c>
-      <c r="Q9" s="164">
+      <c r="Q9" s="163">
         <v>6</v>
       </c>
-      <c r="R9" s="164" t="s">
+      <c r="R9" s="163" t="s">
         <v>192</v>
       </c>
-      <c r="S9" s="164" t="s">
+      <c r="S9" s="163" t="s">
         <v>193</v>
       </c>
-      <c r="T9" s="180" t="s">
+      <c r="T9" s="173" t="s">
         <v>200</v>
       </c>
-      <c r="U9" s="165" t="s">
+      <c r="U9" s="164" t="s">
         <v>195</v>
       </c>
-      <c r="V9" s="166" t="s">
+      <c r="V9" s="165" t="s">
         <v>250</v>
       </c>
-      <c r="W9" s="154">
+      <c r="W9" s="153">
         <v>42408</v>
       </c>
       <c r="X9" s="3" t="s">
@@ -2948,53 +2925,53 @@
       </c>
       <c r="E11" s="21"/>
       <c r="F11" s="21"/>
-      <c r="G11" s="161" t="s">
+      <c r="G11" s="160" t="s">
         <v>138</v>
       </c>
-      <c r="H11" s="163">
+      <c r="H11" s="162">
         <v>9</v>
       </c>
-      <c r="I11" s="163" t="s">
+      <c r="I11" s="162" t="s">
         <v>20</v>
       </c>
-      <c r="J11" s="149" t="s">
+      <c r="J11" s="148" t="s">
         <v>139</v>
       </c>
-      <c r="K11" s="163" t="s">
+      <c r="K11" s="162" t="s">
         <v>20</v>
       </c>
-      <c r="L11" s="163" t="s">
+      <c r="L11" s="162" t="s">
         <v>8</v>
       </c>
-      <c r="M11" s="163"/>
-      <c r="N11" s="163" t="s">
+      <c r="M11" s="162"/>
+      <c r="N11" s="162" t="s">
         <v>24</v>
       </c>
-      <c r="O11" s="149" t="s">
+      <c r="O11" s="148" t="s">
         <v>140</v>
       </c>
-      <c r="P11" s="162" t="s">
+      <c r="P11" s="161" t="s">
         <v>19</v>
       </c>
-      <c r="Q11" s="164">
+      <c r="Q11" s="163">
         <v>6</v>
       </c>
-      <c r="R11" s="164" t="s">
+      <c r="R11" s="163" t="s">
         <v>192</v>
       </c>
-      <c r="S11" s="164" t="s">
+      <c r="S11" s="163" t="s">
         <v>193</v>
       </c>
-      <c r="T11" s="180" t="s">
+      <c r="T11" s="173" t="s">
         <v>202</v>
       </c>
-      <c r="U11" s="165" t="s">
+      <c r="U11" s="164" t="s">
         <v>195</v>
       </c>
-      <c r="V11" s="166" t="s">
+      <c r="V11" s="165" t="s">
         <v>250</v>
       </c>
-      <c r="W11" s="154">
+      <c r="W11" s="153">
         <v>42408</v>
       </c>
       <c r="X11" s="3" t="s">
@@ -3080,56 +3057,56 @@
       </c>
       <c r="E13" s="28"/>
       <c r="F13" s="28"/>
-      <c r="G13" s="197" t="s">
+      <c r="G13" s="190" t="s">
         <v>232</v>
       </c>
-      <c r="H13" s="190">
+      <c r="H13" s="183">
         <v>11</v>
       </c>
-      <c r="I13" s="190" t="s">
+      <c r="I13" s="183" t="s">
         <v>19</v>
       </c>
-      <c r="J13" s="199" t="s">
+      <c r="J13" s="192" t="s">
         <v>238</v>
       </c>
-      <c r="K13" s="190" t="s">
+      <c r="K13" s="183" t="s">
         <v>20</v>
       </c>
-      <c r="L13" s="190" t="s">
+      <c r="L13" s="183" t="s">
         <v>5</v>
       </c>
-      <c r="M13" s="190" t="s">
+      <c r="M13" s="183" t="s">
         <v>54</v>
       </c>
-      <c r="N13" s="190"/>
-      <c r="O13" s="199" t="s">
+      <c r="N13" s="183"/>
+      <c r="O13" s="192" t="s">
         <v>239</v>
       </c>
-      <c r="P13" s="192" t="s">
+      <c r="P13" s="185" t="s">
         <v>19</v>
       </c>
-      <c r="Q13" s="193">
+      <c r="Q13" s="186">
         <v>6</v>
       </c>
-      <c r="R13" s="193" t="s">
+      <c r="R13" s="186" t="s">
         <v>188</v>
       </c>
-      <c r="S13" s="193" t="s">
+      <c r="S13" s="186" t="s">
         <v>189</v>
       </c>
-      <c r="T13" s="194" t="s">
+      <c r="T13" s="187" t="s">
         <v>204</v>
       </c>
-      <c r="U13" s="195" t="s">
+      <c r="U13" s="188" t="s">
         <v>191</v>
       </c>
-      <c r="V13" s="166" t="s">
+      <c r="V13" s="165" t="s">
         <v>252</v>
       </c>
-      <c r="W13" s="181">
+      <c r="W13" s="174">
         <v>42412</v>
       </c>
-      <c r="X13" s="182">
+      <c r="X13" s="175">
         <v>42412</v>
       </c>
     </row>
@@ -3148,53 +3125,53 @@
       </c>
       <c r="E14" s="31"/>
       <c r="F14" s="31"/>
-      <c r="G14" s="161" t="s">
+      <c r="G14" s="160" t="s">
         <v>144</v>
       </c>
-      <c r="H14" s="163">
+      <c r="H14" s="162">
         <v>12</v>
       </c>
-      <c r="I14" s="163" t="s">
+      <c r="I14" s="162" t="s">
         <v>20</v>
       </c>
-      <c r="J14" s="149" t="s">
+      <c r="J14" s="148" t="s">
         <v>145</v>
       </c>
-      <c r="K14" s="163" t="s">
+      <c r="K14" s="162" t="s">
         <v>20</v>
       </c>
-      <c r="L14" s="163" t="s">
+      <c r="L14" s="162" t="s">
         <v>8</v>
       </c>
-      <c r="M14" s="163"/>
-      <c r="N14" s="163" t="s">
+      <c r="M14" s="162"/>
+      <c r="N14" s="162" t="s">
         <v>27</v>
       </c>
-      <c r="O14" s="149" t="s">
+      <c r="O14" s="148" t="s">
         <v>146</v>
       </c>
-      <c r="P14" s="162" t="s">
+      <c r="P14" s="161" t="s">
         <v>19</v>
       </c>
-      <c r="Q14" s="164">
+      <c r="Q14" s="163">
         <v>6</v>
       </c>
-      <c r="R14" s="164" t="s">
+      <c r="R14" s="163" t="s">
         <v>192</v>
       </c>
-      <c r="S14" s="164" t="s">
+      <c r="S14" s="163" t="s">
         <v>193</v>
       </c>
-      <c r="T14" s="180" t="s">
+      <c r="T14" s="173" t="s">
         <v>205</v>
       </c>
-      <c r="U14" s="165" t="s">
+      <c r="U14" s="164" t="s">
         <v>195</v>
       </c>
-      <c r="V14" s="166" t="s">
+      <c r="V14" s="165" t="s">
         <v>250</v>
       </c>
-      <c r="W14" s="154">
+      <c r="W14" s="153">
         <v>42414</v>
       </c>
       <c r="X14" s="3" t="s">
@@ -3216,56 +3193,56 @@
       </c>
       <c r="E15" s="31"/>
       <c r="F15" s="31"/>
-      <c r="G15" s="183" t="s">
+      <c r="G15" s="176" t="s">
         <v>141</v>
       </c>
-      <c r="H15" s="185">
+      <c r="H15" s="178">
         <v>13</v>
       </c>
-      <c r="I15" s="184" t="s">
+      <c r="I15" s="177" t="s">
         <v>20</v>
       </c>
-      <c r="J15" s="150" t="s">
+      <c r="J15" s="149" t="s">
         <v>229</v>
       </c>
-      <c r="K15" s="184" t="s">
+      <c r="K15" s="177" t="s">
         <v>20</v>
       </c>
-      <c r="L15" s="184" t="s">
+      <c r="L15" s="177" t="s">
         <v>8</v>
       </c>
-      <c r="M15" s="184"/>
-      <c r="N15" s="184" t="s">
+      <c r="M15" s="177"/>
+      <c r="N15" s="177" t="s">
         <v>48</v>
       </c>
-      <c r="O15" s="150" t="s">
+      <c r="O15" s="149" t="s">
         <v>143</v>
       </c>
-      <c r="P15" s="185" t="s">
+      <c r="P15" s="178" t="s">
         <v>19</v>
       </c>
-      <c r="Q15" s="186">
+      <c r="Q15" s="179">
         <v>6</v>
       </c>
-      <c r="R15" s="186" t="s">
+      <c r="R15" s="179" t="s">
         <v>192</v>
       </c>
-      <c r="S15" s="186" t="s">
+      <c r="S15" s="179" t="s">
         <v>193</v>
       </c>
-      <c r="T15" s="187" t="s">
+      <c r="T15" s="180" t="s">
         <v>206</v>
       </c>
-      <c r="U15" s="188" t="s">
+      <c r="U15" s="181" t="s">
         <v>195</v>
       </c>
-      <c r="V15" s="166" t="s">
+      <c r="V15" s="165" t="s">
         <v>250</v>
       </c>
-      <c r="W15" s="181">
+      <c r="W15" s="174">
         <v>42414</v>
       </c>
-      <c r="X15" s="182">
+      <c r="X15" s="175">
         <v>42414</v>
       </c>
     </row>
@@ -3284,61 +3261,61 @@
       </c>
       <c r="E16" s="20"/>
       <c r="F16" s="20"/>
-      <c r="G16" s="183" t="s">
+      <c r="G16" s="176" t="s">
         <v>147</v>
       </c>
-      <c r="H16" s="184">
+      <c r="H16" s="177">
         <v>14</v>
       </c>
-      <c r="I16" s="184" t="s">
+      <c r="I16" s="177" t="s">
         <v>20</v>
       </c>
-      <c r="J16" s="150" t="s">
+      <c r="J16" s="149" t="s">
         <v>148</v>
       </c>
-      <c r="K16" s="184" t="s">
+      <c r="K16" s="177" t="s">
         <v>20</v>
       </c>
-      <c r="L16" s="184" t="s">
+      <c r="L16" s="177" t="s">
         <v>8</v>
       </c>
-      <c r="M16" s="184"/>
-      <c r="N16" s="184" t="s">
+      <c r="M16" s="177"/>
+      <c r="N16" s="177" t="s">
         <v>120</v>
       </c>
-      <c r="O16" s="150" t="s">
+      <c r="O16" s="149" t="s">
         <v>149</v>
       </c>
-      <c r="P16" s="185" t="s">
+      <c r="P16" s="178" t="s">
         <v>20</v>
       </c>
-      <c r="Q16" s="186">
+      <c r="Q16" s="179">
         <v>6</v>
       </c>
-      <c r="R16" s="186" t="s">
+      <c r="R16" s="179" t="s">
         <v>192</v>
       </c>
-      <c r="S16" s="186" t="s">
+      <c r="S16" s="179" t="s">
         <v>193</v>
       </c>
-      <c r="T16" s="187" t="s">
+      <c r="T16" s="180" t="s">
         <v>208</v>
       </c>
-      <c r="U16" s="188" t="s">
+      <c r="U16" s="181" t="s">
         <v>195</v>
       </c>
-      <c r="V16" s="166" t="s">
+      <c r="V16" s="165" t="s">
         <v>249</v>
       </c>
       <c r="W16" s="3"/>
-      <c r="X16" s="182">
+      <c r="X16" s="175">
         <v>42410</v>
       </c>
       <c r="Y16" s="4" t="s">
-        <v>263</v>
-      </c>
-    </row>
-    <row r="17" spans="1:25" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="17" spans="1:24" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="32" t="s">
         <v>15</v>
       </c>
@@ -3404,7 +3381,7 @@
       <c r="W17" s="3"/>
       <c r="X17" s="3"/>
     </row>
-    <row r="18" spans="1:25" s="13" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:24" s="13" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A18" s="142" t="s">
         <v>15</v>
       </c>
@@ -3419,56 +3396,56 @@
       </c>
       <c r="E18" s="141"/>
       <c r="F18" s="141"/>
-      <c r="G18" s="155" t="s">
+      <c r="G18" s="154" t="s">
         <v>150</v>
       </c>
-      <c r="H18" s="156">
+      <c r="H18" s="155">
         <v>16</v>
       </c>
-      <c r="I18" s="156" t="s">
+      <c r="I18" s="155" t="s">
         <v>19</v>
       </c>
-      <c r="J18" s="157" t="s">
+      <c r="J18" s="156" t="s">
         <v>230</v>
       </c>
-      <c r="K18" s="156" t="s">
+      <c r="K18" s="155" t="s">
         <v>19</v>
       </c>
-      <c r="L18" s="156" t="s">
+      <c r="L18" s="155" t="s">
         <v>5</v>
       </c>
-      <c r="M18" s="156"/>
-      <c r="N18" s="156"/>
-      <c r="O18" s="157"/>
-      <c r="P18" s="158" t="s">
+      <c r="M18" s="155"/>
+      <c r="N18" s="155"/>
+      <c r="O18" s="156"/>
+      <c r="P18" s="157" t="s">
         <v>20</v>
       </c>
-      <c r="Q18" s="159">
+      <c r="Q18" s="158">
         <v>8</v>
       </c>
-      <c r="R18" s="159" t="s">
+      <c r="R18" s="158" t="s">
         <v>217</v>
       </c>
-      <c r="S18" s="159" t="s">
+      <c r="S18" s="158" t="s">
         <v>218</v>
       </c>
-      <c r="T18" s="159" t="s">
+      <c r="T18" s="158" t="s">
         <v>150</v>
       </c>
-      <c r="U18" s="160" t="s">
+      <c r="U18" s="159" t="s">
         <v>219</v>
       </c>
-      <c r="V18" s="166" t="s">
+      <c r="V18" s="165" t="s">
         <v>246</v>
       </c>
-      <c r="W18" s="181">
+      <c r="W18" s="174">
         <v>42403</v>
       </c>
-      <c r="X18" s="153" t="s">
+      <c r="X18" s="152" t="s">
         <v>257</v>
       </c>
     </row>
-    <row r="19" spans="1:25" s="13" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:24" s="13" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A19" s="137" t="s">
         <v>15</v>
       </c>
@@ -3483,56 +3460,56 @@
       </c>
       <c r="E19" s="20"/>
       <c r="F19" s="20"/>
-      <c r="G19" s="161" t="s">
+      <c r="G19" s="160" t="s">
         <v>224</v>
       </c>
-      <c r="H19" s="162">
+      <c r="H19" s="161">
         <v>17</v>
       </c>
-      <c r="I19" s="163" t="s">
+      <c r="I19" s="162" t="s">
         <v>20</v>
       </c>
-      <c r="J19" s="149" t="s">
+      <c r="J19" s="148" t="s">
         <v>152</v>
       </c>
-      <c r="K19" s="163" t="s">
+      <c r="K19" s="162" t="s">
         <v>19</v>
       </c>
-      <c r="L19" s="163" t="s">
+      <c r="L19" s="162" t="s">
         <v>8</v>
       </c>
-      <c r="M19" s="163"/>
-      <c r="N19" s="163"/>
-      <c r="O19" s="149"/>
-      <c r="P19" s="162" t="s">
+      <c r="M19" s="162"/>
+      <c r="N19" s="162"/>
+      <c r="O19" s="148"/>
+      <c r="P19" s="161" t="s">
         <v>20</v>
       </c>
-      <c r="Q19" s="164">
+      <c r="Q19" s="163">
         <v>8</v>
       </c>
-      <c r="R19" s="164" t="s">
+      <c r="R19" s="163" t="s">
         <v>217</v>
       </c>
-      <c r="S19" s="164" t="s">
+      <c r="S19" s="163" t="s">
         <v>218</v>
       </c>
-      <c r="T19" s="164" t="s">
+      <c r="T19" s="163" t="s">
         <v>151</v>
       </c>
-      <c r="U19" s="165" t="s">
+      <c r="U19" s="164" t="s">
         <v>219</v>
       </c>
-      <c r="V19" s="166" t="s">
+      <c r="V19" s="165" t="s">
         <v>246</v>
       </c>
-      <c r="W19" s="181">
+      <c r="W19" s="174">
         <v>42403</v>
       </c>
       <c r="X19" s="20" t="s">
         <v>257</v>
       </c>
     </row>
-    <row r="20" spans="1:25" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:24" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A20" s="81" t="s">
         <v>15</v>
       </c>
@@ -3547,58 +3524,58 @@
       </c>
       <c r="E20" s="14"/>
       <c r="F20" s="14"/>
-      <c r="G20" s="183" t="s">
+      <c r="G20" s="176" t="s">
         <v>241</v>
       </c>
-      <c r="H20" s="184">
+      <c r="H20" s="177">
         <v>18</v>
       </c>
-      <c r="I20" s="184" t="s">
+      <c r="I20" s="177" t="s">
         <v>19</v>
       </c>
-      <c r="J20" s="150" t="s">
+      <c r="J20" s="149" t="s">
         <v>242</v>
       </c>
-      <c r="K20" s="184" t="s">
+      <c r="K20" s="177" t="s">
         <v>20</v>
       </c>
-      <c r="L20" s="184" t="s">
+      <c r="L20" s="177" t="s">
         <v>5</v>
       </c>
-      <c r="M20" s="184" t="s">
+      <c r="M20" s="177" t="s">
         <v>58</v>
       </c>
-      <c r="N20" s="184"/>
-      <c r="O20" s="150" t="s">
+      <c r="N20" s="177"/>
+      <c r="O20" s="149" t="s">
         <v>153</v>
       </c>
-      <c r="P20" s="185" t="s">
+      <c r="P20" s="178" t="s">
         <v>19</v>
       </c>
-      <c r="Q20" s="186">
+      <c r="Q20" s="179">
         <v>6</v>
       </c>
-      <c r="R20" s="186" t="s">
+      <c r="R20" s="179" t="s">
         <v>188</v>
       </c>
-      <c r="S20" s="186" t="s">
+      <c r="S20" s="179" t="s">
         <v>189</v>
       </c>
-      <c r="T20" s="187" t="s">
+      <c r="T20" s="180" t="s">
         <v>209</v>
       </c>
-      <c r="U20" s="188" t="s">
+      <c r="U20" s="181" t="s">
         <v>191</v>
       </c>
-      <c r="V20" s="166" t="s">
+      <c r="V20" s="165" t="s">
         <v>254</v>
       </c>
       <c r="W20" s="3"/>
-      <c r="X20" s="182">
+      <c r="X20" s="175">
         <v>42415</v>
       </c>
     </row>
-    <row r="21" spans="1:25" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:24" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A21" s="81" t="s">
         <v>15</v>
       </c>
@@ -3662,7 +3639,7 @@
       <c r="W21" s="3"/>
       <c r="X21" s="3"/>
     </row>
-    <row r="22" spans="1:25" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:24" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A22" s="81" t="s">
         <v>15</v>
       </c>
@@ -3726,7 +3703,7 @@
       <c r="W22" s="3"/>
       <c r="X22" s="3"/>
     </row>
-    <row r="23" spans="1:25" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:24" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A23" s="81" t="s">
         <v>15</v>
       </c>
@@ -3741,58 +3718,60 @@
       </c>
       <c r="E23" s="14"/>
       <c r="F23" s="14"/>
-      <c r="G23" s="161" t="s">
+      <c r="G23" s="160" t="s">
         <v>159</v>
       </c>
-      <c r="H23" s="162">
+      <c r="H23" s="161">
         <v>21</v>
       </c>
-      <c r="I23" s="163" t="s">
+      <c r="I23" s="162" t="s">
         <v>20</v>
       </c>
-      <c r="J23" s="149" t="s">
+      <c r="J23" s="148" t="s">
         <v>160</v>
       </c>
-      <c r="K23" s="163" t="s">
+      <c r="K23" s="162" t="s">
         <v>20</v>
       </c>
-      <c r="L23" s="163" t="s">
+      <c r="L23" s="162" t="s">
         <v>8</v>
       </c>
-      <c r="M23" s="163"/>
-      <c r="N23" s="163" t="s">
+      <c r="M23" s="162"/>
+      <c r="N23" s="162" t="s">
         <v>24</v>
       </c>
-      <c r="O23" s="149" t="s">
+      <c r="O23" s="148" t="s">
         <v>161</v>
       </c>
-      <c r="P23" s="162" t="s">
+      <c r="P23" s="161" t="s">
         <v>19</v>
       </c>
-      <c r="Q23" s="164">
+      <c r="Q23" s="163">
         <v>6</v>
       </c>
-      <c r="R23" s="164" t="s">
+      <c r="R23" s="163" t="s">
         <v>192</v>
       </c>
-      <c r="S23" s="164" t="s">
+      <c r="S23" s="163" t="s">
         <v>193</v>
       </c>
-      <c r="T23" s="180" t="s">
+      <c r="T23" s="173" t="s">
         <v>212</v>
       </c>
-      <c r="U23" s="165" t="s">
+      <c r="U23" s="164" t="s">
         <v>195</v>
       </c>
-      <c r="V23" s="166" t="s">
+      <c r="V23" s="165" t="s">
         <v>250</v>
       </c>
-      <c r="W23" s="154">
+      <c r="W23" s="153">
         <v>42408</v>
       </c>
-      <c r="X23" s="3"/>
-    </row>
-    <row r="24" spans="1:25" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="X23" s="3" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="24" spans="1:24" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A24" s="89" t="s">
         <v>15</v>
       </c>
@@ -3856,7 +3835,7 @@
       <c r="W24" s="3"/>
       <c r="X24" s="3"/>
     </row>
-    <row r="25" spans="1:25" s="13" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:24" s="13" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A25" s="63" t="s">
         <v>15</v>
       </c>
@@ -3871,56 +3850,56 @@
       </c>
       <c r="E25" s="16"/>
       <c r="F25" s="16"/>
-      <c r="G25" s="155" t="s">
+      <c r="G25" s="154" t="s">
         <v>258</v>
       </c>
-      <c r="H25" s="156">
+      <c r="H25" s="155">
         <v>23</v>
       </c>
-      <c r="I25" s="156" t="s">
+      <c r="I25" s="155" t="s">
         <v>20</v>
       </c>
-      <c r="J25" s="157" t="s">
+      <c r="J25" s="156" t="s">
         <v>164</v>
       </c>
-      <c r="K25" s="156" t="s">
+      <c r="K25" s="155" t="s">
         <v>19</v>
       </c>
-      <c r="L25" s="156" t="s">
+      <c r="L25" s="155" t="s">
         <v>8</v>
       </c>
-      <c r="M25" s="156"/>
-      <c r="N25" s="156"/>
-      <c r="O25" s="157"/>
-      <c r="P25" s="158" t="s">
+      <c r="M25" s="155"/>
+      <c r="N25" s="155"/>
+      <c r="O25" s="156"/>
+      <c r="P25" s="157" t="s">
         <v>19</v>
       </c>
-      <c r="Q25" s="159">
+      <c r="Q25" s="158">
         <v>8</v>
       </c>
-      <c r="R25" s="159" t="s">
+      <c r="R25" s="158" t="s">
         <v>217</v>
       </c>
-      <c r="S25" s="159" t="s">
+      <c r="S25" s="158" t="s">
         <v>218</v>
       </c>
-      <c r="T25" s="159" t="s">
+      <c r="T25" s="158" t="s">
         <v>163</v>
       </c>
-      <c r="U25" s="160" t="s">
+      <c r="U25" s="159" t="s">
         <v>219</v>
       </c>
-      <c r="V25" s="166" t="s">
+      <c r="V25" s="165" t="s">
         <v>246</v>
       </c>
-      <c r="W25" s="181">
+      <c r="W25" s="174">
         <v>42404</v>
       </c>
       <c r="X25" s="20" t="s">
         <v>257</v>
       </c>
     </row>
-    <row r="26" spans="1:25" s="13" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:24" s="13" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A26" s="65" t="s">
         <v>15</v>
       </c>
@@ -3935,56 +3914,56 @@
       </c>
       <c r="E26" s="17"/>
       <c r="F26" s="17"/>
-      <c r="G26" s="161" t="s">
+      <c r="G26" s="160" t="s">
         <v>165</v>
       </c>
-      <c r="H26" s="162">
+      <c r="H26" s="161">
         <v>24</v>
       </c>
-      <c r="I26" s="163" t="s">
+      <c r="I26" s="162" t="s">
         <v>20</v>
       </c>
-      <c r="J26" s="149" t="s">
+      <c r="J26" s="148" t="s">
         <v>166</v>
       </c>
-      <c r="K26" s="163" t="s">
+      <c r="K26" s="162" t="s">
         <v>19</v>
       </c>
-      <c r="L26" s="163" t="s">
+      <c r="L26" s="162" t="s">
         <v>8</v>
       </c>
-      <c r="M26" s="163"/>
-      <c r="N26" s="163"/>
-      <c r="O26" s="149"/>
-      <c r="P26" s="162" t="s">
+      <c r="M26" s="162"/>
+      <c r="N26" s="162"/>
+      <c r="O26" s="148"/>
+      <c r="P26" s="161" t="s">
         <v>19</v>
       </c>
-      <c r="Q26" s="164">
+      <c r="Q26" s="163">
         <v>8</v>
       </c>
-      <c r="R26" s="164" t="s">
+      <c r="R26" s="163" t="s">
         <v>217</v>
       </c>
-      <c r="S26" s="164" t="s">
+      <c r="S26" s="163" t="s">
         <v>218</v>
       </c>
-      <c r="T26" s="164" t="s">
+      <c r="T26" s="163" t="s">
         <v>165</v>
       </c>
-      <c r="U26" s="165" t="s">
+      <c r="U26" s="164" t="s">
         <v>219</v>
       </c>
-      <c r="V26" s="166" t="s">
+      <c r="V26" s="165" t="s">
         <v>246</v>
       </c>
-      <c r="W26" s="181">
+      <c r="W26" s="174">
         <v>42404</v>
       </c>
       <c r="X26" s="20" t="s">
         <v>257</v>
       </c>
     </row>
-    <row r="27" spans="1:25" s="13" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:24" s="13" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A27" s="65" t="s">
         <v>15</v>
       </c>
@@ -3999,46 +3978,46 @@
       </c>
       <c r="E27" s="17"/>
       <c r="F27" s="17"/>
-      <c r="G27" s="172" t="s">
+      <c r="G27" s="166" t="s">
         <v>167</v>
       </c>
-      <c r="H27" s="173">
+      <c r="H27" s="167">
         <v>25</v>
       </c>
-      <c r="I27" s="174" t="s">
+      <c r="I27" s="168" t="s">
         <v>20</v>
       </c>
-      <c r="J27" s="152" t="s">
+      <c r="J27" s="151" t="s">
         <v>259</v>
       </c>
-      <c r="K27" s="174" t="s">
+      <c r="K27" s="168" t="s">
         <v>19</v>
       </c>
-      <c r="L27" s="174" t="s">
+      <c r="L27" s="168" t="s">
         <v>8</v>
       </c>
-      <c r="M27" s="174"/>
-      <c r="N27" s="174"/>
-      <c r="O27" s="152"/>
-      <c r="P27" s="173" t="s">
+      <c r="M27" s="168"/>
+      <c r="N27" s="168"/>
+      <c r="O27" s="151"/>
+      <c r="P27" s="167" t="s">
         <v>19</v>
       </c>
-      <c r="Q27" s="175">
+      <c r="Q27" s="169">
         <v>8</v>
       </c>
-      <c r="R27" s="175" t="s">
+      <c r="R27" s="169" t="s">
         <v>217</v>
       </c>
-      <c r="S27" s="175" t="s">
+      <c r="S27" s="169" t="s">
         <v>218</v>
       </c>
-      <c r="T27" s="175" t="s">
+      <c r="T27" s="169" t="s">
         <v>220</v>
       </c>
-      <c r="U27" s="176" t="s">
+      <c r="U27" s="170" t="s">
         <v>219</v>
       </c>
-      <c r="V27" s="166" t="s">
+      <c r="V27" s="165" t="s">
         <v>246</v>
       </c>
       <c r="W27" s="20" t="s">
@@ -4048,7 +4027,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="28" spans="1:25" s="13" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:24" s="13" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A28" s="65" t="s">
         <v>15</v>
       </c>
@@ -4063,56 +4042,56 @@
       </c>
       <c r="E28" s="17"/>
       <c r="F28" s="17"/>
-      <c r="G28" s="161" t="s">
+      <c r="G28" s="160" t="s">
         <v>168</v>
       </c>
-      <c r="H28" s="163">
+      <c r="H28" s="162">
         <v>26</v>
       </c>
-      <c r="I28" s="163" t="s">
+      <c r="I28" s="162" t="s">
         <v>20</v>
       </c>
-      <c r="J28" s="149" t="s">
+      <c r="J28" s="148" t="s">
         <v>261</v>
       </c>
-      <c r="K28" s="163" t="s">
+      <c r="K28" s="162" t="s">
         <v>19</v>
       </c>
-      <c r="L28" s="163" t="s">
+      <c r="L28" s="162" t="s">
         <v>8</v>
       </c>
-      <c r="M28" s="163"/>
-      <c r="N28" s="163"/>
-      <c r="O28" s="149"/>
-      <c r="P28" s="162" t="s">
+      <c r="M28" s="162"/>
+      <c r="N28" s="162"/>
+      <c r="O28" s="148"/>
+      <c r="P28" s="161" t="s">
         <v>19</v>
       </c>
-      <c r="Q28" s="164">
+      <c r="Q28" s="163">
         <v>8</v>
       </c>
-      <c r="R28" s="164" t="s">
+      <c r="R28" s="163" t="s">
         <v>217</v>
       </c>
-      <c r="S28" s="164" t="s">
+      <c r="S28" s="163" t="s">
         <v>218</v>
       </c>
-      <c r="T28" s="164" t="s">
+      <c r="T28" s="163" t="s">
         <v>221</v>
       </c>
-      <c r="U28" s="165" t="s">
+      <c r="U28" s="164" t="s">
         <v>219</v>
       </c>
-      <c r="V28" s="166" t="s">
+      <c r="V28" s="165" t="s">
         <v>246</v>
       </c>
-      <c r="W28" s="181">
+      <c r="W28" s="174">
         <v>42404</v>
       </c>
       <c r="X28" s="20" t="s">
         <v>257</v>
       </c>
     </row>
-    <row r="29" spans="1:25" s="13" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:24" s="13" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A29" s="137" t="s">
         <v>15</v>
       </c>
@@ -4127,55 +4106,56 @@
       </c>
       <c r="E29" s="20"/>
       <c r="F29" s="20"/>
-      <c r="G29" s="167" t="s">
+      <c r="G29" s="166" t="s">
         <v>169</v>
       </c>
-      <c r="H29" s="168">
+      <c r="H29" s="167">
         <v>27</v>
       </c>
-      <c r="I29" s="169" t="s">
+      <c r="I29" s="168" t="s">
         <v>19</v>
       </c>
-      <c r="J29" s="148" t="s">
+      <c r="J29" s="151" t="s">
         <v>170</v>
       </c>
-      <c r="K29" s="169" t="s">
+      <c r="K29" s="168" t="s">
         <v>19</v>
       </c>
-      <c r="L29" s="169" t="s">
+      <c r="L29" s="168" t="s">
         <v>5</v>
       </c>
-      <c r="M29" s="169"/>
-      <c r="N29" s="169"/>
-      <c r="O29" s="148"/>
-      <c r="P29" s="168" t="s">
+      <c r="M29" s="168"/>
+      <c r="N29" s="168"/>
+      <c r="O29" s="151"/>
+      <c r="P29" s="167" t="s">
         <v>20</v>
       </c>
-      <c r="Q29" s="170">
+      <c r="Q29" s="169">
         <v>8</v>
       </c>
-      <c r="R29" s="170" t="s">
+      <c r="R29" s="169" t="s">
         <v>217</v>
       </c>
-      <c r="S29" s="170" t="s">
+      <c r="S29" s="169" t="s">
         <v>218</v>
       </c>
-      <c r="T29" s="170" t="s">
+      <c r="T29" s="169" t="s">
         <v>169</v>
       </c>
-      <c r="U29" s="171" t="s">
+      <c r="U29" s="170" t="s">
         <v>219</v>
       </c>
-      <c r="V29" s="179" t="s">
+      <c r="V29" s="165" t="s">
         <v>246</v>
       </c>
-      <c r="W29" s="20"/>
-      <c r="X29" s="20"/>
-      <c r="Y29" s="13" t="s">
-        <v>262</v>
-      </c>
-    </row>
-    <row r="30" spans="1:25" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="W29" s="20" t="s">
+        <v>260</v>
+      </c>
+      <c r="X29" s="20" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="30" spans="1:24" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A30" s="65" t="s">
         <v>15</v>
       </c>
@@ -4236,10 +4216,10 @@
       <c r="V30" s="146" t="s">
         <v>248</v>
       </c>
-      <c r="W30" s="151"/>
-      <c r="X30" s="151"/>
-    </row>
-    <row r="31" spans="1:25" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="W30" s="150"/>
+      <c r="X30" s="150"/>
+    </row>
+    <row r="31" spans="1:24" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A31" s="73" t="s">
         <v>15</v>
       </c>
@@ -4300,10 +4280,10 @@
       <c r="V31" s="147" t="s">
         <v>248</v>
       </c>
-      <c r="W31" s="151"/>
-      <c r="X31" s="151"/>
-    </row>
-    <row r="32" spans="1:25" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="W31" s="150"/>
+      <c r="X31" s="150"/>
+    </row>
+    <row r="32" spans="1:24" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A32" s="56" t="s">
         <v>15</v>
       </c>
@@ -4364,8 +4344,8 @@
       <c r="V32" s="146" t="s">
         <v>254</v>
       </c>
-      <c r="W32" s="151"/>
-      <c r="X32" s="151"/>
+      <c r="W32" s="150"/>
+      <c r="X32" s="150"/>
     </row>
     <row r="33" spans="1:24" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A33" s="56" t="s">
@@ -4382,40 +4362,42 @@
       </c>
       <c r="E33" s="57"/>
       <c r="F33" s="57"/>
-      <c r="G33" s="172" t="s">
+      <c r="G33" s="166" t="s">
         <v>10</v>
       </c>
-      <c r="H33" s="173">
+      <c r="H33" s="167">
         <v>31</v>
       </c>
-      <c r="I33" s="174" t="s">
+      <c r="I33" s="168" t="s">
         <v>20</v>
       </c>
-      <c r="J33" s="152" t="s">
+      <c r="J33" s="151" t="s">
         <v>179</v>
       </c>
-      <c r="K33" s="174" t="s">
+      <c r="K33" s="168" t="s">
         <v>20</v>
       </c>
-      <c r="L33" s="174" t="s">
+      <c r="L33" s="168" t="s">
         <v>10</v>
       </c>
-      <c r="M33" s="174"/>
-      <c r="N33" s="174"/>
-      <c r="O33" s="152"/>
-      <c r="P33" s="173" t="s">
+      <c r="M33" s="168"/>
+      <c r="N33" s="168"/>
+      <c r="O33" s="151"/>
+      <c r="P33" s="167" t="s">
         <v>19</v>
       </c>
-      <c r="Q33" s="175"/>
-      <c r="R33" s="175"/>
-      <c r="S33" s="175"/>
-      <c r="T33" s="175"/>
-      <c r="U33" s="175"/>
-      <c r="V33" s="177" t="s">
+      <c r="Q33" s="169"/>
+      <c r="R33" s="169"/>
+      <c r="S33" s="169"/>
+      <c r="T33" s="169"/>
+      <c r="U33" s="169"/>
+      <c r="V33" s="171" t="s">
         <v>246</v>
       </c>
-      <c r="W33" s="173"/>
-      <c r="X33" s="151"/>
+      <c r="W33" s="167"/>
+      <c r="X33" s="150" t="s">
+        <v>260</v>
+      </c>
     </row>
     <row r="34" spans="1:24" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A34" s="56" t="s">
@@ -4476,8 +4458,8 @@
       <c r="V34" s="146" t="s">
         <v>247</v>
       </c>
-      <c r="W34" s="151"/>
-      <c r="X34" s="151"/>
+      <c r="W34" s="150"/>
+      <c r="X34" s="150"/>
     </row>
     <row r="35" spans="1:24" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A35" s="106" t="s">
@@ -4538,8 +4520,8 @@
       <c r="V35" s="147" t="s">
         <v>248</v>
       </c>
-      <c r="W35" s="151"/>
-      <c r="X35" s="151"/>
+      <c r="W35" s="150"/>
+      <c r="X35" s="150"/>
     </row>
     <row r="36" spans="1:24" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A36" s="107"/>
@@ -4590,10 +4572,10 @@
       <c r="T37" s="117"/>
       <c r="U37" s="117"/>
       <c r="V37" s="116" t="s">
-        <v>271</v>
+        <v>268</v>
       </c>
       <c r="W37" s="18" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="X37" s="18"/>
     </row>
@@ -4619,14 +4601,12 @@
       <c r="S38" s="116"/>
       <c r="T38" s="116"/>
       <c r="U38" s="116"/>
-      <c r="V38" s="116" t="s">
-        <v>268</v>
-      </c>
+      <c r="V38" s="116"/>
       <c r="W38" s="18" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="X38" s="18" t="s">
-        <v>269</v>
+        <v>266</v>
       </c>
     </row>
     <row r="39" spans="1:24" ht="15.75" x14ac:dyDescent="0.25">
@@ -4652,13 +4632,13 @@
       <c r="T39" s="116"/>
       <c r="U39" s="116"/>
       <c r="V39" s="116" t="s">
-        <v>272</v>
+        <v>269</v>
       </c>
       <c r="W39" s="18" t="s">
+        <v>270</v>
+      </c>
+      <c r="X39" s="18" t="s">
         <v>267</v>
-      </c>
-      <c r="X39" s="18" t="s">
-        <v>270</v>
       </c>
     </row>
     <row r="40" spans="1:24" ht="15.75" x14ac:dyDescent="0.25">
@@ -5840,12 +5820,6 @@
     <row r="287" hidden="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="20">
-    <mergeCell ref="P1:P2"/>
-    <mergeCell ref="U1:U2"/>
-    <mergeCell ref="T1:T2"/>
-    <mergeCell ref="S1:S2"/>
-    <mergeCell ref="R1:R2"/>
-    <mergeCell ref="Q1:Q2"/>
     <mergeCell ref="I1:I2"/>
     <mergeCell ref="H1:H2"/>
     <mergeCell ref="O1:O2"/>
@@ -5860,6 +5834,12 @@
     <mergeCell ref="D1:D2"/>
     <mergeCell ref="C1:C2"/>
     <mergeCell ref="F1:F2"/>
+    <mergeCell ref="P1:P2"/>
+    <mergeCell ref="U1:U2"/>
+    <mergeCell ref="T1:T2"/>
+    <mergeCell ref="S1:S2"/>
+    <mergeCell ref="R1:R2"/>
+    <mergeCell ref="Q1:Q2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Solicitudes gráficas de recursos
</commit_message>
<xml_diff>
--- a/fuentes/contenidos/grado08/guion08/ESCALETA_MA_08_08_CO.xlsx
+++ b/fuentes/contenidos/grado08/guion08/ESCALETA_MA_08_08_CO.xlsx
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="693" uniqueCount="274">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="694" uniqueCount="275">
   <si>
     <t>Asignatura</t>
   </si>
@@ -983,6 +983,9 @@
   </si>
   <si>
     <t>Autora construyo mal</t>
+  </si>
+  <si>
+    <t>El offline esta en la carpeta de github, falta solicitud gráfica y mejorar presentación</t>
   </si>
 </sst>
 </file>
@@ -1163,7 +1166,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="15">
+  <borders count="16">
     <border>
       <left/>
       <right/>
@@ -1363,11 +1366,22 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="190">
+  <cellXfs count="193">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
@@ -1492,21 +1506,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="15" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="15" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="15" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="15" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="15" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="15" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1734,99 +1733,6 @@
     <xf numFmtId="14" fontId="0" fillId="16" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="17" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="17" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="18" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="18" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="16" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="16" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="12" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="10" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="9" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="11" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="12" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="20" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -1858,6 +1764,121 @@
     <xf numFmtId="0" fontId="0" fillId="20" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="20" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="20" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="12" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="12" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="17" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="17" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="18" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="18" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="16" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="16" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="10" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="11" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="20" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="20" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="20" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="20" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="20" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="20" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="20" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2164,9 +2185,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Y287"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="K1" zoomScale="70" zoomScaleNormal="70" zoomScalePageLayoutView="91" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="T1" zoomScale="70" zoomScaleNormal="70" zoomScalePageLayoutView="91" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="Y17" sqref="Y17"/>
+      <selection pane="bottomLeft" activeCell="AB16" sqref="AB16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2198,375 +2219,375 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:25" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="164" t="s">
+      <c r="A1" s="160" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="162" t="s">
+      <c r="B1" s="158" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="175" t="s">
+      <c r="C1" s="171" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="164" t="s">
+      <c r="D1" s="160" t="s">
         <v>110</v>
       </c>
-      <c r="E1" s="162" t="s">
+      <c r="E1" s="158" t="s">
         <v>111</v>
       </c>
-      <c r="F1" s="160" t="s">
+      <c r="F1" s="154" t="s">
         <v>112</v>
       </c>
-      <c r="G1" s="173" t="s">
+      <c r="G1" s="169" t="s">
         <v>3</v>
       </c>
-      <c r="H1" s="160" t="s">
+      <c r="H1" s="154" t="s">
         <v>113</v>
       </c>
-      <c r="I1" s="160" t="s">
+      <c r="I1" s="154" t="s">
         <v>107</v>
       </c>
-      <c r="J1" s="170" t="s">
+      <c r="J1" s="166" t="s">
         <v>4</v>
       </c>
-      <c r="K1" s="168" t="s">
+      <c r="K1" s="164" t="s">
         <v>108</v>
       </c>
-      <c r="L1" s="166" t="s">
+      <c r="L1" s="162" t="s">
         <v>14</v>
       </c>
-      <c r="M1" s="172" t="s">
+      <c r="M1" s="168" t="s">
         <v>21</v>
       </c>
-      <c r="N1" s="172"/>
-      <c r="O1" s="152" t="s">
+      <c r="N1" s="168"/>
+      <c r="O1" s="156" t="s">
         <v>109</v>
       </c>
-      <c r="P1" s="152" t="s">
+      <c r="P1" s="156" t="s">
         <v>114</v>
       </c>
-      <c r="Q1" s="154" t="s">
+      <c r="Q1" s="179" t="s">
         <v>85</v>
       </c>
-      <c r="R1" s="158" t="s">
+      <c r="R1" s="183" t="s">
         <v>86</v>
       </c>
-      <c r="S1" s="154" t="s">
+      <c r="S1" s="179" t="s">
         <v>87</v>
       </c>
-      <c r="T1" s="156" t="s">
+      <c r="T1" s="181" t="s">
         <v>88</v>
       </c>
-      <c r="U1" s="154" t="s">
+      <c r="U1" s="179" t="s">
         <v>89</v>
       </c>
-      <c r="V1" s="146" t="s">
+      <c r="V1" s="173" t="s">
         <v>251</v>
       </c>
-      <c r="W1" s="148" t="s">
+      <c r="W1" s="175" t="s">
         <v>255</v>
       </c>
-      <c r="X1" s="150" t="s">
+      <c r="X1" s="177" t="s">
         <v>256</v>
       </c>
     </row>
     <row r="2" spans="1:25" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="165"/>
-      <c r="B2" s="163"/>
-      <c r="C2" s="176"/>
-      <c r="D2" s="165"/>
-      <c r="E2" s="163"/>
-      <c r="F2" s="161"/>
-      <c r="G2" s="174"/>
-      <c r="H2" s="161"/>
-      <c r="I2" s="161"/>
-      <c r="J2" s="171"/>
-      <c r="K2" s="169"/>
-      <c r="L2" s="167"/>
+      <c r="A2" s="161"/>
+      <c r="B2" s="159"/>
+      <c r="C2" s="172"/>
+      <c r="D2" s="161"/>
+      <c r="E2" s="159"/>
+      <c r="F2" s="155"/>
+      <c r="G2" s="170"/>
+      <c r="H2" s="155"/>
+      <c r="I2" s="155"/>
+      <c r="J2" s="167"/>
+      <c r="K2" s="165"/>
+      <c r="L2" s="163"/>
       <c r="M2" s="5" t="s">
         <v>90</v>
       </c>
       <c r="N2" s="5" t="s">
         <v>91</v>
       </c>
-      <c r="O2" s="153"/>
-      <c r="P2" s="153"/>
-      <c r="Q2" s="155"/>
-      <c r="R2" s="159"/>
-      <c r="S2" s="155"/>
-      <c r="T2" s="157"/>
-      <c r="U2" s="155"/>
-      <c r="V2" s="147"/>
-      <c r="W2" s="149"/>
-      <c r="X2" s="151"/>
+      <c r="O2" s="157"/>
+      <c r="P2" s="157"/>
+      <c r="Q2" s="180"/>
+      <c r="R2" s="184"/>
+      <c r="S2" s="180"/>
+      <c r="T2" s="182"/>
+      <c r="U2" s="180"/>
+      <c r="V2" s="174"/>
+      <c r="W2" s="176"/>
+      <c r="X2" s="178"/>
     </row>
     <row r="3" spans="1:25" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="76" t="s">
+      <c r="A3" s="71" t="s">
         <v>15</v>
       </c>
-      <c r="B3" s="77" t="s">
+      <c r="B3" s="72" t="s">
         <v>124</v>
       </c>
-      <c r="C3" s="77" t="s">
+      <c r="C3" s="72" t="s">
         <v>123</v>
       </c>
-      <c r="D3" s="77" t="s">
+      <c r="D3" s="72" t="s">
         <v>125</v>
       </c>
-      <c r="E3" s="77"/>
-      <c r="F3" s="77"/>
-      <c r="G3" s="122" t="s">
+      <c r="E3" s="72"/>
+      <c r="F3" s="72"/>
+      <c r="G3" s="117" t="s">
         <v>125</v>
       </c>
-      <c r="H3" s="123">
+      <c r="H3" s="118">
         <v>1</v>
       </c>
-      <c r="I3" s="123" t="s">
+      <c r="I3" s="118" t="s">
         <v>19</v>
       </c>
-      <c r="J3" s="124" t="s">
+      <c r="J3" s="119" t="s">
         <v>225</v>
       </c>
-      <c r="K3" s="123" t="s">
+      <c r="K3" s="118" t="s">
         <v>20</v>
       </c>
-      <c r="L3" s="123" t="s">
+      <c r="L3" s="118" t="s">
         <v>5</v>
       </c>
-      <c r="M3" s="123" t="s">
+      <c r="M3" s="118" t="s">
         <v>60</v>
       </c>
-      <c r="N3" s="123"/>
-      <c r="O3" s="124" t="s">
+      <c r="N3" s="118"/>
+      <c r="O3" s="119" t="s">
         <v>234</v>
       </c>
-      <c r="P3" s="125" t="s">
+      <c r="P3" s="120" t="s">
         <v>19</v>
       </c>
-      <c r="Q3" s="126">
+      <c r="Q3" s="121">
         <v>6</v>
       </c>
-      <c r="R3" s="126" t="s">
+      <c r="R3" s="121" t="s">
         <v>188</v>
       </c>
-      <c r="S3" s="126" t="s">
+      <c r="S3" s="121" t="s">
         <v>189</v>
       </c>
-      <c r="T3" s="127" t="s">
+      <c r="T3" s="122" t="s">
         <v>190</v>
       </c>
-      <c r="U3" s="128" t="s">
+      <c r="U3" s="123" t="s">
         <v>191</v>
       </c>
-      <c r="V3" s="106" t="s">
+      <c r="V3" s="101" t="s">
         <v>250</v>
       </c>
       <c r="W3" s="3"/>
-      <c r="X3" s="115">
+      <c r="X3" s="110">
         <v>42411</v>
       </c>
     </row>
     <row r="4" spans="1:25" ht="18.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="78" t="s">
+      <c r="A4" s="73" t="s">
         <v>15</v>
       </c>
-      <c r="B4" s="79" t="s">
+      <c r="B4" s="74" t="s">
         <v>124</v>
       </c>
-      <c r="C4" s="79" t="s">
+      <c r="C4" s="74" t="s">
         <v>123</v>
       </c>
-      <c r="D4" s="77" t="s">
+      <c r="D4" s="72" t="s">
         <v>125</v>
       </c>
       <c r="E4" s="8"/>
       <c r="F4" s="8"/>
-      <c r="G4" s="133" t="s">
+      <c r="G4" s="128" t="s">
         <v>126</v>
       </c>
-      <c r="H4" s="118">
+      <c r="H4" s="113">
         <v>2</v>
       </c>
-      <c r="I4" s="117" t="s">
+      <c r="I4" s="112" t="s">
         <v>20</v>
       </c>
-      <c r="J4" s="134" t="s">
+      <c r="J4" s="129" t="s">
         <v>131</v>
       </c>
-      <c r="K4" s="117" t="s">
+      <c r="K4" s="112" t="s">
         <v>20</v>
       </c>
-      <c r="L4" s="117" t="s">
+      <c r="L4" s="112" t="s">
         <v>8</v>
       </c>
-      <c r="M4" s="117"/>
-      <c r="N4" s="117" t="s">
+      <c r="M4" s="112"/>
+      <c r="N4" s="112" t="s">
         <v>40</v>
       </c>
-      <c r="O4" s="135" t="s">
+      <c r="O4" s="130" t="s">
         <v>127</v>
       </c>
-      <c r="P4" s="118" t="s">
+      <c r="P4" s="113" t="s">
         <v>19</v>
       </c>
-      <c r="Q4" s="119">
+      <c r="Q4" s="114">
         <v>6</v>
       </c>
-      <c r="R4" s="119" t="s">
+      <c r="R4" s="114" t="s">
         <v>192</v>
       </c>
-      <c r="S4" s="119" t="s">
+      <c r="S4" s="114" t="s">
         <v>193</v>
       </c>
-      <c r="T4" s="120" t="s">
+      <c r="T4" s="115" t="s">
         <v>194</v>
       </c>
-      <c r="U4" s="121" t="s">
+      <c r="U4" s="116" t="s">
         <v>195</v>
       </c>
-      <c r="V4" s="106" t="s">
+      <c r="V4" s="101" t="s">
         <v>247</v>
       </c>
-      <c r="W4" s="114">
+      <c r="W4" s="109">
         <v>42417</v>
       </c>
-      <c r="X4" s="115">
+      <c r="X4" s="110">
         <v>42417</v>
       </c>
     </row>
     <row r="5" spans="1:25" ht="18.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="82" t="s">
+      <c r="A5" s="77" t="s">
         <v>15</v>
       </c>
-      <c r="B5" s="64" t="s">
+      <c r="B5" s="59" t="s">
         <v>124</v>
       </c>
-      <c r="C5" s="64" t="s">
+      <c r="C5" s="59" t="s">
         <v>123</v>
       </c>
-      <c r="D5" s="83" t="s">
+      <c r="D5" s="78" t="s">
         <v>125</v>
       </c>
       <c r="E5" s="18"/>
       <c r="F5" s="18"/>
-      <c r="G5" s="116" t="s">
+      <c r="G5" s="111" t="s">
         <v>128</v>
       </c>
-      <c r="H5" s="117">
+      <c r="H5" s="112">
         <v>3</v>
       </c>
-      <c r="I5" s="117" t="s">
+      <c r="I5" s="112" t="s">
         <v>19</v>
       </c>
-      <c r="J5" s="90" t="s">
+      <c r="J5" s="85" t="s">
         <v>226</v>
       </c>
-      <c r="K5" s="117" t="s">
+      <c r="K5" s="112" t="s">
         <v>20</v>
       </c>
-      <c r="L5" s="117" t="s">
+      <c r="L5" s="112" t="s">
         <v>5</v>
       </c>
-      <c r="M5" s="117" t="s">
+      <c r="M5" s="112" t="s">
         <v>53</v>
       </c>
-      <c r="N5" s="117"/>
-      <c r="O5" s="129" t="s">
+      <c r="N5" s="112"/>
+      <c r="O5" s="124" t="s">
         <v>129</v>
       </c>
-      <c r="P5" s="118" t="s">
+      <c r="P5" s="113" t="s">
         <v>20</v>
       </c>
-      <c r="Q5" s="119">
+      <c r="Q5" s="114">
         <v>6</v>
       </c>
-      <c r="R5" s="119" t="s">
+      <c r="R5" s="114" t="s">
         <v>188</v>
       </c>
-      <c r="S5" s="119" t="s">
+      <c r="S5" s="114" t="s">
         <v>189</v>
       </c>
-      <c r="T5" s="120" t="s">
+      <c r="T5" s="115" t="s">
         <v>196</v>
       </c>
-      <c r="U5" s="121" t="s">
+      <c r="U5" s="116" t="s">
         <v>191</v>
       </c>
-      <c r="V5" s="106" t="s">
+      <c r="V5" s="101" t="s">
         <v>253</v>
       </c>
       <c r="W5" s="3"/>
-      <c r="X5" s="115">
+      <c r="X5" s="110">
         <v>42412</v>
       </c>
-      <c r="Y5" s="72" t="s">
+      <c r="Y5" s="67" t="s">
         <v>263</v>
       </c>
     </row>
     <row r="6" spans="1:25" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="80" t="s">
+      <c r="A6" s="75" t="s">
         <v>15</v>
       </c>
-      <c r="B6" s="81" t="s">
+      <c r="B6" s="76" t="s">
         <v>124</v>
       </c>
-      <c r="C6" s="81" t="s">
+      <c r="C6" s="76" t="s">
         <v>123</v>
       </c>
-      <c r="D6" s="77" t="s">
+      <c r="D6" s="72" t="s">
         <v>125</v>
       </c>
       <c r="E6" s="10" t="s">
         <v>122</v>
       </c>
       <c r="F6" s="10"/>
-      <c r="G6" s="136" t="s">
+      <c r="G6" s="131" t="s">
         <v>236</v>
       </c>
-      <c r="H6" s="137">
+      <c r="H6" s="132">
         <v>4</v>
       </c>
-      <c r="I6" s="138" t="s">
+      <c r="I6" s="133" t="s">
         <v>20</v>
       </c>
-      <c r="J6" s="139" t="s">
+      <c r="J6" s="134" t="s">
         <v>130</v>
       </c>
-      <c r="K6" s="138" t="s">
+      <c r="K6" s="133" t="s">
         <v>20</v>
       </c>
-      <c r="L6" s="138" t="s">
+      <c r="L6" s="133" t="s">
         <v>8</v>
       </c>
-      <c r="M6" s="138"/>
-      <c r="N6" s="138" t="s">
+      <c r="M6" s="133"/>
+      <c r="N6" s="133" t="s">
         <v>121</v>
       </c>
-      <c r="O6" s="139"/>
-      <c r="P6" s="137" t="s">
+      <c r="O6" s="134"/>
+      <c r="P6" s="132" t="s">
         <v>19</v>
       </c>
-      <c r="Q6" s="140">
+      <c r="Q6" s="135">
         <v>6</v>
       </c>
-      <c r="R6" s="140" t="s">
+      <c r="R6" s="135" t="s">
         <v>192</v>
       </c>
-      <c r="S6" s="140" t="s">
+      <c r="S6" s="135" t="s">
         <v>193</v>
       </c>
-      <c r="T6" s="141" t="s">
+      <c r="T6" s="136" t="s">
         <v>197</v>
       </c>
-      <c r="U6" s="142" t="s">
+      <c r="U6" s="137" t="s">
         <v>195</v>
       </c>
-      <c r="V6" s="106" t="s">
+      <c r="V6" s="101" t="s">
         <v>248</v>
       </c>
-      <c r="W6" s="94">
+      <c r="W6" s="89">
         <v>42422</v>
       </c>
-      <c r="X6" s="115">
+      <c r="X6" s="110">
         <v>42422</v>
       </c>
     </row>
@@ -2585,56 +2606,56 @@
       </c>
       <c r="E7" s="33"/>
       <c r="F7" s="33"/>
-      <c r="G7" s="130" t="s">
+      <c r="G7" s="125" t="s">
         <v>132</v>
       </c>
-      <c r="H7" s="123">
+      <c r="H7" s="118">
         <v>5</v>
       </c>
-      <c r="I7" s="123" t="s">
+      <c r="I7" s="118" t="s">
         <v>19</v>
       </c>
-      <c r="J7" s="131" t="s">
+      <c r="J7" s="126" t="s">
         <v>237</v>
       </c>
-      <c r="K7" s="123" t="s">
+      <c r="K7" s="118" t="s">
         <v>20</v>
       </c>
-      <c r="L7" s="123" t="s">
+      <c r="L7" s="118" t="s">
         <v>5</v>
       </c>
-      <c r="M7" s="123" t="s">
+      <c r="M7" s="118" t="s">
         <v>57</v>
       </c>
-      <c r="N7" s="123"/>
-      <c r="O7" s="124" t="s">
+      <c r="N7" s="118"/>
+      <c r="O7" s="119" t="s">
         <v>235</v>
       </c>
-      <c r="P7" s="125" t="s">
+      <c r="P7" s="120" t="s">
         <v>19</v>
       </c>
-      <c r="Q7" s="126">
+      <c r="Q7" s="121">
         <v>6</v>
       </c>
-      <c r="R7" s="126" t="s">
+      <c r="R7" s="121" t="s">
         <v>188</v>
       </c>
-      <c r="S7" s="126" t="s">
+      <c r="S7" s="121" t="s">
         <v>189</v>
       </c>
-      <c r="T7" s="127" t="s">
+      <c r="T7" s="122" t="s">
         <v>198</v>
       </c>
-      <c r="U7" s="128" t="s">
+      <c r="U7" s="123" t="s">
         <v>191</v>
       </c>
-      <c r="V7" s="106" t="s">
+      <c r="V7" s="101" t="s">
         <v>252</v>
       </c>
-      <c r="W7" s="114">
+      <c r="W7" s="109">
         <v>42412</v>
       </c>
-      <c r="X7" s="115">
+      <c r="X7" s="110">
         <v>42047</v>
       </c>
     </row>
@@ -2653,121 +2674,121 @@
       </c>
       <c r="E8" s="19"/>
       <c r="F8" s="19"/>
-      <c r="G8" s="101" t="s">
+      <c r="G8" s="96" t="s">
         <v>133</v>
       </c>
-      <c r="H8" s="102">
+      <c r="H8" s="97">
         <v>6</v>
       </c>
-      <c r="I8" s="103" t="s">
+      <c r="I8" s="98" t="s">
         <v>20</v>
       </c>
-      <c r="J8" s="89" t="s">
+      <c r="J8" s="84" t="s">
         <v>134</v>
       </c>
-      <c r="K8" s="103" t="s">
+      <c r="K8" s="98" t="s">
         <v>20</v>
       </c>
-      <c r="L8" s="103" t="s">
+      <c r="L8" s="98" t="s">
         <v>8</v>
       </c>
-      <c r="M8" s="103"/>
-      <c r="N8" s="103" t="s">
+      <c r="M8" s="98"/>
+      <c r="N8" s="98" t="s">
         <v>40</v>
       </c>
-      <c r="O8" s="89" t="s">
+      <c r="O8" s="84" t="s">
         <v>135</v>
       </c>
-      <c r="P8" s="102" t="s">
+      <c r="P8" s="97" t="s">
         <v>19</v>
       </c>
-      <c r="Q8" s="104">
+      <c r="Q8" s="99">
         <v>6</v>
       </c>
-      <c r="R8" s="104" t="s">
+      <c r="R8" s="99" t="s">
         <v>192</v>
       </c>
-      <c r="S8" s="104" t="s">
+      <c r="S8" s="99" t="s">
         <v>193</v>
       </c>
-      <c r="T8" s="113" t="s">
+      <c r="T8" s="108" t="s">
         <v>199</v>
       </c>
-      <c r="U8" s="105" t="s">
+      <c r="U8" s="100" t="s">
         <v>195</v>
       </c>
-      <c r="V8" s="106" t="s">
+      <c r="V8" s="101" t="s">
         <v>247</v>
       </c>
-      <c r="W8" s="114">
+      <c r="W8" s="109">
         <v>42418</v>
       </c>
-      <c r="X8" s="94">
+      <c r="X8" s="89">
         <v>42418</v>
       </c>
     </row>
     <row r="9" spans="1:25" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="82" t="s">
+      <c r="A9" s="77" t="s">
         <v>15</v>
       </c>
-      <c r="B9" s="64" t="s">
+      <c r="B9" s="59" t="s">
         <v>124</v>
       </c>
-      <c r="C9" s="64" t="s">
+      <c r="C9" s="59" t="s">
         <v>123</v>
       </c>
-      <c r="D9" s="83" t="s">
+      <c r="D9" s="78" t="s">
         <v>132</v>
       </c>
       <c r="E9" s="18"/>
       <c r="F9" s="18"/>
-      <c r="G9" s="101" t="s">
+      <c r="G9" s="96" t="s">
         <v>223</v>
       </c>
-      <c r="H9" s="103">
+      <c r="H9" s="98">
         <v>7</v>
       </c>
-      <c r="I9" s="103" t="s">
+      <c r="I9" s="98" t="s">
         <v>20</v>
       </c>
-      <c r="J9" s="89" t="s">
+      <c r="J9" s="84" t="s">
         <v>227</v>
       </c>
-      <c r="K9" s="103" t="s">
+      <c r="K9" s="98" t="s">
         <v>20</v>
       </c>
-      <c r="L9" s="103" t="s">
+      <c r="L9" s="98" t="s">
         <v>8</v>
       </c>
-      <c r="M9" s="103"/>
-      <c r="N9" s="103" t="s">
+      <c r="M9" s="98"/>
+      <c r="N9" s="98" t="s">
         <v>32</v>
       </c>
-      <c r="O9" s="89" t="s">
+      <c r="O9" s="84" t="s">
         <v>136</v>
       </c>
-      <c r="P9" s="102" t="s">
+      <c r="P9" s="97" t="s">
         <v>20</v>
       </c>
-      <c r="Q9" s="104">
+      <c r="Q9" s="99">
         <v>6</v>
       </c>
-      <c r="R9" s="104" t="s">
+      <c r="R9" s="99" t="s">
         <v>192</v>
       </c>
-      <c r="S9" s="104" t="s">
+      <c r="S9" s="99" t="s">
         <v>193</v>
       </c>
-      <c r="T9" s="113" t="s">
+      <c r="T9" s="108" t="s">
         <v>200</v>
       </c>
-      <c r="U9" s="105" t="s">
+      <c r="U9" s="100" t="s">
         <v>195</v>
       </c>
-      <c r="V9" s="106" t="s">
+      <c r="V9" s="101" t="s">
         <v>250</v>
       </c>
-      <c r="W9" s="114">
+      <c r="W9" s="109">
         <v>42408</v>
       </c>
       <c r="X9" s="3" t="s">
@@ -2775,70 +2796,70 @@
       </c>
     </row>
     <row r="10" spans="1:25" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="82" t="s">
+      <c r="A10" s="77" t="s">
         <v>15</v>
       </c>
-      <c r="B10" s="64" t="s">
+      <c r="B10" s="59" t="s">
         <v>124</v>
       </c>
-      <c r="C10" s="64" t="s">
+      <c r="C10" s="59" t="s">
         <v>123</v>
       </c>
-      <c r="D10" s="83" t="s">
+      <c r="D10" s="78" t="s">
         <v>132</v>
       </c>
       <c r="E10" s="18"/>
       <c r="F10" s="18"/>
-      <c r="G10" s="116" t="s">
+      <c r="G10" s="111" t="s">
         <v>222</v>
       </c>
-      <c r="H10" s="118">
+      <c r="H10" s="113">
         <v>8</v>
       </c>
-      <c r="I10" s="117" t="s">
+      <c r="I10" s="112" t="s">
         <v>20</v>
       </c>
-      <c r="J10" s="90" t="s">
+      <c r="J10" s="85" t="s">
         <v>228</v>
       </c>
-      <c r="K10" s="117" t="s">
+      <c r="K10" s="112" t="s">
         <v>20</v>
       </c>
-      <c r="L10" s="117" t="s">
+      <c r="L10" s="112" t="s">
         <v>8</v>
       </c>
-      <c r="M10" s="117"/>
-      <c r="N10" s="117" t="s">
+      <c r="M10" s="112"/>
+      <c r="N10" s="112" t="s">
         <v>33</v>
       </c>
-      <c r="O10" s="90" t="s">
+      <c r="O10" s="85" t="s">
         <v>137</v>
       </c>
-      <c r="P10" s="118" t="s">
+      <c r="P10" s="113" t="s">
         <v>20</v>
       </c>
-      <c r="Q10" s="119">
+      <c r="Q10" s="114">
         <v>6</v>
       </c>
-      <c r="R10" s="119" t="s">
+      <c r="R10" s="114" t="s">
         <v>192</v>
       </c>
-      <c r="S10" s="119" t="s">
+      <c r="S10" s="114" t="s">
         <v>193</v>
       </c>
-      <c r="T10" s="120" t="s">
+      <c r="T10" s="115" t="s">
         <v>201</v>
       </c>
-      <c r="U10" s="121" t="s">
+      <c r="U10" s="116" t="s">
         <v>195</v>
       </c>
-      <c r="V10" s="106" t="s">
+      <c r="V10" s="101" t="s">
         <v>247</v>
       </c>
-      <c r="W10" s="114">
+      <c r="W10" s="109">
         <v>42419</v>
       </c>
-      <c r="X10" s="115">
+      <c r="X10" s="110">
         <v>42419</v>
       </c>
     </row>
@@ -2857,53 +2878,53 @@
       </c>
       <c r="E11" s="19"/>
       <c r="F11" s="19"/>
-      <c r="G11" s="101" t="s">
+      <c r="G11" s="96" t="s">
         <v>138</v>
       </c>
-      <c r="H11" s="103">
+      <c r="H11" s="98">
         <v>9</v>
       </c>
-      <c r="I11" s="103" t="s">
+      <c r="I11" s="98" t="s">
         <v>20</v>
       </c>
-      <c r="J11" s="89" t="s">
+      <c r="J11" s="84" t="s">
         <v>139</v>
       </c>
-      <c r="K11" s="103" t="s">
+      <c r="K11" s="98" t="s">
         <v>20</v>
       </c>
-      <c r="L11" s="103" t="s">
+      <c r="L11" s="98" t="s">
         <v>8</v>
       </c>
-      <c r="M11" s="103"/>
-      <c r="N11" s="103" t="s">
+      <c r="M11" s="98"/>
+      <c r="N11" s="98" t="s">
         <v>24</v>
       </c>
-      <c r="O11" s="89" t="s">
+      <c r="O11" s="84" t="s">
         <v>140</v>
       </c>
-      <c r="P11" s="102" t="s">
+      <c r="P11" s="97" t="s">
         <v>19</v>
       </c>
-      <c r="Q11" s="104">
+      <c r="Q11" s="99">
         <v>6</v>
       </c>
-      <c r="R11" s="104" t="s">
+      <c r="R11" s="99" t="s">
         <v>192</v>
       </c>
-      <c r="S11" s="104" t="s">
+      <c r="S11" s="99" t="s">
         <v>193</v>
       </c>
-      <c r="T11" s="113" t="s">
+      <c r="T11" s="108" t="s">
         <v>202</v>
       </c>
-      <c r="U11" s="105" t="s">
+      <c r="U11" s="100" t="s">
         <v>195</v>
       </c>
-      <c r="V11" s="106" t="s">
+      <c r="V11" s="101" t="s">
         <v>250</v>
       </c>
-      <c r="W11" s="114">
+      <c r="W11" s="109">
         <v>42408</v>
       </c>
       <c r="X11" s="3" t="s">
@@ -2927,53 +2948,53 @@
         <v>122</v>
       </c>
       <c r="F12" s="36"/>
-      <c r="G12" s="177" t="s">
+      <c r="G12" s="141" t="s">
         <v>182</v>
       </c>
-      <c r="H12" s="180">
+      <c r="H12" s="144">
         <v>10</v>
       </c>
-      <c r="I12" s="178" t="s">
+      <c r="I12" s="142" t="s">
         <v>20</v>
       </c>
-      <c r="J12" s="179" t="s">
+      <c r="J12" s="143" t="s">
         <v>142</v>
       </c>
-      <c r="K12" s="178" t="s">
+      <c r="K12" s="142" t="s">
         <v>20</v>
       </c>
-      <c r="L12" s="178" t="s">
+      <c r="L12" s="142" t="s">
         <v>8</v>
       </c>
-      <c r="M12" s="178"/>
-      <c r="N12" s="178" t="s">
+      <c r="M12" s="142"/>
+      <c r="N12" s="142" t="s">
         <v>121</v>
       </c>
-      <c r="O12" s="179"/>
-      <c r="P12" s="180" t="s">
+      <c r="O12" s="143"/>
+      <c r="P12" s="144" t="s">
         <v>19</v>
       </c>
-      <c r="Q12" s="181">
+      <c r="Q12" s="145">
         <v>6</v>
       </c>
-      <c r="R12" s="181" t="s">
+      <c r="R12" s="145" t="s">
         <v>192</v>
       </c>
-      <c r="S12" s="181" t="s">
+      <c r="S12" s="145" t="s">
         <v>193</v>
       </c>
-      <c r="T12" s="182" t="s">
+      <c r="T12" s="146" t="s">
         <v>203</v>
       </c>
-      <c r="U12" s="183" t="s">
+      <c r="U12" s="147" t="s">
         <v>195</v>
       </c>
-      <c r="V12" s="187" t="s">
+      <c r="V12" s="151" t="s">
         <v>248</v>
       </c>
-      <c r="W12" s="188"/>
-      <c r="X12" s="188"/>
-      <c r="Y12" s="189" t="s">
+      <c r="W12" s="152"/>
+      <c r="X12" s="152"/>
+      <c r="Y12" s="153" t="s">
         <v>273</v>
       </c>
     </row>
@@ -2992,56 +3013,56 @@
       </c>
       <c r="E13" s="25"/>
       <c r="F13" s="25"/>
-      <c r="G13" s="130" t="s">
+      <c r="G13" s="125" t="s">
         <v>232</v>
       </c>
-      <c r="H13" s="123">
+      <c r="H13" s="118">
         <v>11</v>
       </c>
-      <c r="I13" s="123" t="s">
+      <c r="I13" s="118" t="s">
         <v>19</v>
       </c>
-      <c r="J13" s="132" t="s">
+      <c r="J13" s="127" t="s">
         <v>238</v>
       </c>
-      <c r="K13" s="123" t="s">
+      <c r="K13" s="118" t="s">
         <v>20</v>
       </c>
-      <c r="L13" s="123" t="s">
+      <c r="L13" s="118" t="s">
         <v>5</v>
       </c>
-      <c r="M13" s="123" t="s">
+      <c r="M13" s="118" t="s">
         <v>54</v>
       </c>
-      <c r="N13" s="123"/>
-      <c r="O13" s="132" t="s">
+      <c r="N13" s="118"/>
+      <c r="O13" s="127" t="s">
         <v>239</v>
       </c>
-      <c r="P13" s="125" t="s">
+      <c r="P13" s="120" t="s">
         <v>19</v>
       </c>
-      <c r="Q13" s="126">
+      <c r="Q13" s="121">
         <v>6</v>
       </c>
-      <c r="R13" s="126" t="s">
+      <c r="R13" s="121" t="s">
         <v>188</v>
       </c>
-      <c r="S13" s="126" t="s">
+      <c r="S13" s="121" t="s">
         <v>189</v>
       </c>
-      <c r="T13" s="127" t="s">
+      <c r="T13" s="122" t="s">
         <v>204</v>
       </c>
-      <c r="U13" s="128" t="s">
+      <c r="U13" s="123" t="s">
         <v>191</v>
       </c>
-      <c r="V13" s="106" t="s">
+      <c r="V13" s="101" t="s">
         <v>252</v>
       </c>
-      <c r="W13" s="114">
+      <c r="W13" s="109">
         <v>42412</v>
       </c>
-      <c r="X13" s="115">
+      <c r="X13" s="110">
         <v>42412</v>
       </c>
     </row>
@@ -3060,53 +3081,53 @@
       </c>
       <c r="E14" s="28"/>
       <c r="F14" s="28"/>
-      <c r="G14" s="101" t="s">
+      <c r="G14" s="96" t="s">
         <v>144</v>
       </c>
-      <c r="H14" s="103">
+      <c r="H14" s="98">
         <v>12</v>
       </c>
-      <c r="I14" s="103" t="s">
+      <c r="I14" s="98" t="s">
         <v>20</v>
       </c>
-      <c r="J14" s="89" t="s">
+      <c r="J14" s="84" t="s">
         <v>145</v>
       </c>
-      <c r="K14" s="103" t="s">
+      <c r="K14" s="98" t="s">
         <v>20</v>
       </c>
-      <c r="L14" s="103" t="s">
+      <c r="L14" s="98" t="s">
         <v>8</v>
       </c>
-      <c r="M14" s="103"/>
-      <c r="N14" s="103" t="s">
+      <c r="M14" s="98"/>
+      <c r="N14" s="98" t="s">
         <v>27</v>
       </c>
-      <c r="O14" s="89" t="s">
+      <c r="O14" s="84" t="s">
         <v>146</v>
       </c>
-      <c r="P14" s="102" t="s">
+      <c r="P14" s="97" t="s">
         <v>19</v>
       </c>
-      <c r="Q14" s="104">
+      <c r="Q14" s="99">
         <v>6</v>
       </c>
-      <c r="R14" s="104" t="s">
+      <c r="R14" s="99" t="s">
         <v>192</v>
       </c>
-      <c r="S14" s="104" t="s">
+      <c r="S14" s="99" t="s">
         <v>193</v>
       </c>
-      <c r="T14" s="113" t="s">
+      <c r="T14" s="108" t="s">
         <v>205</v>
       </c>
-      <c r="U14" s="105" t="s">
+      <c r="U14" s="100" t="s">
         <v>195</v>
       </c>
-      <c r="V14" s="106" t="s">
+      <c r="V14" s="101" t="s">
         <v>250</v>
       </c>
-      <c r="W14" s="114">
+      <c r="W14" s="109">
         <v>42414</v>
       </c>
       <c r="X14" s="3" t="s">
@@ -3128,122 +3149,122 @@
       </c>
       <c r="E15" s="28"/>
       <c r="F15" s="28"/>
-      <c r="G15" s="116" t="s">
+      <c r="G15" s="111" t="s">
         <v>141</v>
       </c>
-      <c r="H15" s="118">
+      <c r="H15" s="113">
         <v>13</v>
       </c>
-      <c r="I15" s="117" t="s">
+      <c r="I15" s="112" t="s">
         <v>20</v>
       </c>
-      <c r="J15" s="90" t="s">
+      <c r="J15" s="85" t="s">
         <v>229</v>
       </c>
-      <c r="K15" s="117" t="s">
+      <c r="K15" s="112" t="s">
         <v>20</v>
       </c>
-      <c r="L15" s="117" t="s">
+      <c r="L15" s="112" t="s">
         <v>8</v>
       </c>
-      <c r="M15" s="117"/>
-      <c r="N15" s="117" t="s">
+      <c r="M15" s="112"/>
+      <c r="N15" s="112" t="s">
         <v>48</v>
       </c>
-      <c r="O15" s="90" t="s">
+      <c r="O15" s="85" t="s">
         <v>143</v>
       </c>
-      <c r="P15" s="118" t="s">
+      <c r="P15" s="113" t="s">
         <v>19</v>
       </c>
-      <c r="Q15" s="119">
+      <c r="Q15" s="114">
         <v>6</v>
       </c>
-      <c r="R15" s="119" t="s">
+      <c r="R15" s="114" t="s">
         <v>192</v>
       </c>
-      <c r="S15" s="119" t="s">
+      <c r="S15" s="114" t="s">
         <v>193</v>
       </c>
-      <c r="T15" s="120" t="s">
+      <c r="T15" s="115" t="s">
         <v>206</v>
       </c>
-      <c r="U15" s="121" t="s">
+      <c r="U15" s="116" t="s">
         <v>195</v>
       </c>
-      <c r="V15" s="106" t="s">
+      <c r="V15" s="101" t="s">
         <v>250</v>
       </c>
-      <c r="W15" s="114">
+      <c r="W15" s="109">
         <v>42414</v>
       </c>
-      <c r="X15" s="115">
+      <c r="X15" s="110">
         <v>42414</v>
       </c>
     </row>
     <row r="16" spans="1:25" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="82" t="s">
+      <c r="A16" s="77" t="s">
         <v>15</v>
       </c>
-      <c r="B16" s="64" t="s">
+      <c r="B16" s="59" t="s">
         <v>124</v>
       </c>
-      <c r="C16" s="64" t="s">
+      <c r="C16" s="59" t="s">
         <v>123</v>
       </c>
-      <c r="D16" s="83" t="s">
+      <c r="D16" s="78" t="s">
         <v>232</v>
       </c>
       <c r="E16" s="18"/>
       <c r="F16" s="18"/>
-      <c r="G16" s="116" t="s">
+      <c r="G16" s="111" t="s">
         <v>147</v>
       </c>
-      <c r="H16" s="117">
+      <c r="H16" s="112">
         <v>14</v>
       </c>
-      <c r="I16" s="117" t="s">
+      <c r="I16" s="112" t="s">
         <v>20</v>
       </c>
-      <c r="J16" s="90" t="s">
+      <c r="J16" s="85" t="s">
         <v>148</v>
       </c>
-      <c r="K16" s="117" t="s">
+      <c r="K16" s="112" t="s">
         <v>20</v>
       </c>
-      <c r="L16" s="117" t="s">
+      <c r="L16" s="112" t="s">
         <v>8</v>
       </c>
-      <c r="M16" s="117"/>
-      <c r="N16" s="117" t="s">
+      <c r="M16" s="112"/>
+      <c r="N16" s="112" t="s">
         <v>120</v>
       </c>
-      <c r="O16" s="90" t="s">
+      <c r="O16" s="85" t="s">
         <v>149</v>
       </c>
-      <c r="P16" s="118" t="s">
+      <c r="P16" s="113" t="s">
         <v>20</v>
       </c>
-      <c r="Q16" s="119">
+      <c r="Q16" s="114">
         <v>6</v>
       </c>
-      <c r="R16" s="119" t="s">
+      <c r="R16" s="114" t="s">
         <v>192</v>
       </c>
-      <c r="S16" s="119" t="s">
+      <c r="S16" s="114" t="s">
         <v>193</v>
       </c>
-      <c r="T16" s="120" t="s">
+      <c r="T16" s="115" t="s">
         <v>208</v>
       </c>
-      <c r="U16" s="121" t="s">
+      <c r="U16" s="116" t="s">
         <v>195</v>
       </c>
-      <c r="V16" s="106" t="s">
+      <c r="V16" s="101" t="s">
         <v>249</v>
       </c>
       <c r="W16" s="3"/>
-      <c r="X16" s="115">
+      <c r="X16" s="110">
         <v>42410</v>
       </c>
       <c r="Y16" s="4" t="s">
@@ -3267,180 +3288,180 @@
         <v>122</v>
       </c>
       <c r="F17" s="31"/>
-      <c r="G17" s="177" t="s">
+      <c r="G17" s="141" t="s">
         <v>233</v>
       </c>
-      <c r="H17" s="180">
+      <c r="H17" s="144">
         <v>15</v>
       </c>
-      <c r="I17" s="178" t="s">
+      <c r="I17" s="142" t="s">
         <v>20</v>
       </c>
-      <c r="J17" s="179" t="s">
+      <c r="J17" s="143" t="s">
         <v>240</v>
       </c>
-      <c r="K17" s="178" t="s">
+      <c r="K17" s="142" t="s">
         <v>20</v>
       </c>
-      <c r="L17" s="178" t="s">
+      <c r="L17" s="142" t="s">
         <v>8</v>
       </c>
-      <c r="M17" s="178"/>
-      <c r="N17" s="178" t="s">
+      <c r="M17" s="142"/>
+      <c r="N17" s="142" t="s">
         <v>121</v>
       </c>
-      <c r="O17" s="179" t="s">
+      <c r="O17" s="143" t="s">
         <v>187</v>
       </c>
-      <c r="P17" s="180" t="s">
+      <c r="P17" s="144" t="s">
         <v>19</v>
       </c>
-      <c r="Q17" s="181">
+      <c r="Q17" s="145">
         <v>6</v>
       </c>
-      <c r="R17" s="181" t="s">
+      <c r="R17" s="145" t="s">
         <v>192</v>
       </c>
-      <c r="S17" s="181" t="s">
+      <c r="S17" s="145" t="s">
         <v>193</v>
       </c>
-      <c r="T17" s="182" t="s">
+      <c r="T17" s="146" t="s">
         <v>207</v>
       </c>
-      <c r="U17" s="183" t="s">
+      <c r="U17" s="147" t="s">
         <v>195</v>
       </c>
-      <c r="V17" s="187" t="s">
+      <c r="V17" s="151" t="s">
         <v>248</v>
       </c>
-      <c r="W17" s="188"/>
-      <c r="X17" s="188"/>
-      <c r="Y17" s="189" t="s">
+      <c r="W17" s="152"/>
+      <c r="X17" s="152"/>
+      <c r="Y17" s="153" t="s">
         <v>273</v>
       </c>
     </row>
     <row r="18" spans="1:25" s="11" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A18" s="86" t="s">
+      <c r="A18" s="81" t="s">
         <v>15</v>
       </c>
-      <c r="B18" s="83" t="s">
+      <c r="B18" s="78" t="s">
         <v>124</v>
       </c>
-      <c r="C18" s="83" t="s">
+      <c r="C18" s="78" t="s">
         <v>123</v>
       </c>
-      <c r="D18" s="83" t="s">
+      <c r="D18" s="78" t="s">
         <v>185</v>
       </c>
-      <c r="E18" s="85"/>
-      <c r="F18" s="85"/>
-      <c r="G18" s="95" t="s">
+      <c r="E18" s="80"/>
+      <c r="F18" s="80"/>
+      <c r="G18" s="90" t="s">
         <v>150</v>
       </c>
-      <c r="H18" s="96">
+      <c r="H18" s="91">
         <v>16</v>
       </c>
-      <c r="I18" s="96" t="s">
+      <c r="I18" s="91" t="s">
         <v>19</v>
       </c>
-      <c r="J18" s="97" t="s">
+      <c r="J18" s="92" t="s">
         <v>230</v>
       </c>
-      <c r="K18" s="96" t="s">
+      <c r="K18" s="91" t="s">
         <v>19</v>
       </c>
-      <c r="L18" s="96" t="s">
+      <c r="L18" s="91" t="s">
         <v>5</v>
       </c>
-      <c r="M18" s="96"/>
-      <c r="N18" s="96"/>
-      <c r="O18" s="97"/>
-      <c r="P18" s="98" t="s">
+      <c r="M18" s="91"/>
+      <c r="N18" s="91"/>
+      <c r="O18" s="92"/>
+      <c r="P18" s="93" t="s">
         <v>20</v>
       </c>
-      <c r="Q18" s="99">
+      <c r="Q18" s="94">
         <v>8</v>
       </c>
-      <c r="R18" s="99" t="s">
+      <c r="R18" s="94" t="s">
         <v>217</v>
       </c>
-      <c r="S18" s="99" t="s">
+      <c r="S18" s="94" t="s">
         <v>218</v>
       </c>
-      <c r="T18" s="99" t="s">
+      <c r="T18" s="94" t="s">
         <v>150</v>
       </c>
-      <c r="U18" s="100" t="s">
+      <c r="U18" s="95" t="s">
         <v>219</v>
       </c>
-      <c r="V18" s="106" t="s">
+      <c r="V18" s="101" t="s">
         <v>246</v>
       </c>
-      <c r="W18" s="114">
+      <c r="W18" s="109">
         <v>42403</v>
       </c>
-      <c r="X18" s="93" t="s">
+      <c r="X18" s="88" t="s">
         <v>257</v>
       </c>
     </row>
     <row r="19" spans="1:25" s="11" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A19" s="82" t="s">
+      <c r="A19" s="77" t="s">
         <v>15</v>
       </c>
-      <c r="B19" s="64" t="s">
+      <c r="B19" s="59" t="s">
         <v>124</v>
       </c>
-      <c r="C19" s="64" t="s">
+      <c r="C19" s="59" t="s">
         <v>123</v>
       </c>
-      <c r="D19" s="64" t="s">
+      <c r="D19" s="59" t="s">
         <v>185</v>
       </c>
       <c r="E19" s="18"/>
       <c r="F19" s="18"/>
-      <c r="G19" s="101" t="s">
+      <c r="G19" s="96" t="s">
         <v>224</v>
       </c>
-      <c r="H19" s="102">
+      <c r="H19" s="97">
         <v>17</v>
       </c>
-      <c r="I19" s="103" t="s">
+      <c r="I19" s="98" t="s">
         <v>20</v>
       </c>
-      <c r="J19" s="89" t="s">
+      <c r="J19" s="84" t="s">
         <v>152</v>
       </c>
-      <c r="K19" s="103" t="s">
+      <c r="K19" s="98" t="s">
         <v>19</v>
       </c>
-      <c r="L19" s="103" t="s">
+      <c r="L19" s="98" t="s">
         <v>8</v>
       </c>
-      <c r="M19" s="103"/>
-      <c r="N19" s="103"/>
-      <c r="O19" s="89"/>
-      <c r="P19" s="102" t="s">
+      <c r="M19" s="98"/>
+      <c r="N19" s="98"/>
+      <c r="O19" s="84"/>
+      <c r="P19" s="97" t="s">
         <v>20</v>
       </c>
-      <c r="Q19" s="104">
+      <c r="Q19" s="99">
         <v>8</v>
       </c>
-      <c r="R19" s="104" t="s">
+      <c r="R19" s="99" t="s">
         <v>217</v>
       </c>
-      <c r="S19" s="104" t="s">
+      <c r="S19" s="99" t="s">
         <v>218</v>
       </c>
-      <c r="T19" s="104" t="s">
+      <c r="T19" s="99" t="s">
         <v>151</v>
       </c>
-      <c r="U19" s="105" t="s">
+      <c r="U19" s="100" t="s">
         <v>219</v>
       </c>
-      <c r="V19" s="106" t="s">
+      <c r="V19" s="101" t="s">
         <v>246</v>
       </c>
-      <c r="W19" s="114">
+      <c r="W19" s="109">
         <v>42403</v>
       </c>
       <c r="X19" s="18" t="s">
@@ -3462,54 +3483,54 @@
       </c>
       <c r="E20" s="12"/>
       <c r="F20" s="12"/>
-      <c r="G20" s="116" t="s">
+      <c r="G20" s="111" t="s">
         <v>241</v>
       </c>
-      <c r="H20" s="117">
+      <c r="H20" s="112">
         <v>18</v>
       </c>
-      <c r="I20" s="117" t="s">
+      <c r="I20" s="112" t="s">
         <v>19</v>
       </c>
-      <c r="J20" s="90" t="s">
+      <c r="J20" s="85" t="s">
         <v>242</v>
       </c>
-      <c r="K20" s="117" t="s">
+      <c r="K20" s="112" t="s">
         <v>20</v>
       </c>
-      <c r="L20" s="117" t="s">
+      <c r="L20" s="112" t="s">
         <v>5</v>
       </c>
-      <c r="M20" s="117" t="s">
+      <c r="M20" s="112" t="s">
         <v>58</v>
       </c>
-      <c r="N20" s="117"/>
-      <c r="O20" s="90" t="s">
+      <c r="N20" s="112"/>
+      <c r="O20" s="85" t="s">
         <v>153</v>
       </c>
-      <c r="P20" s="118" t="s">
+      <c r="P20" s="113" t="s">
         <v>19</v>
       </c>
-      <c r="Q20" s="119">
+      <c r="Q20" s="114">
         <v>6</v>
       </c>
-      <c r="R20" s="119" t="s">
+      <c r="R20" s="114" t="s">
         <v>188</v>
       </c>
-      <c r="S20" s="119" t="s">
+      <c r="S20" s="114" t="s">
         <v>189</v>
       </c>
-      <c r="T20" s="120" t="s">
+      <c r="T20" s="115" t="s">
         <v>209</v>
       </c>
-      <c r="U20" s="121" t="s">
+      <c r="U20" s="116" t="s">
         <v>191</v>
       </c>
-      <c r="V20" s="106" t="s">
+      <c r="V20" s="101" t="s">
         <v>254</v>
       </c>
       <c r="W20" s="3"/>
-      <c r="X20" s="115">
+      <c r="X20" s="110">
         <v>42415</v>
       </c>
     </row>
@@ -3528,56 +3549,56 @@
       </c>
       <c r="E21" s="12"/>
       <c r="F21" s="12"/>
-      <c r="G21" s="116" t="s">
+      <c r="G21" s="111" t="s">
         <v>154</v>
       </c>
-      <c r="H21" s="118">
+      <c r="H21" s="113">
         <v>19</v>
       </c>
-      <c r="I21" s="117" t="s">
+      <c r="I21" s="112" t="s">
         <v>20</v>
       </c>
-      <c r="J21" s="90" t="s">
+      <c r="J21" s="85" t="s">
         <v>231</v>
       </c>
-      <c r="K21" s="117" t="s">
+      <c r="K21" s="112" t="s">
         <v>20</v>
       </c>
-      <c r="L21" s="117" t="s">
+      <c r="L21" s="112" t="s">
         <v>8</v>
       </c>
-      <c r="M21" s="117"/>
-      <c r="N21" s="117" t="s">
+      <c r="M21" s="112"/>
+      <c r="N21" s="112" t="s">
         <v>33</v>
       </c>
-      <c r="O21" s="90" t="s">
+      <c r="O21" s="85" t="s">
         <v>155</v>
       </c>
-      <c r="P21" s="118" t="s">
+      <c r="P21" s="113" t="s">
         <v>19</v>
       </c>
-      <c r="Q21" s="119">
+      <c r="Q21" s="114">
         <v>6</v>
       </c>
-      <c r="R21" s="119" t="s">
+      <c r="R21" s="114" t="s">
         <v>192</v>
       </c>
-      <c r="S21" s="119" t="s">
+      <c r="S21" s="114" t="s">
         <v>193</v>
       </c>
-      <c r="T21" s="120" t="s">
+      <c r="T21" s="115" t="s">
         <v>210</v>
       </c>
-      <c r="U21" s="121" t="s">
+      <c r="U21" s="116" t="s">
         <v>195</v>
       </c>
-      <c r="V21" s="106" t="s">
+      <c r="V21" s="101" t="s">
         <v>247</v>
       </c>
-      <c r="W21" s="114">
+      <c r="W21" s="109">
         <v>42419</v>
       </c>
-      <c r="X21" s="115">
+      <c r="X21" s="110">
         <v>42419</v>
       </c>
     </row>
@@ -3596,54 +3617,54 @@
       </c>
       <c r="E22" s="12"/>
       <c r="F22" s="12"/>
-      <c r="G22" s="116" t="s">
+      <c r="G22" s="111" t="s">
         <v>156</v>
       </c>
-      <c r="H22" s="117">
+      <c r="H22" s="112">
         <v>20</v>
       </c>
-      <c r="I22" s="117" t="s">
+      <c r="I22" s="112" t="s">
         <v>20</v>
       </c>
-      <c r="J22" s="90" t="s">
+      <c r="J22" s="85" t="s">
         <v>157</v>
       </c>
-      <c r="K22" s="117" t="s">
+      <c r="K22" s="112" t="s">
         <v>20</v>
       </c>
-      <c r="L22" s="117" t="s">
+      <c r="L22" s="112" t="s">
         <v>8</v>
       </c>
-      <c r="M22" s="117"/>
-      <c r="N22" s="117" t="s">
+      <c r="M22" s="112"/>
+      <c r="N22" s="112" t="s">
         <v>120</v>
       </c>
-      <c r="O22" s="90" t="s">
+      <c r="O22" s="85" t="s">
         <v>158</v>
       </c>
-      <c r="P22" s="118" t="s">
+      <c r="P22" s="113" t="s">
         <v>20</v>
       </c>
-      <c r="Q22" s="119">
+      <c r="Q22" s="114">
         <v>6</v>
       </c>
-      <c r="R22" s="119" t="s">
+      <c r="R22" s="114" t="s">
         <v>192</v>
       </c>
-      <c r="S22" s="119" t="s">
+      <c r="S22" s="114" t="s">
         <v>193</v>
       </c>
-      <c r="T22" s="120" t="s">
+      <c r="T22" s="115" t="s">
         <v>211</v>
       </c>
-      <c r="U22" s="121" t="s">
+      <c r="U22" s="116" t="s">
         <v>195</v>
       </c>
-      <c r="V22" s="106" t="s">
+      <c r="V22" s="101" t="s">
         <v>254</v>
       </c>
       <c r="W22" s="18"/>
-      <c r="X22" s="115">
+      <c r="X22" s="110">
         <v>42422</v>
       </c>
       <c r="Y22" s="4" t="s">
@@ -3665,53 +3686,53 @@
       </c>
       <c r="E23" s="12"/>
       <c r="F23" s="12"/>
-      <c r="G23" s="101" t="s">
+      <c r="G23" s="96" t="s">
         <v>159</v>
       </c>
-      <c r="H23" s="102">
+      <c r="H23" s="97">
         <v>21</v>
       </c>
-      <c r="I23" s="103" t="s">
+      <c r="I23" s="98" t="s">
         <v>20</v>
       </c>
-      <c r="J23" s="89" t="s">
+      <c r="J23" s="84" t="s">
         <v>160</v>
       </c>
-      <c r="K23" s="103" t="s">
+      <c r="K23" s="98" t="s">
         <v>20</v>
       </c>
-      <c r="L23" s="103" t="s">
+      <c r="L23" s="98" t="s">
         <v>8</v>
       </c>
-      <c r="M23" s="103"/>
-      <c r="N23" s="103" t="s">
+      <c r="M23" s="98"/>
+      <c r="N23" s="98" t="s">
         <v>24</v>
       </c>
-      <c r="O23" s="89" t="s">
+      <c r="O23" s="84" t="s">
         <v>161</v>
       </c>
-      <c r="P23" s="102" t="s">
+      <c r="P23" s="97" t="s">
         <v>19</v>
       </c>
-      <c r="Q23" s="104">
+      <c r="Q23" s="99">
         <v>6</v>
       </c>
-      <c r="R23" s="104" t="s">
+      <c r="R23" s="99" t="s">
         <v>192</v>
       </c>
-      <c r="S23" s="104" t="s">
+      <c r="S23" s="99" t="s">
         <v>193</v>
       </c>
-      <c r="T23" s="113" t="s">
+      <c r="T23" s="108" t="s">
         <v>212</v>
       </c>
-      <c r="U23" s="105" t="s">
+      <c r="U23" s="100" t="s">
         <v>195</v>
       </c>
-      <c r="V23" s="106" t="s">
+      <c r="V23" s="101" t="s">
         <v>250</v>
       </c>
-      <c r="W23" s="114">
+      <c r="W23" s="109">
         <v>42408</v>
       </c>
       <c r="X23" s="3" t="s">
@@ -3735,54 +3756,54 @@
         <v>122</v>
       </c>
       <c r="F24" s="13"/>
-      <c r="G24" s="136" t="s">
+      <c r="G24" s="131" t="s">
         <v>183</v>
       </c>
-      <c r="H24" s="137">
+      <c r="H24" s="132">
         <v>22</v>
       </c>
-      <c r="I24" s="138" t="s">
+      <c r="I24" s="133" t="s">
         <v>20</v>
       </c>
-      <c r="J24" s="139" t="s">
+      <c r="J24" s="134" t="s">
         <v>162</v>
       </c>
-      <c r="K24" s="138" t="s">
+      <c r="K24" s="133" t="s">
         <v>20</v>
       </c>
-      <c r="L24" s="138" t="s">
+      <c r="L24" s="133" t="s">
         <v>8</v>
       </c>
-      <c r="M24" s="138"/>
-      <c r="N24" s="138" t="s">
+      <c r="M24" s="133"/>
+      <c r="N24" s="133" t="s">
         <v>121</v>
       </c>
-      <c r="O24" s="139"/>
-      <c r="P24" s="137" t="s">
+      <c r="O24" s="134"/>
+      <c r="P24" s="132" t="s">
         <v>19</v>
       </c>
-      <c r="Q24" s="140">
+      <c r="Q24" s="135">
         <v>6</v>
       </c>
-      <c r="R24" s="140" t="s">
+      <c r="R24" s="135" t="s">
         <v>192</v>
       </c>
-      <c r="S24" s="140" t="s">
+      <c r="S24" s="135" t="s">
         <v>193</v>
       </c>
-      <c r="T24" s="141" t="s">
+      <c r="T24" s="136" t="s">
         <v>213</v>
       </c>
-      <c r="U24" s="142" t="s">
+      <c r="U24" s="137" t="s">
         <v>195</v>
       </c>
-      <c r="V24" s="106" t="s">
+      <c r="V24" s="101" t="s">
         <v>247</v>
       </c>
-      <c r="W24" s="114">
+      <c r="W24" s="109">
         <v>42419</v>
       </c>
-      <c r="X24" s="115">
+      <c r="X24" s="110">
         <v>42419</v>
       </c>
     </row>
@@ -3801,49 +3822,49 @@
       </c>
       <c r="E25" s="14"/>
       <c r="F25" s="14"/>
-      <c r="G25" s="95" t="s">
+      <c r="G25" s="90" t="s">
         <v>258</v>
       </c>
-      <c r="H25" s="96">
+      <c r="H25" s="91">
         <v>23</v>
       </c>
-      <c r="I25" s="96" t="s">
+      <c r="I25" s="91" t="s">
         <v>20</v>
       </c>
-      <c r="J25" s="97" t="s">
+      <c r="J25" s="92" t="s">
         <v>164</v>
       </c>
-      <c r="K25" s="96" t="s">
+      <c r="K25" s="91" t="s">
         <v>19</v>
       </c>
-      <c r="L25" s="96" t="s">
+      <c r="L25" s="91" t="s">
         <v>8</v>
       </c>
-      <c r="M25" s="96"/>
-      <c r="N25" s="96"/>
-      <c r="O25" s="97"/>
-      <c r="P25" s="98" t="s">
+      <c r="M25" s="91"/>
+      <c r="N25" s="91"/>
+      <c r="O25" s="92"/>
+      <c r="P25" s="93" t="s">
         <v>19</v>
       </c>
-      <c r="Q25" s="99">
+      <c r="Q25" s="94">
         <v>8</v>
       </c>
-      <c r="R25" s="99" t="s">
+      <c r="R25" s="94" t="s">
         <v>217</v>
       </c>
-      <c r="S25" s="99" t="s">
+      <c r="S25" s="94" t="s">
         <v>218</v>
       </c>
-      <c r="T25" s="99" t="s">
+      <c r="T25" s="94" t="s">
         <v>163</v>
       </c>
-      <c r="U25" s="100" t="s">
+      <c r="U25" s="95" t="s">
         <v>219</v>
       </c>
-      <c r="V25" s="106" t="s">
+      <c r="V25" s="101" t="s">
         <v>246</v>
       </c>
-      <c r="W25" s="114">
+      <c r="W25" s="109">
         <v>42404</v>
       </c>
       <c r="X25" s="18" t="s">
@@ -3865,49 +3886,49 @@
       </c>
       <c r="E26" s="15"/>
       <c r="F26" s="15"/>
-      <c r="G26" s="101" t="s">
+      <c r="G26" s="96" t="s">
         <v>165</v>
       </c>
-      <c r="H26" s="102">
+      <c r="H26" s="97">
         <v>24</v>
       </c>
-      <c r="I26" s="103" t="s">
+      <c r="I26" s="98" t="s">
         <v>20</v>
       </c>
-      <c r="J26" s="89" t="s">
+      <c r="J26" s="84" t="s">
         <v>166</v>
       </c>
-      <c r="K26" s="103" t="s">
+      <c r="K26" s="98" t="s">
         <v>19</v>
       </c>
-      <c r="L26" s="103" t="s">
+      <c r="L26" s="98" t="s">
         <v>8</v>
       </c>
-      <c r="M26" s="103"/>
-      <c r="N26" s="103"/>
-      <c r="O26" s="89"/>
-      <c r="P26" s="102" t="s">
+      <c r="M26" s="98"/>
+      <c r="N26" s="98"/>
+      <c r="O26" s="84"/>
+      <c r="P26" s="97" t="s">
         <v>19</v>
       </c>
-      <c r="Q26" s="104">
+      <c r="Q26" s="99">
         <v>8</v>
       </c>
-      <c r="R26" s="104" t="s">
+      <c r="R26" s="99" t="s">
         <v>217</v>
       </c>
-      <c r="S26" s="104" t="s">
+      <c r="S26" s="99" t="s">
         <v>218</v>
       </c>
-      <c r="T26" s="104" t="s">
+      <c r="T26" s="99" t="s">
         <v>165</v>
       </c>
-      <c r="U26" s="105" t="s">
+      <c r="U26" s="100" t="s">
         <v>219</v>
       </c>
-      <c r="V26" s="106" t="s">
+      <c r="V26" s="101" t="s">
         <v>246</v>
       </c>
-      <c r="W26" s="114">
+      <c r="W26" s="109">
         <v>42404</v>
       </c>
       <c r="X26" s="18" t="s">
@@ -3929,46 +3950,46 @@
       </c>
       <c r="E27" s="15"/>
       <c r="F27" s="15"/>
-      <c r="G27" s="107" t="s">
+      <c r="G27" s="102" t="s">
         <v>167</v>
       </c>
-      <c r="H27" s="108">
+      <c r="H27" s="103">
         <v>25</v>
       </c>
-      <c r="I27" s="109" t="s">
+      <c r="I27" s="104" t="s">
         <v>20</v>
       </c>
-      <c r="J27" s="92" t="s">
+      <c r="J27" s="87" t="s">
         <v>259</v>
       </c>
-      <c r="K27" s="109" t="s">
+      <c r="K27" s="104" t="s">
         <v>19</v>
       </c>
-      <c r="L27" s="109" t="s">
+      <c r="L27" s="104" t="s">
         <v>8</v>
       </c>
-      <c r="M27" s="109"/>
-      <c r="N27" s="109"/>
-      <c r="O27" s="92"/>
-      <c r="P27" s="108" t="s">
+      <c r="M27" s="104"/>
+      <c r="N27" s="104"/>
+      <c r="O27" s="87"/>
+      <c r="P27" s="103" t="s">
         <v>19</v>
       </c>
-      <c r="Q27" s="110">
+      <c r="Q27" s="105">
         <v>8</v>
       </c>
-      <c r="R27" s="110" t="s">
+      <c r="R27" s="105" t="s">
         <v>217</v>
       </c>
-      <c r="S27" s="110" t="s">
+      <c r="S27" s="105" t="s">
         <v>218</v>
       </c>
-      <c r="T27" s="110" t="s">
+      <c r="T27" s="105" t="s">
         <v>220</v>
       </c>
-      <c r="U27" s="111" t="s">
+      <c r="U27" s="106" t="s">
         <v>219</v>
       </c>
-      <c r="V27" s="106" t="s">
+      <c r="V27" s="101" t="s">
         <v>246</v>
       </c>
       <c r="W27" s="18" t="s">
@@ -3993,49 +4014,49 @@
       </c>
       <c r="E28" s="15"/>
       <c r="F28" s="15"/>
-      <c r="G28" s="101" t="s">
+      <c r="G28" s="96" t="s">
         <v>168</v>
       </c>
-      <c r="H28" s="103">
+      <c r="H28" s="98">
         <v>26</v>
       </c>
-      <c r="I28" s="103" t="s">
+      <c r="I28" s="98" t="s">
         <v>20</v>
       </c>
-      <c r="J28" s="89" t="s">
+      <c r="J28" s="84" t="s">
         <v>261</v>
       </c>
-      <c r="K28" s="103" t="s">
+      <c r="K28" s="98" t="s">
         <v>19</v>
       </c>
-      <c r="L28" s="103" t="s">
+      <c r="L28" s="98" t="s">
         <v>8</v>
       </c>
-      <c r="M28" s="103"/>
-      <c r="N28" s="103"/>
-      <c r="O28" s="89"/>
-      <c r="P28" s="102" t="s">
+      <c r="M28" s="98"/>
+      <c r="N28" s="98"/>
+      <c r="O28" s="84"/>
+      <c r="P28" s="97" t="s">
         <v>19</v>
       </c>
-      <c r="Q28" s="104">
+      <c r="Q28" s="99">
         <v>8</v>
       </c>
-      <c r="R28" s="104" t="s">
+      <c r="R28" s="99" t="s">
         <v>217</v>
       </c>
-      <c r="S28" s="104" t="s">
+      <c r="S28" s="99" t="s">
         <v>218</v>
       </c>
-      <c r="T28" s="104" t="s">
+      <c r="T28" s="99" t="s">
         <v>221</v>
       </c>
-      <c r="U28" s="105" t="s">
+      <c r="U28" s="100" t="s">
         <v>219</v>
       </c>
-      <c r="V28" s="106" t="s">
+      <c r="V28" s="101" t="s">
         <v>246</v>
       </c>
-      <c r="W28" s="114">
+      <c r="W28" s="109">
         <v>42404</v>
       </c>
       <c r="X28" s="18" t="s">
@@ -4043,60 +4064,60 @@
       </c>
     </row>
     <row r="29" spans="1:25" s="11" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A29" s="82" t="s">
+      <c r="A29" s="77" t="s">
         <v>15</v>
       </c>
-      <c r="B29" s="64" t="s">
+      <c r="B29" s="59" t="s">
         <v>124</v>
       </c>
-      <c r="C29" s="64" t="s">
+      <c r="C29" s="59" t="s">
         <v>123</v>
       </c>
-      <c r="D29" s="64" t="s">
+      <c r="D29" s="59" t="s">
         <v>186</v>
       </c>
       <c r="E29" s="18"/>
       <c r="F29" s="18"/>
-      <c r="G29" s="107" t="s">
+      <c r="G29" s="102" t="s">
         <v>169</v>
       </c>
-      <c r="H29" s="108">
+      <c r="H29" s="103">
         <v>27</v>
       </c>
-      <c r="I29" s="109" t="s">
+      <c r="I29" s="104" t="s">
         <v>19</v>
       </c>
-      <c r="J29" s="92" t="s">
+      <c r="J29" s="87" t="s">
         <v>170</v>
       </c>
-      <c r="K29" s="109" t="s">
+      <c r="K29" s="104" t="s">
         <v>19</v>
       </c>
-      <c r="L29" s="109" t="s">
+      <c r="L29" s="104" t="s">
         <v>5</v>
       </c>
-      <c r="M29" s="109"/>
-      <c r="N29" s="109"/>
-      <c r="O29" s="92"/>
-      <c r="P29" s="108" t="s">
+      <c r="M29" s="104"/>
+      <c r="N29" s="104"/>
+      <c r="O29" s="87"/>
+      <c r="P29" s="103" t="s">
         <v>20</v>
       </c>
-      <c r="Q29" s="110">
+      <c r="Q29" s="105">
         <v>8</v>
       </c>
-      <c r="R29" s="110" t="s">
+      <c r="R29" s="105" t="s">
         <v>217</v>
       </c>
-      <c r="S29" s="110" t="s">
+      <c r="S29" s="105" t="s">
         <v>218</v>
       </c>
-      <c r="T29" s="110" t="s">
+      <c r="T29" s="105" t="s">
         <v>169</v>
       </c>
-      <c r="U29" s="111" t="s">
+      <c r="U29" s="106" t="s">
         <v>219</v>
       </c>
-      <c r="V29" s="106" t="s">
+      <c r="V29" s="101" t="s">
         <v>246</v>
       </c>
       <c r="W29" s="18" t="s">
@@ -4164,11 +4185,11 @@
       <c r="U30" s="48" t="s">
         <v>191</v>
       </c>
-      <c r="V30" s="87" t="s">
+      <c r="V30" s="82" t="s">
         <v>248</v>
       </c>
-      <c r="W30" s="91"/>
-      <c r="X30" s="91"/>
+      <c r="W30" s="86"/>
+      <c r="X30" s="86"/>
     </row>
     <row r="31" spans="1:25" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A31" s="49" t="s">
@@ -4185,57 +4206,57 @@
       </c>
       <c r="E31" s="17"/>
       <c r="F31" s="17"/>
-      <c r="G31" s="177" t="s">
+      <c r="G31" s="141" t="s">
         <v>243</v>
       </c>
-      <c r="H31" s="178">
+      <c r="H31" s="142">
         <v>29</v>
       </c>
-      <c r="I31" s="178" t="s">
+      <c r="I31" s="142" t="s">
         <v>20</v>
       </c>
-      <c r="J31" s="179" t="s">
+      <c r="J31" s="143" t="s">
         <v>244</v>
       </c>
-      <c r="K31" s="178" t="s">
+      <c r="K31" s="142" t="s">
         <v>20</v>
       </c>
-      <c r="L31" s="178" t="s">
+      <c r="L31" s="142" t="s">
         <v>8</v>
       </c>
-      <c r="M31" s="178"/>
-      <c r="N31" s="178" t="s">
+      <c r="M31" s="142"/>
+      <c r="N31" s="142" t="s">
         <v>121</v>
       </c>
-      <c r="O31" s="179" t="s">
+      <c r="O31" s="143" t="s">
         <v>174</v>
       </c>
-      <c r="P31" s="180" t="s">
+      <c r="P31" s="144" t="s">
         <v>19</v>
       </c>
-      <c r="Q31" s="181">
+      <c r="Q31" s="145">
         <v>6</v>
       </c>
-      <c r="R31" s="181" t="s">
+      <c r="R31" s="145" t="s">
         <v>192</v>
       </c>
-      <c r="S31" s="181" t="s">
+      <c r="S31" s="145" t="s">
         <v>193</v>
       </c>
-      <c r="T31" s="182" t="s">
+      <c r="T31" s="146" t="s">
         <v>213</v>
       </c>
-      <c r="U31" s="183" t="s">
+      <c r="U31" s="147" t="s">
         <v>195</v>
       </c>
-      <c r="V31" s="184" t="s">
+      <c r="V31" s="148" t="s">
         <v>248</v>
       </c>
-      <c r="W31" s="185"/>
-      <c r="X31" s="185" t="s">
+      <c r="W31" s="149"/>
+      <c r="X31" s="149" t="s">
         <v>257</v>
       </c>
-      <c r="Y31" s="186" t="s">
+      <c r="Y31" s="150" t="s">
         <v>272</v>
       </c>
     </row>
@@ -4254,54 +4275,57 @@
       </c>
       <c r="E32" s="55"/>
       <c r="F32" s="55"/>
-      <c r="G32" s="56" t="s">
+      <c r="G32" s="186" t="s">
         <v>175</v>
       </c>
-      <c r="H32" s="57">
+      <c r="H32" s="187">
         <v>30</v>
       </c>
-      <c r="I32" s="37" t="s">
+      <c r="I32" s="188" t="s">
         <v>20</v>
       </c>
-      <c r="J32" s="55" t="s">
+      <c r="J32" s="189" t="s">
         <v>245</v>
       </c>
-      <c r="K32" s="37" t="s">
+      <c r="K32" s="188" t="s">
         <v>20</v>
       </c>
-      <c r="L32" s="37" t="s">
+      <c r="L32" s="188" t="s">
         <v>8</v>
       </c>
-      <c r="M32" s="37"/>
-      <c r="N32" s="37" t="s">
+      <c r="M32" s="188"/>
+      <c r="N32" s="188" t="s">
         <v>120</v>
       </c>
-      <c r="O32" s="58" t="s">
+      <c r="O32" s="190" t="s">
         <v>176</v>
       </c>
-      <c r="P32" s="57" t="s">
+      <c r="P32" s="187" t="s">
         <v>19</v>
       </c>
-      <c r="Q32" s="59">
+      <c r="Q32" s="191">
         <v>6</v>
       </c>
-      <c r="R32" s="59" t="s">
+      <c r="R32" s="191" t="s">
         <v>192</v>
       </c>
-      <c r="S32" s="59" t="s">
+      <c r="S32" s="191" t="s">
         <v>193</v>
       </c>
-      <c r="T32" s="60" t="s">
+      <c r="T32" s="192" t="s">
         <v>214</v>
       </c>
-      <c r="U32" s="59" t="s">
+      <c r="U32" s="191" t="s">
         <v>195</v>
       </c>
-      <c r="V32" s="87" t="s">
+      <c r="V32" s="148" t="s">
         <v>254</v>
       </c>
-      <c r="W32" s="91"/>
-      <c r="X32" s="91"/>
+      <c r="W32" s="149"/>
+      <c r="X32" s="149"/>
+      <c r="Y32" s="185" t="s">
+        <v>274</v>
+      </c>
     </row>
     <row r="33" spans="1:24" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A33" s="37" t="s">
@@ -4318,40 +4342,40 @@
       </c>
       <c r="E33" s="38"/>
       <c r="F33" s="38"/>
-      <c r="G33" s="107" t="s">
+      <c r="G33" s="102" t="s">
         <v>10</v>
       </c>
-      <c r="H33" s="108">
+      <c r="H33" s="103">
         <v>31</v>
       </c>
-      <c r="I33" s="109" t="s">
+      <c r="I33" s="104" t="s">
         <v>20</v>
       </c>
-      <c r="J33" s="92" t="s">
+      <c r="J33" s="87" t="s">
         <v>179</v>
       </c>
-      <c r="K33" s="109" t="s">
+      <c r="K33" s="104" t="s">
         <v>20</v>
       </c>
-      <c r="L33" s="109" t="s">
+      <c r="L33" s="104" t="s">
         <v>10</v>
       </c>
-      <c r="M33" s="109"/>
-      <c r="N33" s="109"/>
-      <c r="O33" s="92"/>
-      <c r="P33" s="108" t="s">
+      <c r="M33" s="104"/>
+      <c r="N33" s="104"/>
+      <c r="O33" s="87"/>
+      <c r="P33" s="103" t="s">
         <v>19</v>
       </c>
-      <c r="Q33" s="110"/>
-      <c r="R33" s="110"/>
-      <c r="S33" s="110"/>
-      <c r="T33" s="110"/>
-      <c r="U33" s="110"/>
-      <c r="V33" s="112" t="s">
+      <c r="Q33" s="105"/>
+      <c r="R33" s="105"/>
+      <c r="S33" s="105"/>
+      <c r="T33" s="105"/>
+      <c r="U33" s="105"/>
+      <c r="V33" s="107" t="s">
         <v>246</v>
       </c>
-      <c r="W33" s="108"/>
-      <c r="X33" s="91" t="s">
+      <c r="W33" s="103"/>
+      <c r="X33" s="86" t="s">
         <v>260</v>
       </c>
     </row>
@@ -4370,65 +4394,65 @@
       </c>
       <c r="E34" s="38"/>
       <c r="F34" s="38"/>
-      <c r="G34" s="116" t="s">
+      <c r="G34" s="111" t="s">
         <v>177</v>
       </c>
-      <c r="H34" s="117">
+      <c r="H34" s="112">
         <v>32</v>
       </c>
-      <c r="I34" s="117" t="s">
+      <c r="I34" s="112" t="s">
         <v>20</v>
       </c>
-      <c r="J34" s="90" t="s">
+      <c r="J34" s="85" t="s">
         <v>180</v>
       </c>
-      <c r="K34" s="117" t="s">
+      <c r="K34" s="112" t="s">
         <v>20</v>
       </c>
-      <c r="L34" s="117" t="s">
+      <c r="L34" s="112" t="s">
         <v>8</v>
       </c>
-      <c r="M34" s="117"/>
-      <c r="N34" s="117" t="s">
+      <c r="M34" s="112"/>
+      <c r="N34" s="112" t="s">
         <v>33</v>
       </c>
-      <c r="O34" s="90"/>
-      <c r="P34" s="118" t="s">
+      <c r="O34" s="85"/>
+      <c r="P34" s="113" t="s">
         <v>19</v>
       </c>
-      <c r="Q34" s="119">
+      <c r="Q34" s="114">
         <v>6</v>
       </c>
-      <c r="R34" s="119" t="s">
+      <c r="R34" s="114" t="s">
         <v>192</v>
       </c>
-      <c r="S34" s="119" t="s">
+      <c r="S34" s="114" t="s">
         <v>193</v>
       </c>
-      <c r="T34" s="120" t="s">
+      <c r="T34" s="115" t="s">
         <v>215</v>
       </c>
-      <c r="U34" s="119" t="s">
+      <c r="U34" s="114" t="s">
         <v>195</v>
       </c>
-      <c r="V34" s="143" t="s">
+      <c r="V34" s="138" t="s">
         <v>247</v>
       </c>
-      <c r="W34" s="144">
+      <c r="W34" s="139">
         <v>42420</v>
       </c>
-      <c r="X34" s="145">
+      <c r="X34" s="140">
         <v>42420</v>
       </c>
     </row>
     <row r="35" spans="1:24" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A35" s="64" t="s">
+      <c r="A35" s="59" t="s">
         <v>15</v>
       </c>
-      <c r="B35" s="64" t="s">
+      <c r="B35" s="59" t="s">
         <v>124</v>
       </c>
-      <c r="C35" s="64" t="s">
+      <c r="C35" s="59" t="s">
         <v>123</v>
       </c>
       <c r="D35" s="18" t="s">
@@ -4439,99 +4463,99 @@
       <c r="G35" s="21" t="s">
         <v>178</v>
       </c>
-      <c r="H35" s="62">
+      <c r="H35" s="57">
         <v>33</v>
       </c>
-      <c r="I35" s="61" t="s">
+      <c r="I35" s="56" t="s">
         <v>20</v>
       </c>
       <c r="J35" s="18" t="s">
         <v>181</v>
       </c>
-      <c r="K35" s="61" t="s">
+      <c r="K35" s="56" t="s">
         <v>20</v>
       </c>
-      <c r="L35" s="61" t="s">
+      <c r="L35" s="56" t="s">
         <v>8</v>
       </c>
-      <c r="M35" s="61"/>
-      <c r="N35" s="61" t="s">
+      <c r="M35" s="56"/>
+      <c r="N35" s="56" t="s">
         <v>52</v>
       </c>
       <c r="O35" s="18"/>
-      <c r="P35" s="62" t="s">
+      <c r="P35" s="57" t="s">
         <v>20</v>
       </c>
-      <c r="Q35" s="63">
+      <c r="Q35" s="58">
         <v>6</v>
       </c>
-      <c r="R35" s="63" t="s">
+      <c r="R35" s="58" t="s">
         <v>192</v>
       </c>
-      <c r="S35" s="63" t="s">
+      <c r="S35" s="58" t="s">
         <v>193</v>
       </c>
-      <c r="T35" s="84" t="s">
+      <c r="T35" s="79" t="s">
         <v>216</v>
       </c>
-      <c r="U35" s="63" t="s">
+      <c r="U35" s="58" t="s">
         <v>195</v>
       </c>
-      <c r="V35" s="88" t="s">
+      <c r="V35" s="83" t="s">
         <v>248</v>
       </c>
-      <c r="W35" s="91"/>
-      <c r="X35" s="91"/>
+      <c r="W35" s="86"/>
+      <c r="X35" s="86"/>
     </row>
     <row r="36" spans="1:24" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A36" s="65"/>
-      <c r="B36" s="66"/>
-      <c r="C36" s="66"/>
-      <c r="D36" s="66"/>
-      <c r="E36" s="66"/>
-      <c r="F36" s="66"/>
-      <c r="G36" s="67"/>
-      <c r="H36" s="66"/>
-      <c r="I36" s="65"/>
-      <c r="J36" s="66"/>
-      <c r="K36" s="65"/>
-      <c r="L36" s="65"/>
-      <c r="M36" s="65"/>
-      <c r="N36" s="65"/>
-      <c r="O36" s="66"/>
-      <c r="P36" s="68"/>
-      <c r="Q36" s="69"/>
-      <c r="R36" s="69"/>
-      <c r="S36" s="69"/>
-      <c r="T36" s="69"/>
-      <c r="U36" s="69"/>
-      <c r="V36" s="70"/>
+      <c r="A36" s="60"/>
+      <c r="B36" s="61"/>
+      <c r="C36" s="61"/>
+      <c r="D36" s="61"/>
+      <c r="E36" s="61"/>
+      <c r="F36" s="61"/>
+      <c r="G36" s="62"/>
+      <c r="H36" s="61"/>
+      <c r="I36" s="60"/>
+      <c r="J36" s="61"/>
+      <c r="K36" s="60"/>
+      <c r="L36" s="60"/>
+      <c r="M36" s="60"/>
+      <c r="N36" s="60"/>
+      <c r="O36" s="61"/>
+      <c r="P36" s="63"/>
+      <c r="Q36" s="64"/>
+      <c r="R36" s="64"/>
+      <c r="S36" s="64"/>
+      <c r="T36" s="64"/>
+      <c r="U36" s="64"/>
+      <c r="V36" s="65"/>
       <c r="W36" s="16"/>
       <c r="X36" s="16"/>
     </row>
     <row r="37" spans="1:24" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A37" s="71"/>
-      <c r="B37" s="72"/>
-      <c r="C37" s="72"/>
-      <c r="D37" s="72"/>
-      <c r="E37" s="72"/>
-      <c r="F37" s="72"/>
-      <c r="G37" s="73"/>
-      <c r="H37" s="72"/>
-      <c r="I37" s="71"/>
-      <c r="J37" s="72"/>
-      <c r="K37" s="71"/>
-      <c r="L37" s="71"/>
-      <c r="M37" s="71"/>
-      <c r="N37" s="71"/>
-      <c r="O37" s="72"/>
-      <c r="P37" s="74"/>
-      <c r="Q37" s="75"/>
-      <c r="R37" s="75"/>
-      <c r="S37" s="75"/>
-      <c r="T37" s="75"/>
-      <c r="U37" s="75"/>
-      <c r="V37" s="74" t="s">
+      <c r="A37" s="66"/>
+      <c r="B37" s="67"/>
+      <c r="C37" s="67"/>
+      <c r="D37" s="67"/>
+      <c r="E37" s="67"/>
+      <c r="F37" s="67"/>
+      <c r="G37" s="68"/>
+      <c r="H37" s="67"/>
+      <c r="I37" s="66"/>
+      <c r="J37" s="67"/>
+      <c r="K37" s="66"/>
+      <c r="L37" s="66"/>
+      <c r="M37" s="66"/>
+      <c r="N37" s="66"/>
+      <c r="O37" s="67"/>
+      <c r="P37" s="69"/>
+      <c r="Q37" s="70"/>
+      <c r="R37" s="70"/>
+      <c r="S37" s="70"/>
+      <c r="T37" s="70"/>
+      <c r="U37" s="70"/>
+      <c r="V37" s="69" t="s">
         <v>270</v>
       </c>
       <c r="W37" s="16" t="s">
@@ -4540,28 +4564,28 @@
       <c r="X37" s="16"/>
     </row>
     <row r="38" spans="1:24" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A38" s="71"/>
-      <c r="B38" s="72"/>
-      <c r="C38" s="72"/>
-      <c r="D38" s="72"/>
-      <c r="E38" s="72"/>
-      <c r="F38" s="72"/>
-      <c r="G38" s="73"/>
-      <c r="H38" s="72"/>
-      <c r="I38" s="71"/>
-      <c r="J38" s="72"/>
-      <c r="K38" s="71"/>
-      <c r="L38" s="71"/>
-      <c r="M38" s="71"/>
-      <c r="N38" s="71"/>
-      <c r="O38" s="72"/>
-      <c r="P38" s="74"/>
-      <c r="Q38" s="74"/>
-      <c r="R38" s="74"/>
-      <c r="S38" s="74"/>
-      <c r="T38" s="74"/>
-      <c r="U38" s="74"/>
-      <c r="V38" s="74"/>
+      <c r="A38" s="66"/>
+      <c r="B38" s="67"/>
+      <c r="C38" s="67"/>
+      <c r="D38" s="67"/>
+      <c r="E38" s="67"/>
+      <c r="F38" s="67"/>
+      <c r="G38" s="68"/>
+      <c r="H38" s="67"/>
+      <c r="I38" s="66"/>
+      <c r="J38" s="67"/>
+      <c r="K38" s="66"/>
+      <c r="L38" s="66"/>
+      <c r="M38" s="66"/>
+      <c r="N38" s="66"/>
+      <c r="O38" s="67"/>
+      <c r="P38" s="69"/>
+      <c r="Q38" s="69"/>
+      <c r="R38" s="69"/>
+      <c r="S38" s="69"/>
+      <c r="T38" s="69"/>
+      <c r="U38" s="69"/>
+      <c r="V38" s="69"/>
       <c r="W38" s="16" t="s">
         <v>268</v>
       </c>
@@ -4570,28 +4594,28 @@
       </c>
     </row>
     <row r="39" spans="1:24" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A39" s="71"/>
-      <c r="B39" s="72"/>
-      <c r="C39" s="72"/>
-      <c r="D39" s="72"/>
-      <c r="E39" s="72"/>
-      <c r="F39" s="72"/>
-      <c r="G39" s="73"/>
-      <c r="H39" s="72"/>
-      <c r="I39" s="71"/>
-      <c r="J39" s="72"/>
-      <c r="K39" s="71"/>
-      <c r="L39" s="71"/>
-      <c r="M39" s="71"/>
-      <c r="N39" s="71"/>
-      <c r="O39" s="72"/>
-      <c r="P39" s="74"/>
-      <c r="Q39" s="74"/>
-      <c r="R39" s="74"/>
-      <c r="S39" s="74"/>
-      <c r="T39" s="74"/>
-      <c r="U39" s="74"/>
-      <c r="V39" s="74" t="s">
+      <c r="A39" s="66"/>
+      <c r="B39" s="67"/>
+      <c r="C39" s="67"/>
+      <c r="D39" s="67"/>
+      <c r="E39" s="67"/>
+      <c r="F39" s="67"/>
+      <c r="G39" s="68"/>
+      <c r="H39" s="67"/>
+      <c r="I39" s="66"/>
+      <c r="J39" s="67"/>
+      <c r="K39" s="66"/>
+      <c r="L39" s="66"/>
+      <c r="M39" s="66"/>
+      <c r="N39" s="66"/>
+      <c r="O39" s="67"/>
+      <c r="P39" s="69"/>
+      <c r="Q39" s="69"/>
+      <c r="R39" s="69"/>
+      <c r="S39" s="69"/>
+      <c r="T39" s="69"/>
+      <c r="U39" s="69"/>
+      <c r="V39" s="69" t="s">
         <v>269</v>
       </c>
       <c r="W39" s="16" t="s">
@@ -4602,820 +4626,820 @@
       </c>
     </row>
     <row r="40" spans="1:24" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A40" s="71"/>
-      <c r="B40" s="72"/>
-      <c r="C40" s="72"/>
-      <c r="D40" s="72"/>
-      <c r="E40" s="72"/>
-      <c r="F40" s="72"/>
-      <c r="G40" s="73"/>
-      <c r="H40" s="72"/>
-      <c r="I40" s="71"/>
-      <c r="J40" s="72"/>
-      <c r="K40" s="71"/>
-      <c r="L40" s="71"/>
-      <c r="M40" s="71"/>
-      <c r="N40" s="71"/>
-      <c r="O40" s="72"/>
-      <c r="P40" s="74"/>
-      <c r="Q40" s="74"/>
-      <c r="R40" s="74"/>
-      <c r="S40" s="74"/>
-      <c r="T40" s="74"/>
-      <c r="U40" s="74"/>
-      <c r="V40" s="72"/>
+      <c r="A40" s="66"/>
+      <c r="B40" s="67"/>
+      <c r="C40" s="67"/>
+      <c r="D40" s="67"/>
+      <c r="E40" s="67"/>
+      <c r="F40" s="67"/>
+      <c r="G40" s="68"/>
+      <c r="H40" s="67"/>
+      <c r="I40" s="66"/>
+      <c r="J40" s="67"/>
+      <c r="K40" s="66"/>
+      <c r="L40" s="66"/>
+      <c r="M40" s="66"/>
+      <c r="N40" s="66"/>
+      <c r="O40" s="67"/>
+      <c r="P40" s="69"/>
+      <c r="Q40" s="69"/>
+      <c r="R40" s="69"/>
+      <c r="S40" s="69"/>
+      <c r="T40" s="69"/>
+      <c r="U40" s="69"/>
+      <c r="V40" s="67"/>
     </row>
     <row r="41" spans="1:24" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A41" s="71"/>
-      <c r="B41" s="72"/>
-      <c r="C41" s="72"/>
-      <c r="D41" s="72"/>
-      <c r="E41" s="72"/>
-      <c r="F41" s="72"/>
-      <c r="G41" s="73"/>
-      <c r="H41" s="72"/>
-      <c r="I41" s="71"/>
-      <c r="J41" s="72"/>
-      <c r="K41" s="71"/>
-      <c r="L41" s="71"/>
-      <c r="M41" s="71"/>
-      <c r="N41" s="71"/>
-      <c r="O41" s="72"/>
-      <c r="P41" s="74"/>
-      <c r="Q41" s="74"/>
-      <c r="R41" s="74"/>
-      <c r="S41" s="74"/>
-      <c r="T41" s="74"/>
-      <c r="U41" s="74"/>
-      <c r="V41" s="72"/>
+      <c r="A41" s="66"/>
+      <c r="B41" s="67"/>
+      <c r="C41" s="67"/>
+      <c r="D41" s="67"/>
+      <c r="E41" s="67"/>
+      <c r="F41" s="67"/>
+      <c r="G41" s="68"/>
+      <c r="H41" s="67"/>
+      <c r="I41" s="66"/>
+      <c r="J41" s="67"/>
+      <c r="K41" s="66"/>
+      <c r="L41" s="66"/>
+      <c r="M41" s="66"/>
+      <c r="N41" s="66"/>
+      <c r="O41" s="67"/>
+      <c r="P41" s="69"/>
+      <c r="Q41" s="69"/>
+      <c r="R41" s="69"/>
+      <c r="S41" s="69"/>
+      <c r="T41" s="69"/>
+      <c r="U41" s="69"/>
+      <c r="V41" s="67"/>
     </row>
     <row r="42" spans="1:24" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A42" s="71"/>
-      <c r="B42" s="72"/>
-      <c r="C42" s="72"/>
-      <c r="D42" s="72"/>
-      <c r="E42" s="72"/>
-      <c r="F42" s="72"/>
-      <c r="G42" s="73"/>
-      <c r="H42" s="72"/>
-      <c r="I42" s="71"/>
-      <c r="J42" s="72"/>
-      <c r="K42" s="71"/>
-      <c r="L42" s="71"/>
-      <c r="M42" s="71"/>
-      <c r="N42" s="71"/>
-      <c r="O42" s="72"/>
-      <c r="P42" s="74"/>
-      <c r="Q42" s="74"/>
-      <c r="R42" s="74"/>
-      <c r="S42" s="74"/>
-      <c r="T42" s="74"/>
-      <c r="U42" s="74"/>
-      <c r="V42" s="72"/>
+      <c r="A42" s="66"/>
+      <c r="B42" s="67"/>
+      <c r="C42" s="67"/>
+      <c r="D42" s="67"/>
+      <c r="E42" s="67"/>
+      <c r="F42" s="67"/>
+      <c r="G42" s="68"/>
+      <c r="H42" s="67"/>
+      <c r="I42" s="66"/>
+      <c r="J42" s="67"/>
+      <c r="K42" s="66"/>
+      <c r="L42" s="66"/>
+      <c r="M42" s="66"/>
+      <c r="N42" s="66"/>
+      <c r="O42" s="67"/>
+      <c r="P42" s="69"/>
+      <c r="Q42" s="69"/>
+      <c r="R42" s="69"/>
+      <c r="S42" s="69"/>
+      <c r="T42" s="69"/>
+      <c r="U42" s="69"/>
+      <c r="V42" s="67"/>
     </row>
     <row r="43" spans="1:24" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A43" s="71"/>
-      <c r="B43" s="72"/>
-      <c r="C43" s="72"/>
-      <c r="D43" s="72"/>
-      <c r="E43" s="72"/>
-      <c r="F43" s="72"/>
-      <c r="G43" s="73"/>
-      <c r="H43" s="72"/>
-      <c r="I43" s="71"/>
-      <c r="J43" s="72"/>
-      <c r="K43" s="71"/>
-      <c r="L43" s="71"/>
-      <c r="M43" s="71"/>
-      <c r="N43" s="71"/>
-      <c r="O43" s="72"/>
-      <c r="P43" s="74"/>
-      <c r="Q43" s="74"/>
-      <c r="R43" s="74"/>
-      <c r="S43" s="74"/>
-      <c r="T43" s="74"/>
-      <c r="U43" s="74"/>
-      <c r="V43" s="72"/>
+      <c r="A43" s="66"/>
+      <c r="B43" s="67"/>
+      <c r="C43" s="67"/>
+      <c r="D43" s="67"/>
+      <c r="E43" s="67"/>
+      <c r="F43" s="67"/>
+      <c r="G43" s="68"/>
+      <c r="H43" s="67"/>
+      <c r="I43" s="66"/>
+      <c r="J43" s="67"/>
+      <c r="K43" s="66"/>
+      <c r="L43" s="66"/>
+      <c r="M43" s="66"/>
+      <c r="N43" s="66"/>
+      <c r="O43" s="67"/>
+      <c r="P43" s="69"/>
+      <c r="Q43" s="69"/>
+      <c r="R43" s="69"/>
+      <c r="S43" s="69"/>
+      <c r="T43" s="69"/>
+      <c r="U43" s="69"/>
+      <c r="V43" s="67"/>
     </row>
     <row r="44" spans="1:24" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A44" s="71"/>
-      <c r="B44" s="72"/>
-      <c r="C44" s="72"/>
-      <c r="D44" s="72"/>
-      <c r="E44" s="72"/>
-      <c r="F44" s="72"/>
-      <c r="G44" s="73"/>
-      <c r="H44" s="72"/>
-      <c r="I44" s="71"/>
-      <c r="J44" s="72"/>
-      <c r="K44" s="71"/>
-      <c r="L44" s="71"/>
-      <c r="M44" s="71"/>
-      <c r="N44" s="71"/>
-      <c r="O44" s="72"/>
-      <c r="P44" s="74"/>
-      <c r="Q44" s="74"/>
-      <c r="R44" s="74"/>
-      <c r="S44" s="74"/>
-      <c r="T44" s="74"/>
-      <c r="U44" s="74"/>
-      <c r="V44" s="72"/>
+      <c r="A44" s="66"/>
+      <c r="B44" s="67"/>
+      <c r="C44" s="67"/>
+      <c r="D44" s="67"/>
+      <c r="E44" s="67"/>
+      <c r="F44" s="67"/>
+      <c r="G44" s="68"/>
+      <c r="H44" s="67"/>
+      <c r="I44" s="66"/>
+      <c r="J44" s="67"/>
+      <c r="K44" s="66"/>
+      <c r="L44" s="66"/>
+      <c r="M44" s="66"/>
+      <c r="N44" s="66"/>
+      <c r="O44" s="67"/>
+      <c r="P44" s="69"/>
+      <c r="Q44" s="69"/>
+      <c r="R44" s="69"/>
+      <c r="S44" s="69"/>
+      <c r="T44" s="69"/>
+      <c r="U44" s="69"/>
+      <c r="V44" s="67"/>
     </row>
     <row r="45" spans="1:24" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A45" s="71"/>
-      <c r="B45" s="72"/>
-      <c r="C45" s="72"/>
-      <c r="D45" s="72"/>
-      <c r="E45" s="72"/>
-      <c r="F45" s="72"/>
-      <c r="G45" s="73"/>
-      <c r="H45" s="72"/>
-      <c r="I45" s="71"/>
-      <c r="J45" s="72"/>
-      <c r="K45" s="71"/>
-      <c r="L45" s="71"/>
-      <c r="M45" s="71"/>
-      <c r="N45" s="71"/>
-      <c r="O45" s="72"/>
-      <c r="P45" s="74"/>
-      <c r="Q45" s="74"/>
-      <c r="R45" s="74"/>
-      <c r="S45" s="74"/>
-      <c r="T45" s="74"/>
-      <c r="U45" s="74"/>
-      <c r="V45" s="72"/>
+      <c r="A45" s="66"/>
+      <c r="B45" s="67"/>
+      <c r="C45" s="67"/>
+      <c r="D45" s="67"/>
+      <c r="E45" s="67"/>
+      <c r="F45" s="67"/>
+      <c r="G45" s="68"/>
+      <c r="H45" s="67"/>
+      <c r="I45" s="66"/>
+      <c r="J45" s="67"/>
+      <c r="K45" s="66"/>
+      <c r="L45" s="66"/>
+      <c r="M45" s="66"/>
+      <c r="N45" s="66"/>
+      <c r="O45" s="67"/>
+      <c r="P45" s="69"/>
+      <c r="Q45" s="69"/>
+      <c r="R45" s="69"/>
+      <c r="S45" s="69"/>
+      <c r="T45" s="69"/>
+      <c r="U45" s="69"/>
+      <c r="V45" s="67"/>
     </row>
     <row r="46" spans="1:24" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A46" s="71"/>
-      <c r="B46" s="72"/>
-      <c r="C46" s="72"/>
-      <c r="D46" s="72"/>
-      <c r="E46" s="72"/>
-      <c r="F46" s="72"/>
-      <c r="G46" s="73"/>
-      <c r="H46" s="72"/>
-      <c r="I46" s="71"/>
-      <c r="J46" s="72"/>
-      <c r="K46" s="71"/>
-      <c r="L46" s="71"/>
-      <c r="M46" s="71"/>
-      <c r="N46" s="71"/>
-      <c r="O46" s="72"/>
-      <c r="P46" s="74"/>
-      <c r="Q46" s="74"/>
-      <c r="R46" s="74"/>
-      <c r="S46" s="74"/>
-      <c r="T46" s="74"/>
-      <c r="U46" s="74"/>
-      <c r="V46" s="72"/>
+      <c r="A46" s="66"/>
+      <c r="B46" s="67"/>
+      <c r="C46" s="67"/>
+      <c r="D46" s="67"/>
+      <c r="E46" s="67"/>
+      <c r="F46" s="67"/>
+      <c r="G46" s="68"/>
+      <c r="H46" s="67"/>
+      <c r="I46" s="66"/>
+      <c r="J46" s="67"/>
+      <c r="K46" s="66"/>
+      <c r="L46" s="66"/>
+      <c r="M46" s="66"/>
+      <c r="N46" s="66"/>
+      <c r="O46" s="67"/>
+      <c r="P46" s="69"/>
+      <c r="Q46" s="69"/>
+      <c r="R46" s="69"/>
+      <c r="S46" s="69"/>
+      <c r="T46" s="69"/>
+      <c r="U46" s="69"/>
+      <c r="V46" s="67"/>
     </row>
     <row r="47" spans="1:24" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A47" s="71"/>
-      <c r="B47" s="72"/>
-      <c r="C47" s="72"/>
-      <c r="D47" s="72"/>
-      <c r="E47" s="72"/>
-      <c r="F47" s="72"/>
-      <c r="G47" s="73"/>
-      <c r="H47" s="72"/>
-      <c r="I47" s="71"/>
-      <c r="J47" s="72"/>
-      <c r="K47" s="71"/>
-      <c r="L47" s="71"/>
-      <c r="M47" s="71"/>
-      <c r="N47" s="71"/>
-      <c r="O47" s="72"/>
-      <c r="P47" s="74"/>
-      <c r="Q47" s="74"/>
-      <c r="R47" s="74"/>
-      <c r="S47" s="74"/>
-      <c r="T47" s="74"/>
-      <c r="U47" s="74"/>
-      <c r="V47" s="72"/>
+      <c r="A47" s="66"/>
+      <c r="B47" s="67"/>
+      <c r="C47" s="67"/>
+      <c r="D47" s="67"/>
+      <c r="E47" s="67"/>
+      <c r="F47" s="67"/>
+      <c r="G47" s="68"/>
+      <c r="H47" s="67"/>
+      <c r="I47" s="66"/>
+      <c r="J47" s="67"/>
+      <c r="K47" s="66"/>
+      <c r="L47" s="66"/>
+      <c r="M47" s="66"/>
+      <c r="N47" s="66"/>
+      <c r="O47" s="67"/>
+      <c r="P47" s="69"/>
+      <c r="Q47" s="69"/>
+      <c r="R47" s="69"/>
+      <c r="S47" s="69"/>
+      <c r="T47" s="69"/>
+      <c r="U47" s="69"/>
+      <c r="V47" s="67"/>
     </row>
     <row r="48" spans="1:24" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A48" s="71"/>
-      <c r="B48" s="72"/>
-      <c r="C48" s="72"/>
-      <c r="D48" s="72"/>
-      <c r="E48" s="72"/>
-      <c r="F48" s="72"/>
-      <c r="G48" s="73"/>
-      <c r="H48" s="72"/>
-      <c r="I48" s="71"/>
-      <c r="J48" s="72"/>
-      <c r="K48" s="71"/>
-      <c r="L48" s="71"/>
-      <c r="M48" s="71"/>
-      <c r="N48" s="71"/>
-      <c r="O48" s="72"/>
-      <c r="P48" s="74"/>
-      <c r="Q48" s="74"/>
-      <c r="R48" s="74"/>
-      <c r="S48" s="74"/>
-      <c r="T48" s="74"/>
-      <c r="U48" s="74"/>
-      <c r="V48" s="72"/>
+      <c r="A48" s="66"/>
+      <c r="B48" s="67"/>
+      <c r="C48" s="67"/>
+      <c r="D48" s="67"/>
+      <c r="E48" s="67"/>
+      <c r="F48" s="67"/>
+      <c r="G48" s="68"/>
+      <c r="H48" s="67"/>
+      <c r="I48" s="66"/>
+      <c r="J48" s="67"/>
+      <c r="K48" s="66"/>
+      <c r="L48" s="66"/>
+      <c r="M48" s="66"/>
+      <c r="N48" s="66"/>
+      <c r="O48" s="67"/>
+      <c r="P48" s="69"/>
+      <c r="Q48" s="69"/>
+      <c r="R48" s="69"/>
+      <c r="S48" s="69"/>
+      <c r="T48" s="69"/>
+      <c r="U48" s="69"/>
+      <c r="V48" s="67"/>
     </row>
     <row r="49" spans="1:22" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A49" s="71"/>
-      <c r="B49" s="72"/>
-      <c r="C49" s="72"/>
-      <c r="D49" s="72"/>
-      <c r="E49" s="72"/>
-      <c r="F49" s="72"/>
-      <c r="G49" s="73"/>
-      <c r="H49" s="72"/>
-      <c r="I49" s="71"/>
-      <c r="J49" s="72"/>
-      <c r="K49" s="71"/>
-      <c r="L49" s="71"/>
-      <c r="M49" s="71"/>
-      <c r="N49" s="71"/>
-      <c r="O49" s="72"/>
-      <c r="P49" s="74"/>
-      <c r="Q49" s="74"/>
-      <c r="R49" s="74"/>
-      <c r="S49" s="74"/>
-      <c r="T49" s="74"/>
-      <c r="U49" s="74"/>
-      <c r="V49" s="72"/>
+      <c r="A49" s="66"/>
+      <c r="B49" s="67"/>
+      <c r="C49" s="67"/>
+      <c r="D49" s="67"/>
+      <c r="E49" s="67"/>
+      <c r="F49" s="67"/>
+      <c r="G49" s="68"/>
+      <c r="H49" s="67"/>
+      <c r="I49" s="66"/>
+      <c r="J49" s="67"/>
+      <c r="K49" s="66"/>
+      <c r="L49" s="66"/>
+      <c r="M49" s="66"/>
+      <c r="N49" s="66"/>
+      <c r="O49" s="67"/>
+      <c r="P49" s="69"/>
+      <c r="Q49" s="69"/>
+      <c r="R49" s="69"/>
+      <c r="S49" s="69"/>
+      <c r="T49" s="69"/>
+      <c r="U49" s="69"/>
+      <c r="V49" s="67"/>
     </row>
     <row r="50" spans="1:22" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A50" s="71"/>
-      <c r="B50" s="72"/>
-      <c r="C50" s="72"/>
-      <c r="D50" s="72"/>
-      <c r="E50" s="72"/>
-      <c r="F50" s="72"/>
-      <c r="G50" s="73"/>
-      <c r="H50" s="72"/>
-      <c r="I50" s="71"/>
-      <c r="J50" s="72"/>
-      <c r="K50" s="71"/>
-      <c r="L50" s="71"/>
-      <c r="M50" s="71"/>
-      <c r="N50" s="71"/>
-      <c r="O50" s="72"/>
-      <c r="P50" s="74"/>
-      <c r="Q50" s="74"/>
-      <c r="R50" s="74"/>
-      <c r="S50" s="74"/>
-      <c r="T50" s="74"/>
-      <c r="U50" s="74"/>
-      <c r="V50" s="72"/>
+      <c r="A50" s="66"/>
+      <c r="B50" s="67"/>
+      <c r="C50" s="67"/>
+      <c r="D50" s="67"/>
+      <c r="E50" s="67"/>
+      <c r="F50" s="67"/>
+      <c r="G50" s="68"/>
+      <c r="H50" s="67"/>
+      <c r="I50" s="66"/>
+      <c r="J50" s="67"/>
+      <c r="K50" s="66"/>
+      <c r="L50" s="66"/>
+      <c r="M50" s="66"/>
+      <c r="N50" s="66"/>
+      <c r="O50" s="67"/>
+      <c r="P50" s="69"/>
+      <c r="Q50" s="69"/>
+      <c r="R50" s="69"/>
+      <c r="S50" s="69"/>
+      <c r="T50" s="69"/>
+      <c r="U50" s="69"/>
+      <c r="V50" s="67"/>
     </row>
     <row r="51" spans="1:22" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A51" s="71"/>
-      <c r="B51" s="72"/>
-      <c r="C51" s="72"/>
-      <c r="D51" s="72"/>
-      <c r="E51" s="72"/>
-      <c r="F51" s="72"/>
-      <c r="G51" s="73"/>
-      <c r="H51" s="72"/>
-      <c r="I51" s="71"/>
-      <c r="J51" s="72"/>
-      <c r="K51" s="71"/>
-      <c r="L51" s="71"/>
-      <c r="M51" s="71"/>
-      <c r="N51" s="71"/>
-      <c r="O51" s="72"/>
-      <c r="P51" s="74"/>
-      <c r="Q51" s="74"/>
-      <c r="R51" s="74"/>
-      <c r="S51" s="74"/>
-      <c r="T51" s="74"/>
-      <c r="U51" s="74"/>
-      <c r="V51" s="72"/>
+      <c r="A51" s="66"/>
+      <c r="B51" s="67"/>
+      <c r="C51" s="67"/>
+      <c r="D51" s="67"/>
+      <c r="E51" s="67"/>
+      <c r="F51" s="67"/>
+      <c r="G51" s="68"/>
+      <c r="H51" s="67"/>
+      <c r="I51" s="66"/>
+      <c r="J51" s="67"/>
+      <c r="K51" s="66"/>
+      <c r="L51" s="66"/>
+      <c r="M51" s="66"/>
+      <c r="N51" s="66"/>
+      <c r="O51" s="67"/>
+      <c r="P51" s="69"/>
+      <c r="Q51" s="69"/>
+      <c r="R51" s="69"/>
+      <c r="S51" s="69"/>
+      <c r="T51" s="69"/>
+      <c r="U51" s="69"/>
+      <c r="V51" s="67"/>
     </row>
     <row r="52" spans="1:22" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A52" s="71"/>
-      <c r="B52" s="72"/>
-      <c r="C52" s="72"/>
-      <c r="D52" s="72"/>
-      <c r="E52" s="72"/>
-      <c r="F52" s="72"/>
-      <c r="G52" s="73"/>
-      <c r="H52" s="72"/>
-      <c r="I52" s="71"/>
-      <c r="J52" s="72"/>
-      <c r="K52" s="71"/>
-      <c r="L52" s="71"/>
-      <c r="M52" s="71"/>
-      <c r="N52" s="71"/>
-      <c r="O52" s="72"/>
-      <c r="P52" s="74"/>
-      <c r="Q52" s="74"/>
-      <c r="R52" s="74"/>
-      <c r="S52" s="74"/>
-      <c r="T52" s="74"/>
-      <c r="U52" s="74"/>
-      <c r="V52" s="72"/>
+      <c r="A52" s="66"/>
+      <c r="B52" s="67"/>
+      <c r="C52" s="67"/>
+      <c r="D52" s="67"/>
+      <c r="E52" s="67"/>
+      <c r="F52" s="67"/>
+      <c r="G52" s="68"/>
+      <c r="H52" s="67"/>
+      <c r="I52" s="66"/>
+      <c r="J52" s="67"/>
+      <c r="K52" s="66"/>
+      <c r="L52" s="66"/>
+      <c r="M52" s="66"/>
+      <c r="N52" s="66"/>
+      <c r="O52" s="67"/>
+      <c r="P52" s="69"/>
+      <c r="Q52" s="69"/>
+      <c r="R52" s="69"/>
+      <c r="S52" s="69"/>
+      <c r="T52" s="69"/>
+      <c r="U52" s="69"/>
+      <c r="V52" s="67"/>
     </row>
     <row r="53" spans="1:22" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A53" s="71"/>
-      <c r="B53" s="72"/>
-      <c r="C53" s="72"/>
-      <c r="D53" s="72"/>
-      <c r="E53" s="72"/>
-      <c r="F53" s="72"/>
-      <c r="G53" s="73"/>
-      <c r="H53" s="72"/>
-      <c r="I53" s="71"/>
-      <c r="J53" s="72"/>
-      <c r="K53" s="71"/>
-      <c r="L53" s="71"/>
-      <c r="M53" s="71"/>
-      <c r="N53" s="71"/>
-      <c r="O53" s="72"/>
-      <c r="P53" s="74"/>
-      <c r="Q53" s="74"/>
-      <c r="R53" s="74"/>
-      <c r="S53" s="74"/>
-      <c r="T53" s="74"/>
-      <c r="U53" s="74"/>
-      <c r="V53" s="72"/>
+      <c r="A53" s="66"/>
+      <c r="B53" s="67"/>
+      <c r="C53" s="67"/>
+      <c r="D53" s="67"/>
+      <c r="E53" s="67"/>
+      <c r="F53" s="67"/>
+      <c r="G53" s="68"/>
+      <c r="H53" s="67"/>
+      <c r="I53" s="66"/>
+      <c r="J53" s="67"/>
+      <c r="K53" s="66"/>
+      <c r="L53" s="66"/>
+      <c r="M53" s="66"/>
+      <c r="N53" s="66"/>
+      <c r="O53" s="67"/>
+      <c r="P53" s="69"/>
+      <c r="Q53" s="69"/>
+      <c r="R53" s="69"/>
+      <c r="S53" s="69"/>
+      <c r="T53" s="69"/>
+      <c r="U53" s="69"/>
+      <c r="V53" s="67"/>
     </row>
     <row r="54" spans="1:22" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A54" s="71"/>
-      <c r="B54" s="72"/>
-      <c r="C54" s="72"/>
-      <c r="D54" s="72"/>
-      <c r="E54" s="72"/>
-      <c r="F54" s="72"/>
-      <c r="G54" s="73"/>
-      <c r="H54" s="72"/>
-      <c r="I54" s="71"/>
-      <c r="J54" s="72"/>
-      <c r="K54" s="71"/>
-      <c r="L54" s="71"/>
-      <c r="M54" s="71"/>
-      <c r="N54" s="71"/>
-      <c r="O54" s="72"/>
-      <c r="P54" s="74"/>
-      <c r="Q54" s="74"/>
-      <c r="R54" s="74"/>
-      <c r="S54" s="74"/>
-      <c r="T54" s="74"/>
-      <c r="U54" s="74"/>
-      <c r="V54" s="72"/>
+      <c r="A54" s="66"/>
+      <c r="B54" s="67"/>
+      <c r="C54" s="67"/>
+      <c r="D54" s="67"/>
+      <c r="E54" s="67"/>
+      <c r="F54" s="67"/>
+      <c r="G54" s="68"/>
+      <c r="H54" s="67"/>
+      <c r="I54" s="66"/>
+      <c r="J54" s="67"/>
+      <c r="K54" s="66"/>
+      <c r="L54" s="66"/>
+      <c r="M54" s="66"/>
+      <c r="N54" s="66"/>
+      <c r="O54" s="67"/>
+      <c r="P54" s="69"/>
+      <c r="Q54" s="69"/>
+      <c r="R54" s="69"/>
+      <c r="S54" s="69"/>
+      <c r="T54" s="69"/>
+      <c r="U54" s="69"/>
+      <c r="V54" s="67"/>
     </row>
     <row r="55" spans="1:22" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A55" s="71"/>
-      <c r="B55" s="72"/>
-      <c r="C55" s="72"/>
-      <c r="D55" s="72"/>
-      <c r="E55" s="72"/>
-      <c r="F55" s="72"/>
-      <c r="G55" s="73"/>
-      <c r="H55" s="72"/>
-      <c r="I55" s="71"/>
-      <c r="J55" s="72"/>
-      <c r="K55" s="71"/>
-      <c r="L55" s="71"/>
-      <c r="M55" s="71"/>
-      <c r="N55" s="71"/>
-      <c r="O55" s="72"/>
-      <c r="P55" s="74"/>
-      <c r="Q55" s="74"/>
-      <c r="R55" s="74"/>
-      <c r="S55" s="74"/>
-      <c r="T55" s="74"/>
-      <c r="U55" s="74"/>
-      <c r="V55" s="72"/>
+      <c r="A55" s="66"/>
+      <c r="B55" s="67"/>
+      <c r="C55" s="67"/>
+      <c r="D55" s="67"/>
+      <c r="E55" s="67"/>
+      <c r="F55" s="67"/>
+      <c r="G55" s="68"/>
+      <c r="H55" s="67"/>
+      <c r="I55" s="66"/>
+      <c r="J55" s="67"/>
+      <c r="K55" s="66"/>
+      <c r="L55" s="66"/>
+      <c r="M55" s="66"/>
+      <c r="N55" s="66"/>
+      <c r="O55" s="67"/>
+      <c r="P55" s="69"/>
+      <c r="Q55" s="69"/>
+      <c r="R55" s="69"/>
+      <c r="S55" s="69"/>
+      <c r="T55" s="69"/>
+      <c r="U55" s="69"/>
+      <c r="V55" s="67"/>
     </row>
     <row r="56" spans="1:22" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A56" s="71"/>
-      <c r="B56" s="72"/>
-      <c r="C56" s="72"/>
-      <c r="D56" s="72"/>
-      <c r="E56" s="72"/>
-      <c r="F56" s="72"/>
-      <c r="G56" s="73"/>
-      <c r="H56" s="72"/>
-      <c r="I56" s="71"/>
-      <c r="J56" s="72"/>
-      <c r="K56" s="71"/>
-      <c r="L56" s="71"/>
-      <c r="M56" s="71"/>
-      <c r="N56" s="71"/>
-      <c r="O56" s="72"/>
-      <c r="P56" s="74"/>
-      <c r="Q56" s="74"/>
-      <c r="R56" s="74"/>
-      <c r="S56" s="74"/>
-      <c r="T56" s="74"/>
-      <c r="U56" s="74"/>
-      <c r="V56" s="72"/>
+      <c r="A56" s="66"/>
+      <c r="B56" s="67"/>
+      <c r="C56" s="67"/>
+      <c r="D56" s="67"/>
+      <c r="E56" s="67"/>
+      <c r="F56" s="67"/>
+      <c r="G56" s="68"/>
+      <c r="H56" s="67"/>
+      <c r="I56" s="66"/>
+      <c r="J56" s="67"/>
+      <c r="K56" s="66"/>
+      <c r="L56" s="66"/>
+      <c r="M56" s="66"/>
+      <c r="N56" s="66"/>
+      <c r="O56" s="67"/>
+      <c r="P56" s="69"/>
+      <c r="Q56" s="69"/>
+      <c r="R56" s="69"/>
+      <c r="S56" s="69"/>
+      <c r="T56" s="69"/>
+      <c r="U56" s="69"/>
+      <c r="V56" s="67"/>
     </row>
     <row r="57" spans="1:22" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A57" s="71"/>
-      <c r="B57" s="72"/>
-      <c r="C57" s="72"/>
-      <c r="D57" s="72"/>
-      <c r="E57" s="72"/>
-      <c r="F57" s="72"/>
-      <c r="G57" s="73"/>
-      <c r="H57" s="72"/>
-      <c r="I57" s="71"/>
-      <c r="J57" s="72"/>
-      <c r="K57" s="71"/>
-      <c r="L57" s="71"/>
-      <c r="M57" s="71"/>
-      <c r="N57" s="71"/>
-      <c r="O57" s="72"/>
-      <c r="P57" s="74"/>
-      <c r="Q57" s="74"/>
-      <c r="R57" s="74"/>
-      <c r="S57" s="74"/>
-      <c r="T57" s="74"/>
-      <c r="U57" s="74"/>
-      <c r="V57" s="72"/>
+      <c r="A57" s="66"/>
+      <c r="B57" s="67"/>
+      <c r="C57" s="67"/>
+      <c r="D57" s="67"/>
+      <c r="E57" s="67"/>
+      <c r="F57" s="67"/>
+      <c r="G57" s="68"/>
+      <c r="H57" s="67"/>
+      <c r="I57" s="66"/>
+      <c r="J57" s="67"/>
+      <c r="K57" s="66"/>
+      <c r="L57" s="66"/>
+      <c r="M57" s="66"/>
+      <c r="N57" s="66"/>
+      <c r="O57" s="67"/>
+      <c r="P57" s="69"/>
+      <c r="Q57" s="69"/>
+      <c r="R57" s="69"/>
+      <c r="S57" s="69"/>
+      <c r="T57" s="69"/>
+      <c r="U57" s="69"/>
+      <c r="V57" s="67"/>
     </row>
     <row r="58" spans="1:22" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A58" s="71"/>
-      <c r="B58" s="72"/>
-      <c r="C58" s="72"/>
-      <c r="D58" s="72"/>
-      <c r="E58" s="72"/>
-      <c r="F58" s="72"/>
-      <c r="G58" s="73"/>
-      <c r="H58" s="72"/>
-      <c r="I58" s="71"/>
-      <c r="J58" s="72"/>
-      <c r="K58" s="71"/>
-      <c r="L58" s="71"/>
-      <c r="M58" s="71"/>
-      <c r="N58" s="71"/>
-      <c r="O58" s="72"/>
-      <c r="P58" s="74"/>
-      <c r="Q58" s="74"/>
-      <c r="R58" s="74"/>
-      <c r="S58" s="74"/>
-      <c r="T58" s="74"/>
-      <c r="U58" s="74"/>
-      <c r="V58" s="72"/>
+      <c r="A58" s="66"/>
+      <c r="B58" s="67"/>
+      <c r="C58" s="67"/>
+      <c r="D58" s="67"/>
+      <c r="E58" s="67"/>
+      <c r="F58" s="67"/>
+      <c r="G58" s="68"/>
+      <c r="H58" s="67"/>
+      <c r="I58" s="66"/>
+      <c r="J58" s="67"/>
+      <c r="K58" s="66"/>
+      <c r="L58" s="66"/>
+      <c r="M58" s="66"/>
+      <c r="N58" s="66"/>
+      <c r="O58" s="67"/>
+      <c r="P58" s="69"/>
+      <c r="Q58" s="69"/>
+      <c r="R58" s="69"/>
+      <c r="S58" s="69"/>
+      <c r="T58" s="69"/>
+      <c r="U58" s="69"/>
+      <c r="V58" s="67"/>
     </row>
     <row r="59" spans="1:22" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A59" s="71"/>
-      <c r="B59" s="72"/>
-      <c r="C59" s="72"/>
-      <c r="D59" s="72"/>
-      <c r="E59" s="72"/>
-      <c r="F59" s="72"/>
-      <c r="G59" s="73"/>
-      <c r="H59" s="72"/>
-      <c r="I59" s="71"/>
-      <c r="J59" s="72"/>
-      <c r="K59" s="71"/>
-      <c r="L59" s="71"/>
-      <c r="M59" s="71"/>
-      <c r="N59" s="71"/>
-      <c r="O59" s="72"/>
-      <c r="P59" s="74"/>
-      <c r="Q59" s="74"/>
-      <c r="R59" s="74"/>
-      <c r="S59" s="74"/>
-      <c r="T59" s="74"/>
-      <c r="U59" s="74"/>
-      <c r="V59" s="72"/>
+      <c r="A59" s="66"/>
+      <c r="B59" s="67"/>
+      <c r="C59" s="67"/>
+      <c r="D59" s="67"/>
+      <c r="E59" s="67"/>
+      <c r="F59" s="67"/>
+      <c r="G59" s="68"/>
+      <c r="H59" s="67"/>
+      <c r="I59" s="66"/>
+      <c r="J59" s="67"/>
+      <c r="K59" s="66"/>
+      <c r="L59" s="66"/>
+      <c r="M59" s="66"/>
+      <c r="N59" s="66"/>
+      <c r="O59" s="67"/>
+      <c r="P59" s="69"/>
+      <c r="Q59" s="69"/>
+      <c r="R59" s="69"/>
+      <c r="S59" s="69"/>
+      <c r="T59" s="69"/>
+      <c r="U59" s="69"/>
+      <c r="V59" s="67"/>
     </row>
     <row r="60" spans="1:22" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A60" s="71"/>
-      <c r="B60" s="72"/>
-      <c r="C60" s="72"/>
-      <c r="D60" s="72"/>
-      <c r="E60" s="72"/>
-      <c r="F60" s="72"/>
-      <c r="G60" s="73"/>
-      <c r="H60" s="72"/>
-      <c r="I60" s="71"/>
-      <c r="J60" s="72"/>
-      <c r="K60" s="71"/>
-      <c r="L60" s="71"/>
-      <c r="M60" s="71"/>
-      <c r="N60" s="71"/>
-      <c r="O60" s="72"/>
-      <c r="P60" s="74"/>
-      <c r="Q60" s="74"/>
-      <c r="R60" s="74"/>
-      <c r="S60" s="74"/>
-      <c r="T60" s="74"/>
-      <c r="U60" s="74"/>
-      <c r="V60" s="72"/>
+      <c r="A60" s="66"/>
+      <c r="B60" s="67"/>
+      <c r="C60" s="67"/>
+      <c r="D60" s="67"/>
+      <c r="E60" s="67"/>
+      <c r="F60" s="67"/>
+      <c r="G60" s="68"/>
+      <c r="H60" s="67"/>
+      <c r="I60" s="66"/>
+      <c r="J60" s="67"/>
+      <c r="K60" s="66"/>
+      <c r="L60" s="66"/>
+      <c r="M60" s="66"/>
+      <c r="N60" s="66"/>
+      <c r="O60" s="67"/>
+      <c r="P60" s="69"/>
+      <c r="Q60" s="69"/>
+      <c r="R60" s="69"/>
+      <c r="S60" s="69"/>
+      <c r="T60" s="69"/>
+      <c r="U60" s="69"/>
+      <c r="V60" s="67"/>
     </row>
     <row r="61" spans="1:22" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A61" s="71"/>
-      <c r="B61" s="72"/>
-      <c r="C61" s="72"/>
-      <c r="D61" s="72"/>
-      <c r="E61" s="72"/>
-      <c r="F61" s="72"/>
-      <c r="G61" s="73"/>
-      <c r="H61" s="72"/>
-      <c r="I61" s="71"/>
-      <c r="J61" s="72"/>
-      <c r="K61" s="71"/>
-      <c r="L61" s="71"/>
-      <c r="M61" s="71"/>
-      <c r="N61" s="71"/>
-      <c r="O61" s="72"/>
-      <c r="P61" s="74"/>
-      <c r="Q61" s="74"/>
-      <c r="R61" s="74"/>
-      <c r="S61" s="74"/>
-      <c r="T61" s="74"/>
-      <c r="U61" s="74"/>
-      <c r="V61" s="72"/>
+      <c r="A61" s="66"/>
+      <c r="B61" s="67"/>
+      <c r="C61" s="67"/>
+      <c r="D61" s="67"/>
+      <c r="E61" s="67"/>
+      <c r="F61" s="67"/>
+      <c r="G61" s="68"/>
+      <c r="H61" s="67"/>
+      <c r="I61" s="66"/>
+      <c r="J61" s="67"/>
+      <c r="K61" s="66"/>
+      <c r="L61" s="66"/>
+      <c r="M61" s="66"/>
+      <c r="N61" s="66"/>
+      <c r="O61" s="67"/>
+      <c r="P61" s="69"/>
+      <c r="Q61" s="69"/>
+      <c r="R61" s="69"/>
+      <c r="S61" s="69"/>
+      <c r="T61" s="69"/>
+      <c r="U61" s="69"/>
+      <c r="V61" s="67"/>
     </row>
     <row r="62" spans="1:22" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A62" s="71"/>
-      <c r="B62" s="72"/>
-      <c r="C62" s="72"/>
-      <c r="D62" s="72"/>
-      <c r="E62" s="72"/>
-      <c r="F62" s="72"/>
-      <c r="G62" s="73"/>
-      <c r="H62" s="72"/>
-      <c r="I62" s="71"/>
-      <c r="J62" s="72"/>
-      <c r="K62" s="71"/>
-      <c r="L62" s="71"/>
-      <c r="M62" s="71"/>
-      <c r="N62" s="71"/>
-      <c r="O62" s="72"/>
-      <c r="P62" s="74"/>
-      <c r="Q62" s="74"/>
-      <c r="R62" s="74"/>
-      <c r="S62" s="74"/>
-      <c r="T62" s="74"/>
-      <c r="U62" s="74"/>
-      <c r="V62" s="72"/>
+      <c r="A62" s="66"/>
+      <c r="B62" s="67"/>
+      <c r="C62" s="67"/>
+      <c r="D62" s="67"/>
+      <c r="E62" s="67"/>
+      <c r="F62" s="67"/>
+      <c r="G62" s="68"/>
+      <c r="H62" s="67"/>
+      <c r="I62" s="66"/>
+      <c r="J62" s="67"/>
+      <c r="K62" s="66"/>
+      <c r="L62" s="66"/>
+      <c r="M62" s="66"/>
+      <c r="N62" s="66"/>
+      <c r="O62" s="67"/>
+      <c r="P62" s="69"/>
+      <c r="Q62" s="69"/>
+      <c r="R62" s="69"/>
+      <c r="S62" s="69"/>
+      <c r="T62" s="69"/>
+      <c r="U62" s="69"/>
+      <c r="V62" s="67"/>
     </row>
     <row r="63" spans="1:22" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A63" s="71"/>
-      <c r="B63" s="72"/>
-      <c r="C63" s="72"/>
-      <c r="D63" s="72"/>
-      <c r="E63" s="72"/>
-      <c r="F63" s="72"/>
-      <c r="G63" s="73"/>
-      <c r="H63" s="72"/>
-      <c r="I63" s="71"/>
-      <c r="J63" s="72"/>
-      <c r="K63" s="71"/>
-      <c r="L63" s="71"/>
-      <c r="M63" s="71"/>
-      <c r="N63" s="71"/>
-      <c r="O63" s="72"/>
-      <c r="P63" s="74"/>
-      <c r="Q63" s="74"/>
-      <c r="R63" s="74"/>
-      <c r="S63" s="74"/>
-      <c r="T63" s="74"/>
-      <c r="U63" s="74"/>
-      <c r="V63" s="72"/>
+      <c r="A63" s="66"/>
+      <c r="B63" s="67"/>
+      <c r="C63" s="67"/>
+      <c r="D63" s="67"/>
+      <c r="E63" s="67"/>
+      <c r="F63" s="67"/>
+      <c r="G63" s="68"/>
+      <c r="H63" s="67"/>
+      <c r="I63" s="66"/>
+      <c r="J63" s="67"/>
+      <c r="K63" s="66"/>
+      <c r="L63" s="66"/>
+      <c r="M63" s="66"/>
+      <c r="N63" s="66"/>
+      <c r="O63" s="67"/>
+      <c r="P63" s="69"/>
+      <c r="Q63" s="69"/>
+      <c r="R63" s="69"/>
+      <c r="S63" s="69"/>
+      <c r="T63" s="69"/>
+      <c r="U63" s="69"/>
+      <c r="V63" s="67"/>
     </row>
     <row r="64" spans="1:22" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A64" s="71"/>
-      <c r="B64" s="72"/>
-      <c r="C64" s="72"/>
-      <c r="D64" s="72"/>
-      <c r="E64" s="72"/>
-      <c r="F64" s="72"/>
-      <c r="G64" s="73"/>
-      <c r="H64" s="72"/>
-      <c r="I64" s="71"/>
-      <c r="J64" s="72"/>
-      <c r="K64" s="71"/>
-      <c r="L64" s="71"/>
-      <c r="M64" s="71"/>
-      <c r="N64" s="71"/>
-      <c r="O64" s="72"/>
-      <c r="P64" s="74"/>
-      <c r="Q64" s="74"/>
-      <c r="R64" s="74"/>
-      <c r="S64" s="74"/>
-      <c r="T64" s="74"/>
-      <c r="U64" s="74"/>
-      <c r="V64" s="72"/>
+      <c r="A64" s="66"/>
+      <c r="B64" s="67"/>
+      <c r="C64" s="67"/>
+      <c r="D64" s="67"/>
+      <c r="E64" s="67"/>
+      <c r="F64" s="67"/>
+      <c r="G64" s="68"/>
+      <c r="H64" s="67"/>
+      <c r="I64" s="66"/>
+      <c r="J64" s="67"/>
+      <c r="K64" s="66"/>
+      <c r="L64" s="66"/>
+      <c r="M64" s="66"/>
+      <c r="N64" s="66"/>
+      <c r="O64" s="67"/>
+      <c r="P64" s="69"/>
+      <c r="Q64" s="69"/>
+      <c r="R64" s="69"/>
+      <c r="S64" s="69"/>
+      <c r="T64" s="69"/>
+      <c r="U64" s="69"/>
+      <c r="V64" s="67"/>
     </row>
     <row r="65" spans="1:22" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A65" s="71"/>
-      <c r="B65" s="72"/>
-      <c r="C65" s="72"/>
-      <c r="D65" s="72"/>
-      <c r="E65" s="72"/>
-      <c r="F65" s="72"/>
-      <c r="G65" s="73"/>
-      <c r="H65" s="72"/>
-      <c r="I65" s="71"/>
-      <c r="J65" s="72"/>
-      <c r="K65" s="71"/>
-      <c r="L65" s="71"/>
-      <c r="M65" s="71"/>
-      <c r="N65" s="71"/>
-      <c r="O65" s="72"/>
-      <c r="P65" s="74"/>
-      <c r="Q65" s="74"/>
-      <c r="R65" s="74"/>
-      <c r="S65" s="74"/>
-      <c r="T65" s="74"/>
-      <c r="U65" s="74"/>
-      <c r="V65" s="72"/>
+      <c r="A65" s="66"/>
+      <c r="B65" s="67"/>
+      <c r="C65" s="67"/>
+      <c r="D65" s="67"/>
+      <c r="E65" s="67"/>
+      <c r="F65" s="67"/>
+      <c r="G65" s="68"/>
+      <c r="H65" s="67"/>
+      <c r="I65" s="66"/>
+      <c r="J65" s="67"/>
+      <c r="K65" s="66"/>
+      <c r="L65" s="66"/>
+      <c r="M65" s="66"/>
+      <c r="N65" s="66"/>
+      <c r="O65" s="67"/>
+      <c r="P65" s="69"/>
+      <c r="Q65" s="69"/>
+      <c r="R65" s="69"/>
+      <c r="S65" s="69"/>
+      <c r="T65" s="69"/>
+      <c r="U65" s="69"/>
+      <c r="V65" s="67"/>
     </row>
     <row r="66" spans="1:22" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A66" s="71"/>
-      <c r="B66" s="72"/>
-      <c r="C66" s="72"/>
-      <c r="D66" s="72"/>
-      <c r="E66" s="72"/>
-      <c r="F66" s="72"/>
-      <c r="G66" s="73"/>
-      <c r="H66" s="72"/>
-      <c r="I66" s="71"/>
-      <c r="J66" s="72"/>
-      <c r="K66" s="71"/>
-      <c r="L66" s="71"/>
-      <c r="M66" s="71"/>
-      <c r="N66" s="71"/>
-      <c r="O66" s="72"/>
-      <c r="P66" s="74"/>
-      <c r="Q66" s="74"/>
-      <c r="R66" s="74"/>
-      <c r="S66" s="74"/>
-      <c r="T66" s="74"/>
-      <c r="U66" s="74"/>
-      <c r="V66" s="72"/>
+      <c r="A66" s="66"/>
+      <c r="B66" s="67"/>
+      <c r="C66" s="67"/>
+      <c r="D66" s="67"/>
+      <c r="E66" s="67"/>
+      <c r="F66" s="67"/>
+      <c r="G66" s="68"/>
+      <c r="H66" s="67"/>
+      <c r="I66" s="66"/>
+      <c r="J66" s="67"/>
+      <c r="K66" s="66"/>
+      <c r="L66" s="66"/>
+      <c r="M66" s="66"/>
+      <c r="N66" s="66"/>
+      <c r="O66" s="67"/>
+      <c r="P66" s="69"/>
+      <c r="Q66" s="69"/>
+      <c r="R66" s="69"/>
+      <c r="S66" s="69"/>
+      <c r="T66" s="69"/>
+      <c r="U66" s="69"/>
+      <c r="V66" s="67"/>
     </row>
     <row r="67" spans="1:22" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A67" s="71"/>
-      <c r="B67" s="72"/>
-      <c r="C67" s="72"/>
-      <c r="D67" s="72"/>
-      <c r="E67" s="72"/>
-      <c r="F67" s="72"/>
-      <c r="G67" s="73"/>
-      <c r="H67" s="72"/>
-      <c r="I67" s="71"/>
-      <c r="J67" s="72"/>
-      <c r="K67" s="71"/>
-      <c r="L67" s="71"/>
-      <c r="M67" s="71"/>
-      <c r="N67" s="71"/>
-      <c r="O67" s="72"/>
-      <c r="P67" s="74"/>
-      <c r="Q67" s="74"/>
-      <c r="R67" s="74"/>
-      <c r="S67" s="74"/>
-      <c r="T67" s="74"/>
-      <c r="U67" s="74"/>
-      <c r="V67" s="72"/>
+      <c r="A67" s="66"/>
+      <c r="B67" s="67"/>
+      <c r="C67" s="67"/>
+      <c r="D67" s="67"/>
+      <c r="E67" s="67"/>
+      <c r="F67" s="67"/>
+      <c r="G67" s="68"/>
+      <c r="H67" s="67"/>
+      <c r="I67" s="66"/>
+      <c r="J67" s="67"/>
+      <c r="K67" s="66"/>
+      <c r="L67" s="66"/>
+      <c r="M67" s="66"/>
+      <c r="N67" s="66"/>
+      <c r="O67" s="67"/>
+      <c r="P67" s="69"/>
+      <c r="Q67" s="69"/>
+      <c r="R67" s="69"/>
+      <c r="S67" s="69"/>
+      <c r="T67" s="69"/>
+      <c r="U67" s="69"/>
+      <c r="V67" s="67"/>
     </row>
     <row r="68" spans="1:22" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A68" s="71"/>
-      <c r="B68" s="72"/>
-      <c r="C68" s="72"/>
-      <c r="D68" s="72"/>
-      <c r="E68" s="72"/>
-      <c r="F68" s="72"/>
-      <c r="G68" s="73"/>
-      <c r="H68" s="72"/>
-      <c r="I68" s="71"/>
-      <c r="J68" s="72"/>
-      <c r="K68" s="71"/>
-      <c r="L68" s="71"/>
-      <c r="M68" s="71"/>
-      <c r="N68" s="71"/>
-      <c r="O68" s="72"/>
-      <c r="P68" s="74"/>
-      <c r="Q68" s="74"/>
-      <c r="R68" s="74"/>
-      <c r="S68" s="74"/>
-      <c r="T68" s="74"/>
-      <c r="U68" s="74"/>
-      <c r="V68" s="72"/>
+      <c r="A68" s="66"/>
+      <c r="B68" s="67"/>
+      <c r="C68" s="67"/>
+      <c r="D68" s="67"/>
+      <c r="E68" s="67"/>
+      <c r="F68" s="67"/>
+      <c r="G68" s="68"/>
+      <c r="H68" s="67"/>
+      <c r="I68" s="66"/>
+      <c r="J68" s="67"/>
+      <c r="K68" s="66"/>
+      <c r="L68" s="66"/>
+      <c r="M68" s="66"/>
+      <c r="N68" s="66"/>
+      <c r="O68" s="67"/>
+      <c r="P68" s="69"/>
+      <c r="Q68" s="69"/>
+      <c r="R68" s="69"/>
+      <c r="S68" s="69"/>
+      <c r="T68" s="69"/>
+      <c r="U68" s="69"/>
+      <c r="V68" s="67"/>
     </row>
     <row r="69" spans="1:22" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A69" s="71"/>
-      <c r="B69" s="72"/>
-      <c r="C69" s="72"/>
-      <c r="D69" s="72"/>
-      <c r="E69" s="72"/>
-      <c r="F69" s="72"/>
-      <c r="G69" s="73"/>
-      <c r="H69" s="72"/>
-      <c r="I69" s="71"/>
-      <c r="J69" s="72"/>
-      <c r="K69" s="71"/>
-      <c r="L69" s="71"/>
-      <c r="M69" s="71"/>
-      <c r="N69" s="71"/>
-      <c r="O69" s="72"/>
-      <c r="P69" s="74"/>
-      <c r="Q69" s="74"/>
-      <c r="R69" s="74"/>
-      <c r="S69" s="74"/>
-      <c r="T69" s="74"/>
-      <c r="U69" s="74"/>
-      <c r="V69" s="72"/>
+      <c r="A69" s="66"/>
+      <c r="B69" s="67"/>
+      <c r="C69" s="67"/>
+      <c r="D69" s="67"/>
+      <c r="E69" s="67"/>
+      <c r="F69" s="67"/>
+      <c r="G69" s="68"/>
+      <c r="H69" s="67"/>
+      <c r="I69" s="66"/>
+      <c r="J69" s="67"/>
+      <c r="K69" s="66"/>
+      <c r="L69" s="66"/>
+      <c r="M69" s="66"/>
+      <c r="N69" s="66"/>
+      <c r="O69" s="67"/>
+      <c r="P69" s="69"/>
+      <c r="Q69" s="69"/>
+      <c r="R69" s="69"/>
+      <c r="S69" s="69"/>
+      <c r="T69" s="69"/>
+      <c r="U69" s="69"/>
+      <c r="V69" s="67"/>
     </row>
     <row r="70" spans="1:22" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A70" s="71"/>
-      <c r="B70" s="72"/>
-      <c r="C70" s="72"/>
-      <c r="D70" s="72"/>
-      <c r="E70" s="72"/>
-      <c r="F70" s="72"/>
-      <c r="G70" s="73"/>
-      <c r="H70" s="72"/>
-      <c r="I70" s="71"/>
-      <c r="J70" s="72"/>
-      <c r="K70" s="71"/>
-      <c r="L70" s="71"/>
-      <c r="M70" s="71"/>
-      <c r="N70" s="71"/>
-      <c r="O70" s="72"/>
-      <c r="P70" s="74"/>
-      <c r="Q70" s="74"/>
-      <c r="R70" s="74"/>
-      <c r="S70" s="74"/>
-      <c r="T70" s="74"/>
-      <c r="U70" s="74"/>
-      <c r="V70" s="72"/>
+      <c r="A70" s="66"/>
+      <c r="B70" s="67"/>
+      <c r="C70" s="67"/>
+      <c r="D70" s="67"/>
+      <c r="E70" s="67"/>
+      <c r="F70" s="67"/>
+      <c r="G70" s="68"/>
+      <c r="H70" s="67"/>
+      <c r="I70" s="66"/>
+      <c r="J70" s="67"/>
+      <c r="K70" s="66"/>
+      <c r="L70" s="66"/>
+      <c r="M70" s="66"/>
+      <c r="N70" s="66"/>
+      <c r="O70" s="67"/>
+      <c r="P70" s="69"/>
+      <c r="Q70" s="69"/>
+      <c r="R70" s="69"/>
+      <c r="S70" s="69"/>
+      <c r="T70" s="69"/>
+      <c r="U70" s="69"/>
+      <c r="V70" s="67"/>
     </row>
     <row r="71" spans="1:22" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A71" s="71"/>
-      <c r="B71" s="72"/>
-      <c r="C71" s="72"/>
-      <c r="D71" s="72"/>
-      <c r="E71" s="72"/>
-      <c r="F71" s="72"/>
-      <c r="G71" s="73"/>
-      <c r="H71" s="72"/>
-      <c r="I71" s="71"/>
-      <c r="J71" s="72"/>
-      <c r="K71" s="71"/>
-      <c r="L71" s="71"/>
-      <c r="M71" s="71"/>
-      <c r="N71" s="71"/>
-      <c r="O71" s="72"/>
-      <c r="P71" s="74"/>
-      <c r="Q71" s="74"/>
-      <c r="R71" s="74"/>
-      <c r="S71" s="74"/>
-      <c r="T71" s="74"/>
-      <c r="U71" s="74"/>
-      <c r="V71" s="72"/>
+      <c r="A71" s="66"/>
+      <c r="B71" s="67"/>
+      <c r="C71" s="67"/>
+      <c r="D71" s="67"/>
+      <c r="E71" s="67"/>
+      <c r="F71" s="67"/>
+      <c r="G71" s="68"/>
+      <c r="H71" s="67"/>
+      <c r="I71" s="66"/>
+      <c r="J71" s="67"/>
+      <c r="K71" s="66"/>
+      <c r="L71" s="66"/>
+      <c r="M71" s="66"/>
+      <c r="N71" s="66"/>
+      <c r="O71" s="67"/>
+      <c r="P71" s="69"/>
+      <c r="Q71" s="69"/>
+      <c r="R71" s="69"/>
+      <c r="S71" s="69"/>
+      <c r="T71" s="69"/>
+      <c r="U71" s="69"/>
+      <c r="V71" s="67"/>
     </row>
     <row r="72" spans="1:22" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A72" s="71"/>
-      <c r="B72" s="72"/>
-      <c r="C72" s="72"/>
-      <c r="D72" s="72"/>
-      <c r="E72" s="72"/>
-      <c r="F72" s="72"/>
-      <c r="G72" s="73"/>
-      <c r="H72" s="72"/>
-      <c r="I72" s="71"/>
-      <c r="J72" s="72"/>
-      <c r="K72" s="71"/>
-      <c r="L72" s="71"/>
-      <c r="M72" s="71"/>
-      <c r="N72" s="71"/>
-      <c r="O72" s="72"/>
-      <c r="P72" s="74"/>
-      <c r="Q72" s="74"/>
-      <c r="R72" s="74"/>
-      <c r="S72" s="74"/>
-      <c r="T72" s="74"/>
-      <c r="U72" s="74"/>
-      <c r="V72" s="72"/>
+      <c r="A72" s="66"/>
+      <c r="B72" s="67"/>
+      <c r="C72" s="67"/>
+      <c r="D72" s="67"/>
+      <c r="E72" s="67"/>
+      <c r="F72" s="67"/>
+      <c r="G72" s="68"/>
+      <c r="H72" s="67"/>
+      <c r="I72" s="66"/>
+      <c r="J72" s="67"/>
+      <c r="K72" s="66"/>
+      <c r="L72" s="66"/>
+      <c r="M72" s="66"/>
+      <c r="N72" s="66"/>
+      <c r="O72" s="67"/>
+      <c r="P72" s="69"/>
+      <c r="Q72" s="69"/>
+      <c r="R72" s="69"/>
+      <c r="S72" s="69"/>
+      <c r="T72" s="69"/>
+      <c r="U72" s="69"/>
+      <c r="V72" s="67"/>
     </row>
     <row r="73" spans="1:22" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A73" s="71"/>
-      <c r="B73" s="72"/>
-      <c r="C73" s="72"/>
-      <c r="D73" s="72"/>
-      <c r="E73" s="72"/>
-      <c r="F73" s="72"/>
-      <c r="G73" s="73"/>
-      <c r="H73" s="72"/>
-      <c r="I73" s="71"/>
-      <c r="J73" s="72"/>
-      <c r="K73" s="71"/>
-      <c r="L73" s="71"/>
-      <c r="M73" s="71"/>
-      <c r="N73" s="71"/>
-      <c r="O73" s="72"/>
-      <c r="P73" s="74"/>
-      <c r="Q73" s="74"/>
-      <c r="R73" s="74"/>
-      <c r="S73" s="74"/>
-      <c r="T73" s="74"/>
-      <c r="U73" s="74"/>
-      <c r="V73" s="72"/>
+      <c r="A73" s="66"/>
+      <c r="B73" s="67"/>
+      <c r="C73" s="67"/>
+      <c r="D73" s="67"/>
+      <c r="E73" s="67"/>
+      <c r="F73" s="67"/>
+      <c r="G73" s="68"/>
+      <c r="H73" s="67"/>
+      <c r="I73" s="66"/>
+      <c r="J73" s="67"/>
+      <c r="K73" s="66"/>
+      <c r="L73" s="66"/>
+      <c r="M73" s="66"/>
+      <c r="N73" s="66"/>
+      <c r="O73" s="67"/>
+      <c r="P73" s="69"/>
+      <c r="Q73" s="69"/>
+      <c r="R73" s="69"/>
+      <c r="S73" s="69"/>
+      <c r="T73" s="69"/>
+      <c r="U73" s="69"/>
+      <c r="V73" s="67"/>
     </row>
     <row r="75" spans="1:22" hidden="1" x14ac:dyDescent="0.25"/>
     <row r="76" spans="1:22" hidden="1" x14ac:dyDescent="0.25"/>
@@ -5780,6 +5804,15 @@
     <row r="287" hidden="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="23">
+    <mergeCell ref="V1:V2"/>
+    <mergeCell ref="W1:W2"/>
+    <mergeCell ref="X1:X2"/>
+    <mergeCell ref="P1:P2"/>
+    <mergeCell ref="U1:U2"/>
+    <mergeCell ref="T1:T2"/>
+    <mergeCell ref="S1:S2"/>
+    <mergeCell ref="R1:R2"/>
+    <mergeCell ref="Q1:Q2"/>
     <mergeCell ref="I1:I2"/>
     <mergeCell ref="H1:H2"/>
     <mergeCell ref="O1:O2"/>
@@ -5794,15 +5827,6 @@
     <mergeCell ref="D1:D2"/>
     <mergeCell ref="C1:C2"/>
     <mergeCell ref="F1:F2"/>
-    <mergeCell ref="V1:V2"/>
-    <mergeCell ref="W1:W2"/>
-    <mergeCell ref="X1:X2"/>
-    <mergeCell ref="P1:P2"/>
-    <mergeCell ref="U1:U2"/>
-    <mergeCell ref="T1:T2"/>
-    <mergeCell ref="S1:S2"/>
-    <mergeCell ref="R1:R2"/>
-    <mergeCell ref="Q1:Q2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Solicitud gráfica recurso MA_08_08_CO_REC150
</commit_message>
<xml_diff>
--- a/fuentes/contenidos/grado08/guion08/ESCALETA_MA_08_08_CO.xlsx
+++ b/fuentes/contenidos/grado08/guion08/ESCALETA_MA_08_08_CO.xlsx
@@ -1382,7 +1382,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="200">
+  <cellXfs count="197">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
@@ -1759,9 +1759,6 @@
     <xf numFmtId="0" fontId="0" fillId="20" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="20" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="20" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="20" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1808,6 +1805,63 @@
     <xf numFmtId="0" fontId="0" fillId="19" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="12" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="12" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="17" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1826,12 +1880,6 @@
     <xf numFmtId="0" fontId="0" fillId="16" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="12" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1848,57 +1896,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="11" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="12" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -2209,7 +2206,7 @@
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="G1" zoomScale="70" zoomScaleNormal="70" zoomScalePageLayoutView="91" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G17" sqref="G17"/>
+      <selection pane="bottomLeft" activeCell="G18" sqref="G18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2241,106 +2238,106 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:25" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="187" t="s">
+      <c r="A1" s="172" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="185" t="s">
+      <c r="B1" s="170" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="198" t="s">
+      <c r="C1" s="183" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="187" t="s">
+      <c r="D1" s="172" t="s">
         <v>110</v>
       </c>
-      <c r="E1" s="185" t="s">
+      <c r="E1" s="170" t="s">
         <v>111</v>
       </c>
-      <c r="F1" s="183" t="s">
+      <c r="F1" s="166" t="s">
         <v>112</v>
       </c>
-      <c r="G1" s="196" t="s">
+      <c r="G1" s="181" t="s">
         <v>3</v>
       </c>
-      <c r="H1" s="183" t="s">
+      <c r="H1" s="166" t="s">
         <v>113</v>
       </c>
-      <c r="I1" s="183" t="s">
+      <c r="I1" s="166" t="s">
         <v>107</v>
       </c>
-      <c r="J1" s="193" t="s">
+      <c r="J1" s="178" t="s">
         <v>4</v>
       </c>
-      <c r="K1" s="191" t="s">
+      <c r="K1" s="176" t="s">
         <v>108</v>
       </c>
-      <c r="L1" s="189" t="s">
+      <c r="L1" s="174" t="s">
         <v>14</v>
       </c>
-      <c r="M1" s="195" t="s">
+      <c r="M1" s="180" t="s">
         <v>21</v>
       </c>
-      <c r="N1" s="195"/>
-      <c r="O1" s="175" t="s">
+      <c r="N1" s="180"/>
+      <c r="O1" s="168" t="s">
         <v>109</v>
       </c>
-      <c r="P1" s="175" t="s">
+      <c r="P1" s="168" t="s">
         <v>114</v>
       </c>
-      <c r="Q1" s="177" t="s">
+      <c r="Q1" s="191" t="s">
         <v>85</v>
       </c>
-      <c r="R1" s="181" t="s">
+      <c r="R1" s="195" t="s">
         <v>86</v>
       </c>
-      <c r="S1" s="177" t="s">
+      <c r="S1" s="191" t="s">
         <v>87</v>
       </c>
-      <c r="T1" s="179" t="s">
+      <c r="T1" s="193" t="s">
         <v>88</v>
       </c>
-      <c r="U1" s="177" t="s">
+      <c r="U1" s="191" t="s">
         <v>89</v>
       </c>
-      <c r="V1" s="169" t="s">
+      <c r="V1" s="185" t="s">
         <v>251</v>
       </c>
-      <c r="W1" s="171" t="s">
+      <c r="W1" s="187" t="s">
         <v>255</v>
       </c>
-      <c r="X1" s="173" t="s">
+      <c r="X1" s="189" t="s">
         <v>256</v>
       </c>
     </row>
     <row r="2" spans="1:25" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="188"/>
-      <c r="B2" s="186"/>
-      <c r="C2" s="199"/>
-      <c r="D2" s="188"/>
-      <c r="E2" s="186"/>
-      <c r="F2" s="184"/>
-      <c r="G2" s="197"/>
-      <c r="H2" s="184"/>
-      <c r="I2" s="184"/>
-      <c r="J2" s="194"/>
-      <c r="K2" s="192"/>
-      <c r="L2" s="190"/>
+      <c r="A2" s="173"/>
+      <c r="B2" s="171"/>
+      <c r="C2" s="184"/>
+      <c r="D2" s="173"/>
+      <c r="E2" s="171"/>
+      <c r="F2" s="167"/>
+      <c r="G2" s="182"/>
+      <c r="H2" s="167"/>
+      <c r="I2" s="167"/>
+      <c r="J2" s="179"/>
+      <c r="K2" s="177"/>
+      <c r="L2" s="175"/>
       <c r="M2" s="5" t="s">
         <v>90</v>
       </c>
       <c r="N2" s="5" t="s">
         <v>91</v>
       </c>
-      <c r="O2" s="176"/>
-      <c r="P2" s="176"/>
-      <c r="Q2" s="178"/>
-      <c r="R2" s="182"/>
-      <c r="S2" s="178"/>
-      <c r="T2" s="180"/>
-      <c r="U2" s="178"/>
-      <c r="V2" s="170"/>
-      <c r="W2" s="172"/>
-      <c r="X2" s="174"/>
+      <c r="O2" s="169"/>
+      <c r="P2" s="169"/>
+      <c r="Q2" s="192"/>
+      <c r="R2" s="196"/>
+      <c r="S2" s="192"/>
+      <c r="T2" s="194"/>
+      <c r="U2" s="192"/>
+      <c r="V2" s="186"/>
+      <c r="W2" s="188"/>
+      <c r="X2" s="190"/>
     </row>
     <row r="3" spans="1:25" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="71" t="s">
@@ -2628,47 +2625,47 @@
       </c>
       <c r="E7" s="33"/>
       <c r="F7" s="33"/>
-      <c r="G7" s="161" t="s">
+      <c r="G7" s="158" t="s">
         <v>132</v>
       </c>
-      <c r="H7" s="162">
+      <c r="H7" s="159">
         <v>5</v>
       </c>
-      <c r="I7" s="162" t="s">
+      <c r="I7" s="159" t="s">
         <v>19</v>
       </c>
-      <c r="J7" s="163" t="s">
+      <c r="J7" s="160" t="s">
         <v>237</v>
       </c>
-      <c r="K7" s="162" t="s">
+      <c r="K7" s="159" t="s">
         <v>20</v>
       </c>
-      <c r="L7" s="162" t="s">
+      <c r="L7" s="159" t="s">
         <v>5</v>
       </c>
-      <c r="M7" s="162" t="s">
+      <c r="M7" s="159" t="s">
         <v>57</v>
       </c>
-      <c r="N7" s="162"/>
-      <c r="O7" s="164" t="s">
+      <c r="N7" s="159"/>
+      <c r="O7" s="161" t="s">
         <v>235</v>
       </c>
-      <c r="P7" s="165" t="s">
+      <c r="P7" s="162" t="s">
         <v>19</v>
       </c>
-      <c r="Q7" s="166">
+      <c r="Q7" s="163">
         <v>6</v>
       </c>
-      <c r="R7" s="166" t="s">
+      <c r="R7" s="163" t="s">
         <v>188</v>
       </c>
-      <c r="S7" s="166" t="s">
+      <c r="S7" s="163" t="s">
         <v>189</v>
       </c>
-      <c r="T7" s="167" t="s">
+      <c r="T7" s="164" t="s">
         <v>198</v>
       </c>
-      <c r="U7" s="168" t="s">
+      <c r="U7" s="165" t="s">
         <v>191</v>
       </c>
       <c r="V7" s="101" t="s">
@@ -3014,7 +3011,7 @@
       <c r="V12" s="101" t="s">
         <v>248</v>
       </c>
-      <c r="W12" s="89">
+      <c r="W12" s="109">
         <v>42423</v>
       </c>
       <c r="X12" s="110">
@@ -3312,55 +3309,57 @@
         <v>122</v>
       </c>
       <c r="F17" s="31"/>
-      <c r="G17" s="140" t="s">
+      <c r="G17" s="130" t="s">
         <v>233</v>
       </c>
-      <c r="H17" s="143">
+      <c r="H17" s="131">
         <v>15</v>
       </c>
-      <c r="I17" s="141" t="s">
+      <c r="I17" s="132" t="s">
         <v>20</v>
       </c>
-      <c r="J17" s="142" t="s">
+      <c r="J17" s="133" t="s">
         <v>240</v>
       </c>
-      <c r="K17" s="141" t="s">
+      <c r="K17" s="132" t="s">
         <v>20</v>
       </c>
-      <c r="L17" s="141" t="s">
+      <c r="L17" s="132" t="s">
         <v>8</v>
       </c>
-      <c r="M17" s="141"/>
-      <c r="N17" s="141" t="s">
+      <c r="M17" s="132"/>
+      <c r="N17" s="132" t="s">
         <v>121</v>
       </c>
-      <c r="O17" s="142" t="s">
+      <c r="O17" s="133" t="s">
         <v>187</v>
       </c>
-      <c r="P17" s="143" t="s">
+      <c r="P17" s="131" t="s">
         <v>19</v>
       </c>
-      <c r="Q17" s="144">
+      <c r="Q17" s="134">
         <v>6</v>
       </c>
-      <c r="R17" s="144" t="s">
+      <c r="R17" s="134" t="s">
         <v>192</v>
       </c>
-      <c r="S17" s="144" t="s">
+      <c r="S17" s="134" t="s">
         <v>193</v>
       </c>
-      <c r="T17" s="145" t="s">
+      <c r="T17" s="135" t="s">
         <v>207</v>
       </c>
-      <c r="U17" s="146" t="s">
+      <c r="U17" s="136" t="s">
         <v>195</v>
       </c>
-      <c r="V17" s="150" t="s">
+      <c r="V17" s="101" t="s">
         <v>248</v>
       </c>
-      <c r="W17" s="151"/>
-      <c r="X17" s="151"/>
-      <c r="Y17" s="152" t="s">
+      <c r="W17" s="18"/>
+      <c r="X17" s="110">
+        <v>42424</v>
+      </c>
+      <c r="Y17" s="67" t="s">
         <v>273</v>
       </c>
     </row>
@@ -4299,47 +4298,47 @@
       </c>
       <c r="E32" s="55"/>
       <c r="F32" s="55"/>
-      <c r="G32" s="154" t="s">
+      <c r="G32" s="151" t="s">
         <v>175</v>
       </c>
-      <c r="H32" s="155">
+      <c r="H32" s="152">
         <v>30</v>
       </c>
-      <c r="I32" s="156" t="s">
+      <c r="I32" s="153" t="s">
         <v>20</v>
       </c>
-      <c r="J32" s="157" t="s">
+      <c r="J32" s="154" t="s">
         <v>245</v>
       </c>
-      <c r="K32" s="156" t="s">
+      <c r="K32" s="153" t="s">
         <v>20</v>
       </c>
-      <c r="L32" s="156" t="s">
+      <c r="L32" s="153" t="s">
         <v>8</v>
       </c>
-      <c r="M32" s="156"/>
-      <c r="N32" s="156" t="s">
+      <c r="M32" s="153"/>
+      <c r="N32" s="153" t="s">
         <v>120</v>
       </c>
-      <c r="O32" s="158" t="s">
+      <c r="O32" s="155" t="s">
         <v>176</v>
       </c>
-      <c r="P32" s="155" t="s">
+      <c r="P32" s="152" t="s">
         <v>19</v>
       </c>
-      <c r="Q32" s="159">
+      <c r="Q32" s="156">
         <v>6</v>
       </c>
-      <c r="R32" s="159" t="s">
+      <c r="R32" s="156" t="s">
         <v>192</v>
       </c>
-      <c r="S32" s="159" t="s">
+      <c r="S32" s="156" t="s">
         <v>193</v>
       </c>
-      <c r="T32" s="160" t="s">
+      <c r="T32" s="157" t="s">
         <v>214</v>
       </c>
-      <c r="U32" s="159" t="s">
+      <c r="U32" s="156" t="s">
         <v>195</v>
       </c>
       <c r="V32" s="147" t="s">
@@ -4347,7 +4346,7 @@
       </c>
       <c r="W32" s="148"/>
       <c r="X32" s="148"/>
-      <c r="Y32" s="153" t="s">
+      <c r="Y32" s="150" t="s">
         <v>274</v>
       </c>
     </row>
@@ -5828,6 +5827,15 @@
     <row r="287" hidden="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="23">
+    <mergeCell ref="V1:V2"/>
+    <mergeCell ref="W1:W2"/>
+    <mergeCell ref="X1:X2"/>
+    <mergeCell ref="P1:P2"/>
+    <mergeCell ref="U1:U2"/>
+    <mergeCell ref="T1:T2"/>
+    <mergeCell ref="S1:S2"/>
+    <mergeCell ref="R1:R2"/>
+    <mergeCell ref="Q1:Q2"/>
     <mergeCell ref="I1:I2"/>
     <mergeCell ref="H1:H2"/>
     <mergeCell ref="O1:O2"/>
@@ -5842,15 +5850,6 @@
     <mergeCell ref="D1:D2"/>
     <mergeCell ref="C1:C2"/>
     <mergeCell ref="F1:F2"/>
-    <mergeCell ref="V1:V2"/>
-    <mergeCell ref="W1:W2"/>
-    <mergeCell ref="X1:X2"/>
-    <mergeCell ref="P1:P2"/>
-    <mergeCell ref="U1:U2"/>
-    <mergeCell ref="T1:T2"/>
-    <mergeCell ref="S1:S2"/>
-    <mergeCell ref="R1:R2"/>
-    <mergeCell ref="Q1:Q2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Cambios en recurso MA_08_11_CO_REC190
</commit_message>
<xml_diff>
--- a/fuentes/contenidos/grado08/guion08/ESCALETA_MA_08_08_CO.xlsx
+++ b/fuentes/contenidos/grado08/guion08/ESCALETA_MA_08_08_CO.xlsx
@@ -1799,111 +1799,6 @@
     <xf numFmtId="14" fontId="0" fillId="18" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="12" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="12" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="17" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="17" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="18" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="18" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="16" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="16" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="10" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="9" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="11" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="20" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="18" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="17" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="19" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -1949,6 +1844,111 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="18" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="17" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="17" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="18" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="18" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="16" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="16" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="12" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="10" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="11" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="12" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="20" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="18" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="17" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -2257,9 +2257,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Y287"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" zoomScale="70" zoomScaleNormal="70" zoomScalePageLayoutView="91" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="F1" zoomScale="70" zoomScaleNormal="70" zoomScalePageLayoutView="91" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G22" sqref="G22"/>
+      <selection pane="bottomLeft" activeCell="G34" sqref="G34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2292,50 +2292,50 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:25" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="159" t="s">
+      <c r="A1" s="188" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="157" t="s">
+      <c r="B1" s="186" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="170" t="s">
+      <c r="C1" s="199" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="159" t="s">
+      <c r="D1" s="188" t="s">
         <v>110</v>
       </c>
-      <c r="E1" s="157" t="s">
+      <c r="E1" s="186" t="s">
         <v>111</v>
       </c>
-      <c r="F1" s="153" t="s">
+      <c r="F1" s="184" t="s">
         <v>112</v>
       </c>
-      <c r="G1" s="168" t="s">
+      <c r="G1" s="197" t="s">
         <v>3</v>
       </c>
-      <c r="H1" s="153" t="s">
+      <c r="H1" s="184" t="s">
         <v>113</v>
       </c>
-      <c r="I1" s="153" t="s">
+      <c r="I1" s="184" t="s">
         <v>107</v>
       </c>
-      <c r="J1" s="165" t="s">
+      <c r="J1" s="194" t="s">
         <v>4</v>
       </c>
-      <c r="K1" s="163" t="s">
+      <c r="K1" s="192" t="s">
         <v>108</v>
       </c>
-      <c r="L1" s="161" t="s">
+      <c r="L1" s="190" t="s">
         <v>14</v>
       </c>
-      <c r="M1" s="167" t="s">
+      <c r="M1" s="196" t="s">
         <v>21</v>
       </c>
-      <c r="N1" s="167"/>
-      <c r="O1" s="155" t="s">
+      <c r="N1" s="196"/>
+      <c r="O1" s="176" t="s">
         <v>109</v>
       </c>
-      <c r="P1" s="155" t="s">
+      <c r="P1" s="176" t="s">
         <v>114</v>
       </c>
       <c r="Q1" s="178" t="s">
@@ -2353,45 +2353,45 @@
       <c r="U1" s="178" t="s">
         <v>89</v>
       </c>
-      <c r="V1" s="172" t="s">
+      <c r="V1" s="170" t="s">
         <v>251</v>
       </c>
-      <c r="W1" s="174" t="s">
+      <c r="W1" s="172" t="s">
         <v>255</v>
       </c>
-      <c r="X1" s="176" t="s">
+      <c r="X1" s="174" t="s">
         <v>256</v>
       </c>
     </row>
     <row r="2" spans="1:25" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="160"/>
-      <c r="B2" s="158"/>
-      <c r="C2" s="171"/>
-      <c r="D2" s="160"/>
-      <c r="E2" s="158"/>
-      <c r="F2" s="154"/>
-      <c r="G2" s="169"/>
-      <c r="H2" s="154"/>
-      <c r="I2" s="154"/>
-      <c r="J2" s="166"/>
-      <c r="K2" s="164"/>
-      <c r="L2" s="162"/>
+      <c r="A2" s="189"/>
+      <c r="B2" s="187"/>
+      <c r="C2" s="200"/>
+      <c r="D2" s="189"/>
+      <c r="E2" s="187"/>
+      <c r="F2" s="185"/>
+      <c r="G2" s="198"/>
+      <c r="H2" s="185"/>
+      <c r="I2" s="185"/>
+      <c r="J2" s="195"/>
+      <c r="K2" s="193"/>
+      <c r="L2" s="191"/>
       <c r="M2" s="5" t="s">
         <v>90</v>
       </c>
       <c r="N2" s="5" t="s">
         <v>91</v>
       </c>
-      <c r="O2" s="156"/>
-      <c r="P2" s="156"/>
+      <c r="O2" s="177"/>
+      <c r="P2" s="177"/>
       <c r="Q2" s="179"/>
       <c r="R2" s="183"/>
       <c r="S2" s="179"/>
       <c r="T2" s="181"/>
       <c r="U2" s="179"/>
-      <c r="V2" s="173"/>
-      <c r="W2" s="175"/>
-      <c r="X2" s="177"/>
+      <c r="V2" s="171"/>
+      <c r="W2" s="173"/>
+      <c r="X2" s="175"/>
     </row>
     <row r="3" spans="1:25" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="62" t="s">
@@ -2476,7 +2476,7 @@
       </c>
       <c r="E4" s="8"/>
       <c r="F4" s="8"/>
-      <c r="G4" s="195" t="s">
+      <c r="G4" s="160" t="s">
         <v>126</v>
       </c>
       <c r="H4" s="79">
@@ -2485,7 +2485,7 @@
       <c r="I4" s="80" t="s">
         <v>20</v>
       </c>
-      <c r="J4" s="196" t="s">
+      <c r="J4" s="161" t="s">
         <v>131</v>
       </c>
       <c r="K4" s="80" t="s">
@@ -2498,7 +2498,7 @@
       <c r="N4" s="80" t="s">
         <v>40</v>
       </c>
-      <c r="O4" s="197" t="s">
+      <c r="O4" s="162" t="s">
         <v>127</v>
       </c>
       <c r="P4" s="79" t="s">
@@ -2615,45 +2615,45 @@
         <v>122</v>
       </c>
       <c r="F6" s="10"/>
-      <c r="G6" s="188" t="s">
+      <c r="G6" s="153" t="s">
         <v>236</v>
       </c>
-      <c r="H6" s="189">
+      <c r="H6" s="154">
         <v>4</v>
       </c>
-      <c r="I6" s="190" t="s">
+      <c r="I6" s="155" t="s">
         <v>20</v>
       </c>
-      <c r="J6" s="191" t="s">
+      <c r="J6" s="156" t="s">
         <v>130</v>
       </c>
-      <c r="K6" s="190" t="s">
+      <c r="K6" s="155" t="s">
         <v>20</v>
       </c>
-      <c r="L6" s="190" t="s">
+      <c r="L6" s="155" t="s">
         <v>8</v>
       </c>
-      <c r="M6" s="190"/>
-      <c r="N6" s="190" t="s">
+      <c r="M6" s="155"/>
+      <c r="N6" s="155" t="s">
         <v>121</v>
       </c>
-      <c r="O6" s="191"/>
-      <c r="P6" s="189" t="s">
+      <c r="O6" s="156"/>
+      <c r="P6" s="154" t="s">
         <v>19</v>
       </c>
-      <c r="Q6" s="192">
+      <c r="Q6" s="157">
         <v>6</v>
       </c>
-      <c r="R6" s="192" t="s">
+      <c r="R6" s="157" t="s">
         <v>192</v>
       </c>
-      <c r="S6" s="192" t="s">
+      <c r="S6" s="157" t="s">
         <v>193</v>
       </c>
-      <c r="T6" s="193" t="s">
+      <c r="T6" s="158" t="s">
         <v>197</v>
       </c>
-      <c r="U6" s="194" t="s">
+      <c r="U6" s="159" t="s">
         <v>195</v>
       </c>
       <c r="V6" s="77" t="s">
@@ -3564,47 +3564,47 @@
       </c>
       <c r="E20" s="12"/>
       <c r="F20" s="12"/>
-      <c r="G20" s="198" t="s">
+      <c r="G20" s="163" t="s">
         <v>241</v>
       </c>
-      <c r="H20" s="199">
+      <c r="H20" s="164">
         <v>18</v>
       </c>
-      <c r="I20" s="199" t="s">
+      <c r="I20" s="164" t="s">
         <v>19</v>
       </c>
-      <c r="J20" s="200" t="s">
+      <c r="J20" s="165" t="s">
         <v>242</v>
       </c>
-      <c r="K20" s="199" t="s">
+      <c r="K20" s="164" t="s">
         <v>20</v>
       </c>
-      <c r="L20" s="199" t="s">
+      <c r="L20" s="164" t="s">
         <v>5</v>
       </c>
-      <c r="M20" s="199" t="s">
+      <c r="M20" s="164" t="s">
         <v>58</v>
       </c>
-      <c r="N20" s="199"/>
-      <c r="O20" s="200" t="s">
+      <c r="N20" s="164"/>
+      <c r="O20" s="165" t="s">
         <v>153</v>
       </c>
-      <c r="P20" s="201" t="s">
+      <c r="P20" s="166" t="s">
         <v>19</v>
       </c>
-      <c r="Q20" s="202">
+      <c r="Q20" s="167">
         <v>6</v>
       </c>
-      <c r="R20" s="202" t="s">
+      <c r="R20" s="167" t="s">
         <v>188</v>
       </c>
-      <c r="S20" s="202" t="s">
+      <c r="S20" s="167" t="s">
         <v>189</v>
       </c>
-      <c r="T20" s="203" t="s">
+      <c r="T20" s="168" t="s">
         <v>209</v>
       </c>
-      <c r="U20" s="204" t="s">
+      <c r="U20" s="169" t="s">
         <v>191</v>
       </c>
       <c r="V20" s="77" t="s">
@@ -5897,15 +5897,6 @@
     <row r="287" hidden="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="23">
-    <mergeCell ref="V1:V2"/>
-    <mergeCell ref="W1:W2"/>
-    <mergeCell ref="X1:X2"/>
-    <mergeCell ref="P1:P2"/>
-    <mergeCell ref="U1:U2"/>
-    <mergeCell ref="T1:T2"/>
-    <mergeCell ref="S1:S2"/>
-    <mergeCell ref="R1:R2"/>
-    <mergeCell ref="Q1:Q2"/>
     <mergeCell ref="I1:I2"/>
     <mergeCell ref="H1:H2"/>
     <mergeCell ref="O1:O2"/>
@@ -5920,6 +5911,15 @@
     <mergeCell ref="D1:D2"/>
     <mergeCell ref="C1:C2"/>
     <mergeCell ref="F1:F2"/>
+    <mergeCell ref="V1:V2"/>
+    <mergeCell ref="W1:W2"/>
+    <mergeCell ref="X1:X2"/>
+    <mergeCell ref="P1:P2"/>
+    <mergeCell ref="U1:U2"/>
+    <mergeCell ref="T1:T2"/>
+    <mergeCell ref="S1:S2"/>
+    <mergeCell ref="R1:R2"/>
+    <mergeCell ref="Q1:Q2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -5980,30 +5980,30 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B2" s="185" t="s">
+      <c r="B2" s="202" t="s">
         <v>273</v>
       </c>
-      <c r="C2" s="187" t="s">
+      <c r="C2" s="204" t="s">
         <v>3</v>
       </c>
-      <c r="D2" s="186" t="s">
+      <c r="D2" s="203" t="s">
         <v>21</v>
       </c>
-      <c r="E2" s="186"/>
-      <c r="F2" s="184" t="s">
+      <c r="E2" s="203"/>
+      <c r="F2" s="201" t="s">
         <v>256</v>
       </c>
     </row>
     <row r="3" spans="2:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B3" s="185"/>
-      <c r="C3" s="187"/>
+      <c r="B3" s="202"/>
+      <c r="C3" s="204"/>
       <c r="D3" s="122" t="s">
         <v>90</v>
       </c>
       <c r="E3" s="123" t="s">
         <v>91</v>
       </c>
-      <c r="F3" s="184"/>
+      <c r="F3" s="201"/>
     </row>
     <row r="4" spans="2:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B4" s="118">

</xml_diff>